<commit_message>
Actualización SUMP Planeación ciclo 2
Actualización de tareas de equipo faltantes
</commit_message>
<xml_diff>
--- a/NoteBook/summary/TASK_TEAM.xlsx
+++ b/NoteBook/summary/TASK_TEAM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="118">
   <si>
     <t>TSPi Example Task Planning Template - Form TASK</t>
   </si>
@@ -364,6 +364,12 @@
   </si>
   <si>
     <t>Actualizar plan de calidad-Diligenciar SUMQ</t>
+  </si>
+  <si>
+    <t>Management and Miscellaneous</t>
+  </si>
+  <si>
+    <t>Planeación de Implementación</t>
   </si>
 </sst>
 </file>
@@ -1414,7 +1420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1505,30 +1511,150 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="42" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="73" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1538,53 +1664,29 @@
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="42" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1595,97 +1697,13 @@
     <xf numFmtId="0" fontId="49" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="71" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="68" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="58" fillId="10" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1960,7 +1978,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1968,10 +1986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S113"/>
+  <dimension ref="A1:S115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="Q67" sqref="Q67"/>
+    <sheetView tabSelected="1" topLeftCell="C95" workbookViewId="0">
+      <selection activeCell="Q68" sqref="Q68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1993,16 +2011,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
+      <c r="A1" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="30"/>
@@ -2012,51 +2030,51 @@
       <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="51"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="64"/>
       <c r="E3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="53">
+      <c r="F3" s="66">
         <v>41719</v>
       </c>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
     </row>
     <row r="4" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="55"/>
-      <c r="D4" s="49"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="68"/>
       <c r="E4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="49" t="s">
+      <c r="F4" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
     </row>
     <row r="5" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="48"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="70"/>
       <c r="E5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="49">
-        <v>1</v>
-      </c>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
+      <c r="F5" s="68">
+        <v>1</v>
+      </c>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
@@ -2080,200 +2098,200 @@
       <c r="S6" s="25"/>
     </row>
     <row r="7" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="45" t="s">
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="45" t="s">
+      <c r="F7" s="71"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="71"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="46"/>
-      <c r="N7" s="46"/>
-      <c r="O7" s="46"/>
-      <c r="P7" s="47"/>
-      <c r="Q7" s="45" t="s">
+      <c r="M7" s="71"/>
+      <c r="N7" s="71"/>
+      <c r="O7" s="71"/>
+      <c r="P7" s="73"/>
+      <c r="Q7" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="R7" s="46"/>
-      <c r="S7" s="47"/>
+      <c r="R7" s="71"/>
+      <c r="S7" s="73"/>
     </row>
     <row r="8" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="35" t="s">
+      <c r="I8" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="35" t="s">
+      <c r="J8" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="35" t="s">
+      <c r="K8" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="38" t="s">
+      <c r="L8" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="M8" s="35" t="s">
+      <c r="M8" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="N8" s="35" t="s">
+      <c r="N8" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="O8" s="35" t="s">
+      <c r="O8" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="P8" s="35" t="s">
+      <c r="P8" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="Q8" s="35" t="s">
+      <c r="Q8" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="R8" s="35" t="s">
+      <c r="R8" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="S8" s="35" t="s">
+      <c r="S8" s="74" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="36"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="36"/>
-      <c r="Q9" s="36"/>
-      <c r="R9" s="36"/>
-      <c r="S9" s="36"/>
+      <c r="A9" s="75"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="75"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="78"/>
+      <c r="M9" s="75"/>
+      <c r="N9" s="75"/>
+      <c r="O9" s="75"/>
+      <c r="P9" s="75"/>
+      <c r="Q9" s="75"/>
+      <c r="R9" s="75"/>
+      <c r="S9" s="75"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="36"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="36"/>
-      <c r="N10" s="36"/>
-      <c r="O10" s="36"/>
-      <c r="P10" s="36"/>
-      <c r="Q10" s="36"/>
-      <c r="R10" s="36"/>
-      <c r="S10" s="36"/>
+      <c r="A10" s="75"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="75"/>
+      <c r="L10" s="78"/>
+      <c r="M10" s="75"/>
+      <c r="N10" s="75"/>
+      <c r="O10" s="75"/>
+      <c r="P10" s="75"/>
+      <c r="Q10" s="75"/>
+      <c r="R10" s="75"/>
+      <c r="S10" s="75"/>
     </row>
     <row r="11" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="36"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="36"/>
-      <c r="N11" s="36"/>
-      <c r="O11" s="36"/>
-      <c r="P11" s="36"/>
-      <c r="Q11" s="36"/>
-      <c r="R11" s="36"/>
-      <c r="S11" s="36"/>
+      <c r="A11" s="75"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="75"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="75"/>
+      <c r="L11" s="78"/>
+      <c r="M11" s="75"/>
+      <c r="N11" s="75"/>
+      <c r="O11" s="75"/>
+      <c r="P11" s="75"/>
+      <c r="Q11" s="75"/>
+      <c r="R11" s="75"/>
+      <c r="S11" s="75"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="36"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="36"/>
-      <c r="P12" s="36"/>
-      <c r="Q12" s="36"/>
-      <c r="R12" s="36"/>
-      <c r="S12" s="36"/>
+      <c r="A12" s="75"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="75"/>
+      <c r="I12" s="75"/>
+      <c r="J12" s="75"/>
+      <c r="K12" s="75"/>
+      <c r="L12" s="78"/>
+      <c r="M12" s="75"/>
+      <c r="N12" s="75"/>
+      <c r="O12" s="75"/>
+      <c r="P12" s="75"/>
+      <c r="Q12" s="75"/>
+      <c r="R12" s="75"/>
+      <c r="S12" s="75"/>
     </row>
     <row r="13" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="37"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="40"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37"/>
-      <c r="P13" s="36"/>
-      <c r="Q13" s="37"/>
-      <c r="R13" s="37"/>
-      <c r="S13" s="37"/>
+      <c r="A13" s="76"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="79"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="76"/>
+      <c r="I13" s="76"/>
+      <c r="J13" s="76"/>
+      <c r="K13" s="75"/>
+      <c r="L13" s="79"/>
+      <c r="M13" s="76"/>
+      <c r="N13" s="76"/>
+      <c r="O13" s="76"/>
+      <c r="P13" s="75"/>
+      <c r="Q13" s="76"/>
+      <c r="R13" s="76"/>
+      <c r="S13" s="76"/>
     </row>
     <row r="14" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="80" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="26"/>
@@ -2335,7 +2353,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="34"/>
+      <c r="A15" s="81"/>
       <c r="B15" s="26"/>
       <c r="C15" s="19" t="s">
         <v>34</v>
@@ -2395,7 +2413,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="42"/>
+      <c r="A16" s="82"/>
       <c r="B16" s="26"/>
       <c r="C16" s="19" t="s">
         <v>35</v>
@@ -2455,7 +2473,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="80" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="26"/>
@@ -2517,7 +2535,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="34"/>
+      <c r="A18" s="81"/>
       <c r="B18" s="26"/>
       <c r="C18" s="19" t="s">
         <v>38</v>
@@ -2577,7 +2595,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="42"/>
+      <c r="A19" s="82"/>
       <c r="B19" s="26"/>
       <c r="C19" s="19" t="s">
         <v>39</v>
@@ -2637,7 +2655,7 @@
       </c>
     </row>
     <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="80" t="s">
         <v>40</v>
       </c>
       <c r="B20" s="26"/>
@@ -2699,7 +2717,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="34"/>
+      <c r="A21" s="81"/>
       <c r="B21" s="26"/>
       <c r="C21" s="19" t="s">
         <v>42</v>
@@ -2759,7 +2777,7 @@
       </c>
     </row>
     <row r="22" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="34"/>
+      <c r="A22" s="81"/>
       <c r="B22" s="26"/>
       <c r="C22" s="19" t="s">
         <v>43</v>
@@ -2819,7 +2837,7 @@
       </c>
     </row>
     <row r="23" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="34"/>
+      <c r="A23" s="81"/>
       <c r="B23" s="26"/>
       <c r="C23" s="19" t="s">
         <v>44</v>
@@ -2879,7 +2897,7 @@
       </c>
     </row>
     <row r="24" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="34"/>
+      <c r="A24" s="81"/>
       <c r="B24" s="26"/>
       <c r="C24" s="19" t="s">
         <v>45</v>
@@ -2939,7 +2957,7 @@
       </c>
     </row>
     <row r="25" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="34"/>
+      <c r="A25" s="81"/>
       <c r="B25" s="26"/>
       <c r="C25" s="19" t="s">
         <v>46</v>
@@ -2999,7 +3017,7 @@
       </c>
     </row>
     <row r="26" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="42"/>
+      <c r="A26" s="82"/>
       <c r="B26" s="26"/>
       <c r="C26" s="19" t="s">
         <v>47</v>
@@ -3059,7 +3077,7 @@
       </c>
     </row>
     <row r="27" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="41" t="s">
+      <c r="A27" s="80" t="s">
         <v>48</v>
       </c>
       <c r="B27" s="26"/>
@@ -3121,7 +3139,7 @@
       </c>
     </row>
     <row r="28" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="34"/>
+      <c r="A28" s="81"/>
       <c r="B28" s="26"/>
       <c r="C28" s="19" t="s">
         <v>50</v>
@@ -3181,7 +3199,7 @@
       </c>
     </row>
     <row r="29" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="34"/>
+      <c r="A29" s="81"/>
       <c r="B29" s="26"/>
       <c r="C29" s="19" t="s">
         <v>51</v>
@@ -3241,7 +3259,7 @@
       </c>
     </row>
     <row r="30" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="34"/>
+      <c r="A30" s="81"/>
       <c r="B30" s="26"/>
       <c r="C30" s="19" t="s">
         <v>52</v>
@@ -3301,7 +3319,7 @@
       </c>
     </row>
     <row r="31" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="41" t="s">
+      <c r="A31" s="80" t="s">
         <v>53</v>
       </c>
       <c r="B31" s="26"/>
@@ -3363,7 +3381,7 @@
       </c>
     </row>
     <row r="32" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="34"/>
+      <c r="A32" s="81"/>
       <c r="B32" s="26"/>
       <c r="C32" s="19" t="s">
         <v>55</v>
@@ -3423,7 +3441,7 @@
       </c>
     </row>
     <row r="33" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="34"/>
+      <c r="A33" s="81"/>
       <c r="B33" s="26"/>
       <c r="C33" s="19" t="s">
         <v>56</v>
@@ -3483,7 +3501,7 @@
       </c>
     </row>
     <row r="34" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="34"/>
+      <c r="A34" s="81"/>
       <c r="B34" s="26"/>
       <c r="C34" s="19" t="s">
         <v>57</v>
@@ -3543,7 +3561,7 @@
       </c>
     </row>
     <row r="35" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="42"/>
+      <c r="A35" s="82"/>
       <c r="B35" s="26"/>
       <c r="C35" s="19" t="s">
         <v>58</v>
@@ -3603,7 +3621,7 @@
       </c>
     </row>
     <row r="36" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="41" t="s">
+      <c r="A36" s="80" t="s">
         <v>59</v>
       </c>
       <c r="B36" s="26"/>
@@ -3665,7 +3683,7 @@
       </c>
     </row>
     <row r="37" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="34"/>
+      <c r="A37" s="81"/>
       <c r="B37" s="26"/>
       <c r="C37" s="19" t="s">
         <v>61</v>
@@ -3725,7 +3743,7 @@
       </c>
     </row>
     <row r="38" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="34"/>
+      <c r="A38" s="81"/>
       <c r="B38" s="26"/>
       <c r="C38" s="19" t="s">
         <v>62</v>
@@ -3781,7 +3799,7 @@
       </c>
     </row>
     <row r="39" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="34"/>
+      <c r="A39" s="81"/>
       <c r="B39" s="26"/>
       <c r="C39" s="19" t="s">
         <v>63</v>
@@ -3839,7 +3857,7 @@
       </c>
     </row>
     <row r="40" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="34"/>
+      <c r="A40" s="81"/>
       <c r="B40" s="26"/>
       <c r="C40" s="19" t="s">
         <v>64</v>
@@ -3899,7 +3917,7 @@
       </c>
     </row>
     <row r="41" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="34"/>
+      <c r="A41" s="81"/>
       <c r="B41" s="26"/>
       <c r="C41" s="19" t="s">
         <v>65</v>
@@ -3959,7 +3977,7 @@
       </c>
     </row>
     <row r="42" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="34"/>
+      <c r="A42" s="81"/>
       <c r="B42" s="26"/>
       <c r="C42" s="19" t="s">
         <v>67</v>
@@ -4015,7 +4033,7 @@
       </c>
     </row>
     <row r="43" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="42"/>
+      <c r="A43" s="82"/>
       <c r="B43" s="26"/>
       <c r="C43" s="19" t="s">
         <v>68</v>
@@ -4075,7 +4093,7 @@
       </c>
     </row>
     <row r="44" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="41" t="s">
+      <c r="A44" s="80" t="s">
         <v>69</v>
       </c>
       <c r="B44" s="26"/>
@@ -4137,7 +4155,7 @@
       </c>
     </row>
     <row r="45" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="34"/>
+      <c r="A45" s="81"/>
       <c r="B45" s="26"/>
       <c r="C45" s="19" t="s">
         <v>71</v>
@@ -4193,7 +4211,7 @@
       </c>
     </row>
     <row r="46" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="42"/>
+      <c r="A46" s="82"/>
       <c r="B46" s="26"/>
       <c r="C46" s="19" t="s">
         <v>72</v>
@@ -4253,7 +4271,7 @@
       </c>
     </row>
     <row r="47" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="41" t="s">
+      <c r="A47" s="80" t="s">
         <v>73</v>
       </c>
       <c r="B47" s="26"/>
@@ -4315,7 +4333,7 @@
       </c>
     </row>
     <row r="48" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="42"/>
+      <c r="A48" s="82"/>
       <c r="B48" s="26"/>
       <c r="C48" s="19" t="s">
         <v>75</v>
@@ -4441,27 +4459,27 @@
       <c r="S50" s="9"/>
     </row>
     <row r="51" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="43" t="s">
+      <c r="A51" s="83" t="s">
         <v>76</v>
       </c>
-      <c r="B51" s="44"/>
-      <c r="C51" s="43"/>
-      <c r="D51" s="44"/>
-      <c r="E51" s="44"/>
-      <c r="F51" s="44"/>
-      <c r="G51" s="44"/>
-      <c r="H51" s="44"/>
-      <c r="I51" s="44"/>
-      <c r="J51" s="44"/>
-      <c r="K51" s="44"/>
-      <c r="L51" s="44"/>
-      <c r="M51" s="44"/>
-      <c r="N51" s="44"/>
-      <c r="O51" s="44"/>
-      <c r="P51" s="44"/>
-      <c r="Q51" s="44"/>
-      <c r="R51" s="44"/>
-      <c r="S51" s="44"/>
+      <c r="B51" s="84"/>
+      <c r="C51" s="83"/>
+      <c r="D51" s="84"/>
+      <c r="E51" s="84"/>
+      <c r="F51" s="84"/>
+      <c r="G51" s="84"/>
+      <c r="H51" s="84"/>
+      <c r="I51" s="84"/>
+      <c r="J51" s="84"/>
+      <c r="K51" s="84"/>
+      <c r="L51" s="84"/>
+      <c r="M51" s="84"/>
+      <c r="N51" s="84"/>
+      <c r="O51" s="84"/>
+      <c r="P51" s="84"/>
+      <c r="Q51" s="84"/>
+      <c r="R51" s="84"/>
+      <c r="S51" s="84"/>
     </row>
     <row r="52" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="27"/>
@@ -4485,203 +4503,203 @@
       <c r="S52" s="25"/>
     </row>
     <row r="53" spans="1:19" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="45" t="s">
+      <c r="A53" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="B53" s="46"/>
-      <c r="C53" s="46"/>
-      <c r="D53" s="47"/>
-      <c r="E53" s="45" t="s">
+      <c r="B53" s="71"/>
+      <c r="C53" s="71"/>
+      <c r="D53" s="73"/>
+      <c r="E53" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="F53" s="46"/>
-      <c r="G53" s="46"/>
-      <c r="H53" s="46"/>
-      <c r="I53" s="46"/>
-      <c r="J53" s="46"/>
-      <c r="K53" s="47"/>
-      <c r="L53" s="45" t="s">
+      <c r="F53" s="71"/>
+      <c r="G53" s="71"/>
+      <c r="H53" s="71"/>
+      <c r="I53" s="71"/>
+      <c r="J53" s="71"/>
+      <c r="K53" s="73"/>
+      <c r="L53" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="M53" s="46"/>
-      <c r="N53" s="46"/>
-      <c r="O53" s="46"/>
-      <c r="P53" s="47"/>
-      <c r="Q53" s="45" t="s">
+      <c r="M53" s="71"/>
+      <c r="N53" s="71"/>
+      <c r="O53" s="71"/>
+      <c r="P53" s="73"/>
+      <c r="Q53" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="R53" s="46"/>
-      <c r="S53" s="47"/>
+      <c r="R53" s="71"/>
+      <c r="S53" s="73"/>
     </row>
     <row r="54" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="35" t="s">
+      <c r="A54" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="B54" s="35" t="s">
+      <c r="B54" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="C54" s="38" t="s">
+      <c r="C54" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="D54" s="35" t="s">
+      <c r="D54" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="E54" s="35" t="s">
+      <c r="E54" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="F54" s="35" t="s">
+      <c r="F54" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="G54" s="35" t="s">
+      <c r="G54" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="H54" s="35" t="s">
+      <c r="H54" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="I54" s="35" t="s">
+      <c r="I54" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="J54" s="35" t="s">
+      <c r="J54" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="K54" s="35" t="s">
+      <c r="K54" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="L54" s="38" t="s">
+      <c r="L54" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="M54" s="35" t="s">
+      <c r="M54" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="N54" s="35" t="s">
+      <c r="N54" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="O54" s="35" t="s">
+      <c r="O54" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="P54" s="35" t="s">
+      <c r="P54" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="Q54" s="35" t="s">
+      <c r="Q54" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="R54" s="35" t="s">
+      <c r="R54" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="S54" s="35" t="s">
+      <c r="S54" s="74" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="55" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="36"/>
-      <c r="B55" s="36"/>
-      <c r="C55" s="39"/>
-      <c r="D55" s="36"/>
-      <c r="E55" s="36"/>
-      <c r="F55" s="36"/>
-      <c r="G55" s="36"/>
-      <c r="H55" s="36"/>
-      <c r="I55" s="36"/>
-      <c r="J55" s="36"/>
-      <c r="K55" s="36"/>
-      <c r="L55" s="39"/>
-      <c r="M55" s="36"/>
-      <c r="N55" s="36"/>
-      <c r="O55" s="36"/>
-      <c r="P55" s="36"/>
-      <c r="Q55" s="36"/>
-      <c r="R55" s="36"/>
-      <c r="S55" s="36"/>
+      <c r="A55" s="75"/>
+      <c r="B55" s="75"/>
+      <c r="C55" s="78"/>
+      <c r="D55" s="75"/>
+      <c r="E55" s="75"/>
+      <c r="F55" s="75"/>
+      <c r="G55" s="75"/>
+      <c r="H55" s="75"/>
+      <c r="I55" s="75"/>
+      <c r="J55" s="75"/>
+      <c r="K55" s="75"/>
+      <c r="L55" s="78"/>
+      <c r="M55" s="75"/>
+      <c r="N55" s="75"/>
+      <c r="O55" s="75"/>
+      <c r="P55" s="75"/>
+      <c r="Q55" s="75"/>
+      <c r="R55" s="75"/>
+      <c r="S55" s="75"/>
     </row>
     <row r="56" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="36"/>
-      <c r="B56" s="36"/>
-      <c r="C56" s="39"/>
-      <c r="D56" s="36"/>
-      <c r="E56" s="36"/>
-      <c r="F56" s="36"/>
-      <c r="G56" s="36"/>
-      <c r="H56" s="36"/>
-      <c r="I56" s="36"/>
-      <c r="J56" s="36"/>
-      <c r="K56" s="36"/>
-      <c r="L56" s="39"/>
-      <c r="M56" s="36"/>
-      <c r="N56" s="36"/>
-      <c r="O56" s="36"/>
-      <c r="P56" s="36"/>
-      <c r="Q56" s="36"/>
-      <c r="R56" s="36"/>
-      <c r="S56" s="36"/>
+      <c r="A56" s="75"/>
+      <c r="B56" s="75"/>
+      <c r="C56" s="78"/>
+      <c r="D56" s="75"/>
+      <c r="E56" s="75"/>
+      <c r="F56" s="75"/>
+      <c r="G56" s="75"/>
+      <c r="H56" s="75"/>
+      <c r="I56" s="75"/>
+      <c r="J56" s="75"/>
+      <c r="K56" s="75"/>
+      <c r="L56" s="78"/>
+      <c r="M56" s="75"/>
+      <c r="N56" s="75"/>
+      <c r="O56" s="75"/>
+      <c r="P56" s="75"/>
+      <c r="Q56" s="75"/>
+      <c r="R56" s="75"/>
+      <c r="S56" s="75"/>
     </row>
     <row r="57" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A57" s="36"/>
-      <c r="B57" s="36"/>
-      <c r="C57" s="39"/>
-      <c r="D57" s="36"/>
-      <c r="E57" s="36"/>
-      <c r="F57" s="36"/>
-      <c r="G57" s="36"/>
-      <c r="H57" s="36"/>
-      <c r="I57" s="36"/>
-      <c r="J57" s="36"/>
-      <c r="K57" s="36"/>
-      <c r="L57" s="39"/>
-      <c r="M57" s="36"/>
-      <c r="N57" s="36"/>
-      <c r="O57" s="36"/>
-      <c r="P57" s="36"/>
-      <c r="Q57" s="36"/>
-      <c r="R57" s="36"/>
-      <c r="S57" s="36"/>
+      <c r="A57" s="75"/>
+      <c r="B57" s="75"/>
+      <c r="C57" s="78"/>
+      <c r="D57" s="75"/>
+      <c r="E57" s="75"/>
+      <c r="F57" s="75"/>
+      <c r="G57" s="75"/>
+      <c r="H57" s="75"/>
+      <c r="I57" s="75"/>
+      <c r="J57" s="75"/>
+      <c r="K57" s="75"/>
+      <c r="L57" s="78"/>
+      <c r="M57" s="75"/>
+      <c r="N57" s="75"/>
+      <c r="O57" s="75"/>
+      <c r="P57" s="75"/>
+      <c r="Q57" s="75"/>
+      <c r="R57" s="75"/>
+      <c r="S57" s="75"/>
     </row>
     <row r="58" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A58" s="36"/>
-      <c r="B58" s="36"/>
-      <c r="C58" s="39"/>
-      <c r="D58" s="36"/>
-      <c r="E58" s="36"/>
-      <c r="F58" s="36"/>
-      <c r="G58" s="36"/>
-      <c r="H58" s="36"/>
-      <c r="I58" s="36"/>
-      <c r="J58" s="36"/>
-      <c r="K58" s="36"/>
-      <c r="L58" s="39"/>
-      <c r="M58" s="36"/>
-      <c r="N58" s="36"/>
-      <c r="O58" s="36"/>
-      <c r="P58" s="36"/>
-      <c r="Q58" s="36"/>
-      <c r="R58" s="36"/>
-      <c r="S58" s="36"/>
+      <c r="A58" s="75"/>
+      <c r="B58" s="75"/>
+      <c r="C58" s="78"/>
+      <c r="D58" s="75"/>
+      <c r="E58" s="75"/>
+      <c r="F58" s="75"/>
+      <c r="G58" s="75"/>
+      <c r="H58" s="75"/>
+      <c r="I58" s="75"/>
+      <c r="J58" s="75"/>
+      <c r="K58" s="75"/>
+      <c r="L58" s="78"/>
+      <c r="M58" s="75"/>
+      <c r="N58" s="75"/>
+      <c r="O58" s="75"/>
+      <c r="P58" s="75"/>
+      <c r="Q58" s="75"/>
+      <c r="R58" s="75"/>
+      <c r="S58" s="75"/>
     </row>
     <row r="59" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="58"/>
-      <c r="B59" s="37"/>
-      <c r="C59" s="40"/>
-      <c r="D59" s="37"/>
-      <c r="E59" s="37"/>
-      <c r="F59" s="37"/>
-      <c r="G59" s="37"/>
-      <c r="H59" s="37"/>
-      <c r="I59" s="37"/>
-      <c r="J59" s="37"/>
-      <c r="K59" s="36"/>
-      <c r="L59" s="40"/>
-      <c r="M59" s="37"/>
-      <c r="N59" s="37"/>
-      <c r="O59" s="37"/>
-      <c r="P59" s="36"/>
-      <c r="Q59" s="37"/>
-      <c r="R59" s="37"/>
-      <c r="S59" s="37"/>
+      <c r="A59" s="86"/>
+      <c r="B59" s="76"/>
+      <c r="C59" s="79"/>
+      <c r="D59" s="76"/>
+      <c r="E59" s="76"/>
+      <c r="F59" s="76"/>
+      <c r="G59" s="76"/>
+      <c r="H59" s="76"/>
+      <c r="I59" s="76"/>
+      <c r="J59" s="76"/>
+      <c r="K59" s="75"/>
+      <c r="L59" s="79"/>
+      <c r="M59" s="76"/>
+      <c r="N59" s="76"/>
+      <c r="O59" s="76"/>
+      <c r="P59" s="75"/>
+      <c r="Q59" s="76"/>
+      <c r="R59" s="76"/>
+      <c r="S59" s="76"/>
     </row>
     <row r="60" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="59" t="s">
+      <c r="A60" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="B60" s="56"/>
+      <c r="B60" s="34"/>
       <c r="C60" s="19" t="s">
         <v>78</v>
       </c>
@@ -4720,12 +4738,12 @@
         <v>6</v>
       </c>
       <c r="O60" s="21">
-        <f>ROUND(((J60/J113)*100),1)</f>
-        <v>1.1000000000000001</v>
+        <f>ROUND(((J60/J115)*100),1)</f>
+        <v>1</v>
       </c>
       <c r="P60" s="21">
         <f>O60</f>
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="Q60" s="21">
         <v>0</v>
@@ -4738,10 +4756,10 @@
       </c>
     </row>
     <row r="61" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="60" t="s">
+      <c r="A61" s="85" t="s">
         <v>80</v>
       </c>
-      <c r="B61" s="57"/>
+      <c r="B61" s="35"/>
       <c r="C61" s="19" t="s">
         <v>81</v>
       </c>
@@ -4764,11 +4782,11 @@
         <v>0.3</v>
       </c>
       <c r="J61" s="31">
-        <f t="shared" ref="J61:J92" si="5">SUM(E61:I61)</f>
+        <f t="shared" ref="J61:J93" si="5">SUM(E61:I61)</f>
         <v>1.5</v>
       </c>
       <c r="K61" s="21">
-        <f t="shared" ref="K61:K92" si="6">J61+K60</f>
+        <f t="shared" ref="K61:K93" si="6">J61+K60</f>
         <v>3</v>
       </c>
       <c r="L61" s="21" t="s">
@@ -4781,12 +4799,12 @@
         <v>6</v>
       </c>
       <c r="O61" s="21">
-        <f>ROUND(((J61/J113)*100),1)</f>
-        <v>1.1000000000000001</v>
+        <f>ROUND(((J61/J115)*100),1)</f>
+        <v>1</v>
       </c>
       <c r="P61" s="21">
-        <f t="shared" ref="P61:P92" si="7">O61+P60</f>
-        <v>2.2000000000000002</v>
+        <f t="shared" ref="P61:P93" si="7">O61+P60</f>
+        <v>2</v>
       </c>
       <c r="Q61" s="21">
         <v>0</v>
@@ -4800,8 +4818,8 @@
       </c>
     </row>
     <row r="62" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="60"/>
-      <c r="B62" s="57"/>
+      <c r="A62" s="85"/>
+      <c r="B62" s="35"/>
       <c r="C62" s="19" t="s">
         <v>38</v>
       </c>
@@ -4841,12 +4859,12 @@
         <v>6</v>
       </c>
       <c r="O62" s="21">
-        <f>ROUND(((J62/J113)*100),1)</f>
+        <f>ROUND(((J62/J115)*100),1)</f>
         <v>0.7</v>
       </c>
       <c r="P62" s="21">
         <f t="shared" si="7"/>
-        <v>2.9000000000000004</v>
+        <v>2.7</v>
       </c>
       <c r="Q62" s="21">
         <v>0</v>
@@ -4860,10 +4878,10 @@
       </c>
     </row>
     <row r="63" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="60" t="s">
+      <c r="A63" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="B63" s="57"/>
+      <c r="B63" s="35"/>
       <c r="C63" s="19" t="s">
         <v>83</v>
       </c>
@@ -4903,12 +4921,12 @@
         <v>6</v>
       </c>
       <c r="O63" s="21">
-        <f>ROUND(((J63/J113)*100),1)</f>
+        <f>ROUND(((J63/J115)*100),1)</f>
         <v>0.7</v>
       </c>
       <c r="P63" s="21">
         <f t="shared" si="7"/>
-        <v>3.6000000000000005</v>
+        <v>3.4000000000000004</v>
       </c>
       <c r="Q63" s="21">
         <v>0</v>
@@ -4922,8 +4940,8 @@
       </c>
     </row>
     <row r="64" spans="1:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="60"/>
-      <c r="B64" s="57"/>
+      <c r="A64" s="85"/>
+      <c r="B64" s="35"/>
       <c r="C64" s="19" t="s">
         <v>44</v>
       </c>
@@ -4963,12 +4981,12 @@
         <v>6</v>
       </c>
       <c r="O64" s="21">
-        <f>ROUND(((J64/J113)*100),1)</f>
-        <v>2.2000000000000002</v>
+        <f>ROUND(((J64/J115)*100),1)</f>
+        <v>2.1</v>
       </c>
       <c r="P64" s="21">
         <f t="shared" si="7"/>
-        <v>5.8000000000000007</v>
+        <v>5.5</v>
       </c>
       <c r="Q64" s="21">
         <v>0</v>
@@ -4982,8 +5000,8 @@
       </c>
     </row>
     <row r="65" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="60"/>
-      <c r="B65" s="57"/>
+      <c r="A65" s="85"/>
+      <c r="B65" s="35"/>
       <c r="C65" s="33" t="s">
         <v>115</v>
       </c>
@@ -5023,12 +5041,12 @@
         <v>6</v>
       </c>
       <c r="O65" s="21">
-        <f>ROUND(((J65/J113)*100),1)</f>
-        <v>1.1000000000000001</v>
+        <f>ROUND(((J65/J115)*100),1)</f>
+        <v>1</v>
       </c>
       <c r="P65" s="21">
         <f t="shared" si="7"/>
-        <v>6.9</v>
+        <v>6.5</v>
       </c>
       <c r="Q65" s="21">
         <v>0</v>
@@ -5042,8 +5060,8 @@
       </c>
     </row>
     <row r="66" spans="1:19" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="60"/>
-      <c r="B66" s="57"/>
+      <c r="A66" s="85"/>
+      <c r="B66" s="35"/>
       <c r="C66" s="19" t="s">
         <v>85</v>
       </c>
@@ -5083,12 +5101,12 @@
         <v>6</v>
       </c>
       <c r="O66" s="21">
-        <f>ROUND(((J66/J113)*100),1)</f>
+        <f>ROUND(((J66/J115)*100),1)</f>
         <v>0.7</v>
       </c>
       <c r="P66" s="21">
         <f t="shared" si="7"/>
-        <v>7.6000000000000005</v>
+        <v>7.2</v>
       </c>
       <c r="Q66" s="21">
         <v>1.5</v>
@@ -5102,8 +5120,8 @@
       </c>
     </row>
     <row r="67" spans="1:19" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="60"/>
-      <c r="B67" s="57"/>
+      <c r="A67" s="85"/>
+      <c r="B67" s="35"/>
       <c r="C67" s="19" t="s">
         <v>86</v>
       </c>
@@ -5143,25 +5161,27 @@
         <v>6</v>
       </c>
       <c r="O67" s="21">
-        <f>ROUND(((J67/J113)*100),1)</f>
+        <f>ROUND(((J67/J115)*100),1)</f>
         <v>0.7</v>
       </c>
       <c r="P67" s="21">
         <f t="shared" si="7"/>
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="Q67" s="21"/>
+        <v>7.9</v>
+      </c>
+      <c r="Q67" s="21">
+        <v>0.4</v>
+      </c>
       <c r="R67" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S67" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:19" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="60"/>
-      <c r="B68" s="57"/>
+      <c r="A68" s="85"/>
+      <c r="B68" s="35"/>
       <c r="C68" s="19" t="s">
         <v>87</v>
       </c>
@@ -5201,29 +5221,29 @@
         <v>6</v>
       </c>
       <c r="O68" s="21">
-        <f>ROUND(((J68/J113)*100),1)</f>
+        <f>ROUND(((J68/J115)*100),1)</f>
         <v>0.7</v>
       </c>
       <c r="P68" s="21">
         <f t="shared" si="7"/>
-        <v>9</v>
+        <v>8.6</v>
       </c>
       <c r="Q68" s="21">
         <v>0</v>
       </c>
       <c r="R68" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S68" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="60" t="s">
+      <c r="A69" s="85" t="s">
         <v>88</v>
       </c>
-      <c r="B69" s="57"/>
+      <c r="B69" s="35"/>
       <c r="C69" s="19" t="s">
         <v>49</v>
       </c>
@@ -5263,27 +5283,27 @@
         <v>7</v>
       </c>
       <c r="O69" s="21">
-        <f>ROUND(((J69/J113)*100),1)</f>
-        <v>1.5</v>
+        <f>ROUND(((J69/J115)*100),1)</f>
+        <v>1.4</v>
       </c>
       <c r="P69" s="21">
         <f t="shared" si="7"/>
-        <v>10.5</v>
+        <v>10</v>
       </c>
       <c r="Q69" s="21">
         <v>0</v>
       </c>
       <c r="R69" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S69" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="60"/>
-      <c r="B70" s="57"/>
+      <c r="A70" s="85"/>
+      <c r="B70" s="35"/>
       <c r="C70" s="19" t="s">
         <v>50</v>
       </c>
@@ -5323,27 +5343,27 @@
         <v>7</v>
       </c>
       <c r="O70" s="21">
-        <f>ROUND(((J70/J113)*100),1)</f>
+        <f>ROUND(((J70/J115)*100),1)</f>
         <v>0.7</v>
       </c>
       <c r="P70" s="21">
         <f t="shared" si="7"/>
-        <v>11.2</v>
+        <v>10.7</v>
       </c>
       <c r="Q70" s="21">
         <v>0</v>
       </c>
       <c r="R70" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S70" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="71" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="60"/>
-      <c r="B71" s="57"/>
+      <c r="A71" s="85"/>
+      <c r="B71" s="35"/>
       <c r="C71" s="19" t="s">
         <v>51</v>
       </c>
@@ -5383,29 +5403,29 @@
         <v>7</v>
       </c>
       <c r="O71" s="21">
-        <f>ROUND(((J71/J113)*100),1)</f>
+        <f>ROUND(((J71/J115)*100),1)</f>
         <v>0.7</v>
       </c>
       <c r="P71" s="21">
         <f t="shared" si="7"/>
-        <v>11.899999999999999</v>
+        <v>11.399999999999999</v>
       </c>
       <c r="Q71" s="21">
         <v>0</v>
       </c>
       <c r="R71" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S71" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="72" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="61" t="s">
+      <c r="A72" s="93" t="s">
         <v>89</v>
       </c>
-      <c r="B72" s="56"/>
+      <c r="B72" s="34"/>
       <c r="C72" s="19" t="s">
         <v>54</v>
       </c>
@@ -5445,27 +5465,27 @@
         <v>7</v>
       </c>
       <c r="O72" s="21">
-        <f>ROUND(((J72/J113)*100),1)</f>
-        <v>1.5</v>
+        <f>ROUND(((J72/J115)*100),1)</f>
+        <v>1.4</v>
       </c>
       <c r="P72" s="21">
         <f t="shared" si="7"/>
-        <v>13.399999999999999</v>
+        <v>12.799999999999999</v>
       </c>
       <c r="Q72" s="21">
         <v>0</v>
       </c>
       <c r="R72" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S72" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="73" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="62"/>
-      <c r="B73" s="56"/>
+      <c r="A73" s="94"/>
+      <c r="B73" s="34"/>
       <c r="C73" s="19" t="s">
         <v>55</v>
       </c>
@@ -5505,27 +5525,27 @@
         <v>7</v>
       </c>
       <c r="O73" s="21">
-        <f>ROUND(((J73/J113)*100),1)</f>
-        <v>1.5</v>
+        <f>ROUND(((J73/J115)*100),1)</f>
+        <v>1.4</v>
       </c>
       <c r="P73" s="21">
         <f t="shared" si="7"/>
-        <v>14.899999999999999</v>
+        <v>14.2</v>
       </c>
       <c r="Q73" s="21">
         <v>0</v>
       </c>
       <c r="R73" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S73" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="74" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="62"/>
-      <c r="B74" s="56"/>
+      <c r="A74" s="94"/>
+      <c r="B74" s="34"/>
       <c r="C74" s="19" t="s">
         <v>56</v>
       </c>
@@ -5565,27 +5585,27 @@
         <v>7</v>
       </c>
       <c r="O74" s="21">
-        <f>ROUND(((J74/J113)*100),1)</f>
+        <f>ROUND(((J74/J115)*100),1)</f>
         <v>0.7</v>
       </c>
       <c r="P74" s="21">
         <f t="shared" si="7"/>
-        <v>15.599999999999998</v>
+        <v>14.899999999999999</v>
       </c>
       <c r="Q74" s="21">
         <v>0</v>
       </c>
       <c r="R74" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S74" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="62"/>
-      <c r="B75" s="56"/>
+      <c r="A75" s="94"/>
+      <c r="B75" s="34"/>
       <c r="C75" s="19" t="s">
         <v>57</v>
       </c>
@@ -5625,27 +5645,27 @@
         <v>7</v>
       </c>
       <c r="O75" s="21">
-        <f>ROUND(((J75/J113)*100),1)</f>
+        <f>ROUND(((J75/J115)*100),1)</f>
         <v>0.7</v>
       </c>
       <c r="P75" s="21">
         <f t="shared" si="7"/>
-        <v>16.299999999999997</v>
+        <v>15.599999999999998</v>
       </c>
       <c r="Q75" s="21">
         <v>0</v>
       </c>
       <c r="R75" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S75" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="76" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="62"/>
-      <c r="B76" s="56"/>
+      <c r="A76" s="94"/>
+      <c r="B76" s="34"/>
       <c r="C76" s="19" t="s">
         <v>58</v>
       </c>
@@ -5685,27 +5705,27 @@
         <v>7</v>
       </c>
       <c r="O76" s="21">
-        <f>ROUND(((J76/J113)*100),1)</f>
+        <f>ROUND(((J76/J115)*100),1)</f>
         <v>0.7</v>
       </c>
       <c r="P76" s="21">
         <f t="shared" si="7"/>
-        <v>16.999999999999996</v>
+        <v>16.299999999999997</v>
       </c>
       <c r="Q76" s="21">
         <v>0</v>
       </c>
       <c r="R76" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S76" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="62"/>
-      <c r="B77" s="56"/>
+      <c r="A77" s="94"/>
+      <c r="B77" s="34"/>
       <c r="C77" s="19" t="s">
         <v>91</v>
       </c>
@@ -5741,25 +5761,25 @@
         <v>7</v>
       </c>
       <c r="O77" s="21">
-        <f>ROUND(((J77/J113)*100),1)</f>
-        <v>3.7</v>
+        <f>ROUND(((J77/J115)*100),1)</f>
+        <v>3.4</v>
       </c>
       <c r="P77" s="21">
         <f t="shared" si="7"/>
-        <v>20.699999999999996</v>
+        <v>19.699999999999996</v>
       </c>
       <c r="Q77" s="21"/>
       <c r="R77" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S77" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="62"/>
-      <c r="B78" s="56"/>
+      <c r="A78" s="94"/>
+      <c r="B78" s="34"/>
       <c r="C78" s="19" t="s">
         <v>92</v>
       </c>
@@ -5799,25 +5819,25 @@
         <v>7</v>
       </c>
       <c r="O78" s="21">
-        <f>ROUND(((J78/J113)*100),1)</f>
+        <f>ROUND(((J78/J115)*100),1)</f>
         <v>0.7</v>
       </c>
       <c r="P78" s="21">
         <f t="shared" si="7"/>
-        <v>21.399999999999995</v>
+        <v>20.399999999999995</v>
       </c>
       <c r="Q78" s="21"/>
       <c r="R78" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S78" s="21">
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="62"/>
-      <c r="B79" s="56"/>
+    <row r="79" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="94"/>
+      <c r="B79" s="34"/>
       <c r="C79" s="19" t="s">
         <v>93</v>
       </c>
@@ -5857,23 +5877,23 @@
         <v>7</v>
       </c>
       <c r="O79" s="21">
-        <f>ROUND(((J79/J113)*100),1)</f>
-        <v>7.4</v>
+        <f>ROUND(((J79/J115)*100),1)</f>
+        <v>6.9</v>
       </c>
       <c r="P79" s="21">
         <f t="shared" si="7"/>
-        <v>28.799999999999997</v>
+        <v>27.299999999999997</v>
       </c>
       <c r="Q79" s="21"/>
       <c r="R79" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S79" s="21"/>
     </row>
     <row r="80" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="62"/>
-      <c r="B80" s="56"/>
+      <c r="A80" s="94"/>
+      <c r="B80" s="34"/>
       <c r="C80" s="19" t="s">
         <v>94</v>
       </c>
@@ -5913,23 +5933,23 @@
         <v>7</v>
       </c>
       <c r="O80" s="21">
-        <f>ROUND(((J80/J113)*100),1)</f>
+        <f>ROUND(((J80/J115)*100),1)</f>
         <v>0.7</v>
       </c>
       <c r="P80" s="21">
         <f t="shared" si="7"/>
-        <v>29.499999999999996</v>
+        <v>27.999999999999996</v>
       </c>
       <c r="Q80" s="21"/>
       <c r="R80" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S80" s="21"/>
     </row>
     <row r="81" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="62"/>
-      <c r="B81" s="56"/>
+      <c r="A81" s="94"/>
+      <c r="B81" s="34"/>
       <c r="C81" s="19" t="s">
         <v>96</v>
       </c>
@@ -5969,23 +5989,23 @@
         <v>7</v>
       </c>
       <c r="O81" s="21">
-        <f>ROUND(((J81/J113)*100),1)</f>
+        <f>ROUND(((J81/J115)*100),1)</f>
         <v>0.7</v>
       </c>
       <c r="P81" s="21">
         <f t="shared" si="7"/>
-        <v>30.199999999999996</v>
+        <v>28.699999999999996</v>
       </c>
       <c r="Q81" s="21"/>
       <c r="R81" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S81" s="21"/>
     </row>
     <row r="82" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="63"/>
-      <c r="B82" s="56"/>
+      <c r="A82" s="95"/>
+      <c r="B82" s="34"/>
       <c r="C82" s="19" t="s">
         <v>97</v>
       </c>
@@ -6025,53 +6045,53 @@
         <v>7</v>
       </c>
       <c r="O82" s="21">
-        <f>ROUND(((J82/J113)*100),1)</f>
+        <f>ROUND(((J82/J115)*100),1)</f>
         <v>0.7</v>
       </c>
       <c r="P82" s="21">
         <f t="shared" si="7"/>
-        <v>30.899999999999995</v>
+        <v>29.399999999999995</v>
       </c>
       <c r="Q82" s="21"/>
       <c r="R82" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S82" s="21"/>
     </row>
     <row r="83" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="60" t="s">
+      <c r="A83" s="85" t="s">
         <v>98</v>
       </c>
-      <c r="B83" s="57"/>
-      <c r="C83" s="19" t="s">
-        <v>61</v>
+      <c r="B83" s="35"/>
+      <c r="C83" s="33" t="s">
+        <v>117</v>
       </c>
       <c r="D83" s="22">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E83" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F83" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G83" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H83" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I83" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J83" s="22">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K83" s="21">
-        <f t="shared" si="6"/>
-        <v>44.5</v>
+        <f>J83+K82</f>
+        <v>47.5</v>
       </c>
       <c r="L83" s="21" t="s">
         <v>33</v>
@@ -6083,88 +6103,87 @@
         <v>8</v>
       </c>
       <c r="O83" s="21">
-        <f>ROUND(((J83/J113)*100),1)</f>
-        <v>1.5</v>
+        <f>ROUND(((J83/J115)*100),1)</f>
+        <v>3.4</v>
       </c>
       <c r="P83" s="21">
-        <f t="shared" si="7"/>
-        <v>32.399999999999991</v>
+        <f>O83+P82</f>
+        <v>32.799999999999997</v>
       </c>
       <c r="Q83" s="21">
         <v>0</v>
       </c>
       <c r="R83" s="21">
-        <f t="shared" si="8"/>
-        <v>1.5</v>
+        <f>Q83+R82</f>
+        <v>1.9</v>
       </c>
       <c r="S83" s="21"/>
     </row>
     <row r="84" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="60"/>
-      <c r="B84" s="57"/>
-      <c r="C84" s="14" t="s">
+      <c r="A84" s="85"/>
+      <c r="B84" s="35"/>
+      <c r="C84" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D84" s="98">
+        <v>1</v>
+      </c>
+      <c r="E84" s="98">
+        <v>0</v>
+      </c>
+      <c r="F84" s="98">
+        <v>0</v>
+      </c>
+      <c r="G84" s="98">
+        <v>0</v>
+      </c>
+      <c r="H84" s="98">
+        <v>0</v>
+      </c>
+      <c r="I84" s="98">
+        <v>2</v>
+      </c>
+      <c r="J84" s="98">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K84" s="21">
+        <f>J84+K83</f>
+        <v>49.5</v>
+      </c>
+      <c r="L84" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="M84" s="96">
+        <v>3</v>
+      </c>
+      <c r="N84" s="96">
+        <v>8</v>
+      </c>
+      <c r="O84" s="21">
+        <f>ROUND(((J84/J115)*100),1)</f>
+        <v>1.4</v>
+      </c>
+      <c r="P84" s="21">
+        <f>O84+P83</f>
+        <v>34.199999999999996</v>
+      </c>
+      <c r="Q84" s="96"/>
+      <c r="R84" s="96"/>
+      <c r="S84" s="96"/>
+    </row>
+    <row r="85" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="85"/>
+      <c r="B85" s="35"/>
+      <c r="C85" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D84" s="22">
-        <v>1</v>
-      </c>
-      <c r="E84" s="22">
+      <c r="D85" s="22">
+        <v>1</v>
+      </c>
+      <c r="E85" s="22">
         <v>0.5</v>
       </c>
-      <c r="F84" s="22">
-        <v>0</v>
-      </c>
-      <c r="G84" s="22">
-        <v>0</v>
-      </c>
-      <c r="H84" s="22">
-        <v>0</v>
-      </c>
-      <c r="I84" s="22">
-        <v>0</v>
-      </c>
-      <c r="J84" s="22">
-        <f t="shared" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="K84" s="21">
-        <f t="shared" si="6"/>
-        <v>45</v>
-      </c>
-      <c r="L84" s="21"/>
-      <c r="M84" s="21"/>
-      <c r="N84" s="21">
-        <v>8</v>
-      </c>
-      <c r="O84" s="21">
-        <f>ROUND(((J84/J113)*100),1)</f>
-        <v>0.4</v>
-      </c>
-      <c r="P84" s="21">
-        <f t="shared" si="7"/>
-        <v>32.79999999999999</v>
-      </c>
-      <c r="Q84" s="21">
-        <v>0</v>
-      </c>
-      <c r="R84" s="21">
-        <f t="shared" si="8"/>
-        <v>1.5</v>
-      </c>
-      <c r="S84" s="21"/>
-    </row>
-    <row r="85" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="60"/>
-      <c r="B85" s="57"/>
-      <c r="C85" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="D85" s="22">
-        <v>0</v>
-      </c>
-      <c r="E85" s="22">
-        <v>0</v>
-      </c>
       <c r="F85" s="22">
         <v>0</v>
       </c>
@@ -6172,7 +6191,7 @@
         <v>0</v>
       </c>
       <c r="H85" s="22">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I85" s="22">
         <v>0</v>
@@ -6182,41 +6201,39 @@
         <v>0.5</v>
       </c>
       <c r="K85" s="21">
-        <f t="shared" si="6"/>
-        <v>45.5</v>
-      </c>
-      <c r="L85" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="M85" s="21">
-        <v>1</v>
-      </c>
+        <f>J85+K83</f>
+        <v>48</v>
+      </c>
+      <c r="L85" s="21"/>
+      <c r="M85" s="21"/>
       <c r="N85" s="21">
         <v>8</v>
       </c>
       <c r="O85" s="21">
-        <f>ROUND(((J85/J113)*100),1)</f>
-        <v>0.4</v>
+        <f>ROUND(((J85/J115)*100),1)</f>
+        <v>0.3</v>
       </c>
       <c r="P85" s="21">
-        <f t="shared" si="7"/>
-        <v>33.199999999999989</v>
-      </c>
-      <c r="Q85" s="21"/>
+        <f>O85+P84</f>
+        <v>34.499999999999993</v>
+      </c>
+      <c r="Q85" s="21">
+        <v>0</v>
+      </c>
       <c r="R85" s="21">
-        <f t="shared" si="8"/>
-        <v>1.5</v>
+        <f>Q85+R83</f>
+        <v>1.9</v>
       </c>
       <c r="S85" s="21"/>
     </row>
     <row r="86" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="60"/>
-      <c r="B86" s="57"/>
+      <c r="A86" s="85"/>
+      <c r="B86" s="35"/>
       <c r="C86" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D86" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E86" s="22">
         <v>0</v>
@@ -6225,183 +6242,185 @@
         <v>0</v>
       </c>
       <c r="G86" s="22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H86" s="22">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I86" s="22">
         <v>0</v>
       </c>
       <c r="J86" s="22">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="K86" s="21">
         <f t="shared" si="6"/>
-        <v>47.5</v>
+        <v>48.5</v>
       </c>
       <c r="L86" s="21" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="M86" s="21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N86" s="21">
         <v>8</v>
       </c>
       <c r="O86" s="21">
-        <f>ROUND(((J86/J113)*100),1)</f>
-        <v>1.5</v>
+        <f>ROUND(((J86/J115)*100),1)</f>
+        <v>0.3</v>
       </c>
       <c r="P86" s="21">
         <f t="shared" si="7"/>
-        <v>34.699999999999989</v>
-      </c>
-      <c r="Q86" s="21">
-        <v>0</v>
-      </c>
+        <v>34.79999999999999</v>
+      </c>
+      <c r="Q86" s="21"/>
       <c r="R86" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S86" s="21"/>
     </row>
     <row r="87" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="60"/>
-      <c r="B87" s="57"/>
+      <c r="A87" s="85"/>
+      <c r="B87" s="35"/>
       <c r="C87" s="19" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="D87" s="22">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E87" s="22">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F87" s="22">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G87" s="22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H87" s="22">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I87" s="22">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J87" s="22">
         <f t="shared" si="5"/>
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="K87" s="21">
         <f t="shared" si="6"/>
-        <v>68.5</v>
+        <v>50.5</v>
       </c>
       <c r="L87" s="21" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="M87" s="21">
-        <v>336</v>
+        <v>2</v>
       </c>
       <c r="N87" s="21">
         <v>8</v>
       </c>
       <c r="O87" s="21">
-        <f>ROUND(((J87/J113)*100),1)</f>
-        <v>15.6</v>
+        <f>ROUND(((J87/J115)*100),1)</f>
+        <v>1.4</v>
       </c>
       <c r="P87" s="21">
         <f t="shared" si="7"/>
-        <v>50.29999999999999</v>
+        <v>36.199999999999989</v>
       </c>
       <c r="Q87" s="21">
         <v>0</v>
       </c>
       <c r="R87" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S87" s="21"/>
     </row>
     <row r="88" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="60"/>
-      <c r="B88" s="57"/>
+      <c r="A88" s="85"/>
+      <c r="B88" s="35"/>
       <c r="C88" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D88" s="22">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E88" s="22">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F88" s="22">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G88" s="22">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H88" s="22">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I88" s="22">
         <v>3</v>
       </c>
       <c r="J88" s="22">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="K88" s="21">
         <f t="shared" si="6"/>
         <v>71.5</v>
       </c>
-      <c r="L88" s="21"/>
-      <c r="M88" s="21"/>
+      <c r="L88" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="M88" s="21">
+        <v>336</v>
+      </c>
       <c r="N88" s="21">
         <v>8</v>
       </c>
       <c r="O88" s="21">
-        <f>ROUND(((J88/J113)*100),1)</f>
-        <v>2.2000000000000002</v>
+        <f>ROUND(((J88/J115)*100),1)</f>
+        <v>14.5</v>
       </c>
       <c r="P88" s="21">
         <f t="shared" si="7"/>
-        <v>52.499999999999993</v>
+        <v>50.699999999999989</v>
       </c>
       <c r="Q88" s="21">
         <v>0</v>
       </c>
       <c r="R88" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S88" s="21"/>
     </row>
     <row r="89" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="60"/>
-      <c r="B89" s="57"/>
+      <c r="A89" s="85"/>
+      <c r="B89" s="35"/>
       <c r="C89" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D89" s="22">
         <v>1</v>
       </c>
       <c r="E89" s="22">
+        <v>0</v>
+      </c>
+      <c r="F89" s="22">
+        <v>0</v>
+      </c>
+      <c r="G89" s="22">
+        <v>0</v>
+      </c>
+      <c r="H89" s="22">
+        <v>0</v>
+      </c>
+      <c r="I89" s="22">
         <v>3</v>
-      </c>
-      <c r="F89" s="22">
-        <v>0</v>
-      </c>
-      <c r="G89" s="22">
-        <v>0</v>
-      </c>
-      <c r="H89" s="22">
-        <v>0</v>
-      </c>
-      <c r="I89" s="22">
-        <v>0</v>
       </c>
       <c r="J89" s="22">
         <f t="shared" si="5"/>
@@ -6411,51 +6430,45 @@
         <f t="shared" si="6"/>
         <v>74.5</v>
       </c>
-      <c r="L89" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="M89" s="21">
-        <v>1</v>
-      </c>
+      <c r="L89" s="21"/>
+      <c r="M89" s="21"/>
       <c r="N89" s="21">
         <v>8</v>
       </c>
       <c r="O89" s="21">
-        <f>ROUND(((J89/J113)*100),1)</f>
-        <v>2.2000000000000002</v>
+        <f>ROUND(((J89/J115)*100),1)</f>
+        <v>2.1</v>
       </c>
       <c r="P89" s="21">
         <f t="shared" si="7"/>
-        <v>54.699999999999996</v>
+        <v>52.79999999999999</v>
       </c>
       <c r="Q89" s="21">
         <v>0</v>
       </c>
       <c r="R89" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S89" s="21"/>
     </row>
     <row r="90" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="60" t="s">
-        <v>101</v>
-      </c>
-      <c r="B90" s="57"/>
+      <c r="A90" s="85"/>
+      <c r="B90" s="35"/>
       <c r="C90" s="19" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="D90" s="22">
         <v>1</v>
       </c>
       <c r="E90" s="22">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F90" s="22">
         <v>0</v>
       </c>
       <c r="G90" s="22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H90" s="22">
         <v>0</v>
@@ -6465,161 +6478,163 @@
       </c>
       <c r="J90" s="22">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K90" s="21">
         <f t="shared" si="6"/>
-        <v>76.5</v>
+        <v>77.5</v>
       </c>
       <c r="L90" s="21" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="M90" s="21">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="N90" s="21">
         <v>8</v>
       </c>
       <c r="O90" s="21">
-        <f>ROUND(((J90/J113)*100),1)</f>
-        <v>1.5</v>
+        <f>ROUND(((J90/J115)*100),1)</f>
+        <v>2.1</v>
       </c>
       <c r="P90" s="21">
         <f t="shared" si="7"/>
-        <v>56.199999999999996</v>
+        <v>54.899999999999991</v>
       </c>
       <c r="Q90" s="21">
         <v>0</v>
       </c>
       <c r="R90" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S90" s="21"/>
     </row>
     <row r="91" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="60" t="s">
+      <c r="A91" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="B91" s="57"/>
+      <c r="B91" s="35"/>
       <c r="C91" s="19" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
       <c r="D91" s="22">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E91" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F91" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G91" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H91" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I91" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J91" s="22">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K91" s="21">
         <f t="shared" si="6"/>
-        <v>81.5</v>
+        <v>79.5</v>
       </c>
       <c r="L91" s="21" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="M91" s="21">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="N91" s="21">
         <v>8</v>
       </c>
       <c r="O91" s="21">
-        <f>ROUND(((J91/J113)*100),1)</f>
-        <v>3.7</v>
+        <f>ROUND(((J91/J115)*100),1)</f>
+        <v>1.4</v>
       </c>
       <c r="P91" s="21">
         <f t="shared" si="7"/>
-        <v>59.9</v>
+        <v>56.29999999999999</v>
       </c>
       <c r="Q91" s="21">
         <v>0</v>
       </c>
       <c r="R91" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S91" s="21"/>
     </row>
     <row r="92" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="60"/>
-      <c r="B92" s="57"/>
+      <c r="A92" s="85" t="s">
+        <v>101</v>
+      </c>
+      <c r="B92" s="35"/>
       <c r="C92" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D92" s="22">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E92" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F92" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G92" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H92" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I92" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J92" s="22">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K92" s="21">
         <f t="shared" si="6"/>
-        <v>83.5</v>
+        <v>84.5</v>
       </c>
       <c r="L92" s="21" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="M92" s="21">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="N92" s="21">
         <v>8</v>
       </c>
       <c r="O92" s="21">
-        <f>ROUND(((J92/J113)*100),1)</f>
-        <v>1.5</v>
+        <f>ROUND(((J92/J115)*100),1)</f>
+        <v>3.4</v>
       </c>
       <c r="P92" s="21">
         <f t="shared" si="7"/>
-        <v>61.4</v>
+        <v>59.699999999999989</v>
       </c>
       <c r="Q92" s="21">
         <v>0</v>
       </c>
       <c r="R92" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S92" s="21"/>
     </row>
     <row r="93" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="60"/>
-      <c r="B93" s="57"/>
+      <c r="A93" s="85"/>
+      <c r="B93" s="35"/>
       <c r="C93" s="19" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="D93" s="22">
         <v>1</v>
@@ -6631,77 +6646,79 @@
         <v>0</v>
       </c>
       <c r="G93" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H93" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I93" s="22">
         <v>0</v>
       </c>
       <c r="J93" s="22">
-        <f t="shared" ref="J93:J112" si="9">SUM(E93:I93)</f>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="K93" s="21">
-        <f t="shared" ref="K93:K112" si="10">J93+K92</f>
-        <v>84.5</v>
+        <f t="shared" si="6"/>
+        <v>86.5</v>
       </c>
       <c r="L93" s="21" t="s">
-        <v>95</v>
+        <v>33</v>
       </c>
       <c r="M93" s="21">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="N93" s="21">
         <v>8</v>
       </c>
       <c r="O93" s="21">
-        <f>ROUND(((J93/J113)*100),1)</f>
-        <v>0.7</v>
+        <f>ROUND(((J93/J115)*100),1)</f>
+        <v>1.4</v>
       </c>
       <c r="P93" s="21">
-        <f t="shared" ref="P93:P112" si="11">O93+P92</f>
-        <v>62.1</v>
-      </c>
-      <c r="Q93" s="21"/>
+        <f t="shared" si="7"/>
+        <v>61.099999999999987</v>
+      </c>
+      <c r="Q93" s="21">
+        <v>0</v>
+      </c>
       <c r="R93" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S93" s="21"/>
     </row>
-    <row r="94" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="60"/>
-      <c r="B94" s="57"/>
+    <row r="94" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="85"/>
+      <c r="B94" s="35"/>
       <c r="C94" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D94" s="22">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E94" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F94" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G94" s="22">
         <v>1</v>
       </c>
       <c r="H94" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I94" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J94" s="22">
-        <f t="shared" si="9"/>
-        <v>5</v>
+        <f t="shared" ref="J94:J114" si="9">SUM(E94:I94)</f>
+        <v>1</v>
       </c>
       <c r="K94" s="21">
-        <f t="shared" si="10"/>
-        <v>89.5</v>
+        <f t="shared" ref="K94:K114" si="10">J94+K93</f>
+        <v>87.5</v>
       </c>
       <c r="L94" s="21" t="s">
         <v>95</v>
@@ -6713,51 +6730,51 @@
         <v>8</v>
       </c>
       <c r="O94" s="21">
-        <f>ROUND(((J94/J113)*100),1)</f>
-        <v>3.7</v>
+        <f>ROUND(((J94/J115)*100),1)</f>
+        <v>0.7</v>
       </c>
       <c r="P94" s="21">
-        <f t="shared" si="11"/>
-        <v>65.8</v>
+        <f t="shared" ref="P94:P114" si="11">O94+P93</f>
+        <v>61.79999999999999</v>
       </c>
       <c r="Q94" s="21"/>
       <c r="R94" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S94" s="21"/>
     </row>
     <row r="95" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="60"/>
-      <c r="B95" s="57"/>
+      <c r="A95" s="85"/>
+      <c r="B95" s="35"/>
       <c r="C95" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D95" s="22">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E95" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F95" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G95" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H95" s="22">
         <v>1</v>
       </c>
       <c r="I95" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J95" s="22">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K95" s="21">
         <f t="shared" si="10"/>
-        <v>90.5</v>
+        <v>92.5</v>
       </c>
       <c r="L95" s="21" t="s">
         <v>95</v>
@@ -6769,149 +6786,149 @@
         <v>8</v>
       </c>
       <c r="O95" s="21">
-        <f>ROUND(((J95/J113)*100),1)</f>
-        <v>0.7</v>
+        <f>ROUND(((J95/J115)*100),1)</f>
+        <v>3.4</v>
       </c>
       <c r="P95" s="21">
         <f t="shared" si="11"/>
-        <v>66.5</v>
+        <v>65.199999999999989</v>
       </c>
       <c r="Q95" s="21"/>
       <c r="R95" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S95" s="21"/>
     </row>
     <row r="96" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="60"/>
-      <c r="B96" s="57"/>
+      <c r="A96" s="85"/>
+      <c r="B96" s="35"/>
       <c r="C96" s="19" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="D96" s="22">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E96" s="22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F96" s="22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G96" s="22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H96" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I96" s="22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J96" s="22">
         <f t="shared" si="9"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K96" s="21">
         <f t="shared" si="10"/>
-        <v>100.5</v>
+        <v>93.5</v>
       </c>
       <c r="L96" s="21" t="s">
         <v>95</v>
       </c>
       <c r="M96" s="21">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="N96" s="21">
         <v>8</v>
       </c>
       <c r="O96" s="21">
-        <f>ROUND(((J96/J113)*100),1)</f>
-        <v>7.4</v>
+        <f>ROUND(((J96/J115)*100),1)</f>
+        <v>0.7</v>
       </c>
       <c r="P96" s="21">
         <f t="shared" si="11"/>
-        <v>73.900000000000006</v>
+        <v>65.899999999999991</v>
       </c>
       <c r="Q96" s="21"/>
       <c r="R96" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S96" s="21"/>
     </row>
-    <row r="97" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="60"/>
-      <c r="B97" s="57"/>
+    <row r="97" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="85"/>
+      <c r="B97" s="35"/>
       <c r="C97" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D97" s="22">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E97" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F97" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G97" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H97" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I97" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J97" s="22">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K97" s="21">
         <f t="shared" si="10"/>
-        <v>101.5</v>
+        <v>103.5</v>
       </c>
       <c r="L97" s="21" t="s">
         <v>95</v>
       </c>
       <c r="M97" s="21">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="N97" s="21">
         <v>8</v>
       </c>
       <c r="O97" s="21">
-        <f>ROUND(((J97/J113)*100),1)</f>
-        <v>0.7</v>
+        <f>ROUND(((J97/J115)*100),1)</f>
+        <v>6.9</v>
       </c>
       <c r="P97" s="21">
         <f t="shared" si="11"/>
-        <v>74.600000000000009</v>
+        <v>72.8</v>
       </c>
       <c r="Q97" s="21"/>
       <c r="R97" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S97" s="21"/>
     </row>
     <row r="98" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="60"/>
-      <c r="B98" s="57"/>
+      <c r="A98" s="85"/>
+      <c r="B98" s="35"/>
       <c r="C98" s="19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D98" s="22">
         <v>1</v>
       </c>
       <c r="E98" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F98" s="22">
         <v>0</v>
       </c>
       <c r="G98" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H98" s="22">
         <v>0</v>
@@ -6925,7 +6942,7 @@
       </c>
       <c r="K98" s="21">
         <f t="shared" si="10"/>
-        <v>102.5</v>
+        <v>104.5</v>
       </c>
       <c r="L98" s="21" t="s">
         <v>95</v>
@@ -6937,31 +6954,31 @@
         <v>8</v>
       </c>
       <c r="O98" s="21">
-        <f>ROUND(((J98/J113)*100),1)</f>
+        <f>ROUND(((J98/J115)*100),1)</f>
         <v>0.7</v>
       </c>
       <c r="P98" s="21">
         <f t="shared" si="11"/>
-        <v>75.300000000000011</v>
+        <v>73.5</v>
       </c>
       <c r="Q98" s="21"/>
       <c r="R98" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S98" s="21"/>
     </row>
     <row r="99" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="60"/>
-      <c r="B99" s="57"/>
+      <c r="A99" s="85"/>
+      <c r="B99" s="35"/>
       <c r="C99" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D99" s="22">
         <v>1</v>
       </c>
       <c r="E99" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F99" s="22">
         <v>0</v>
@@ -6973,7 +6990,7 @@
         <v>0</v>
       </c>
       <c r="I99" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J99" s="22">
         <f t="shared" si="9"/>
@@ -6981,7 +6998,7 @@
       </c>
       <c r="K99" s="21">
         <f t="shared" si="10"/>
-        <v>103.5</v>
+        <v>105.5</v>
       </c>
       <c r="L99" s="21" t="s">
         <v>95</v>
@@ -6993,91 +7010,89 @@
         <v>8</v>
       </c>
       <c r="O99" s="21">
-        <f>ROUND(((J99/J113)*100),1)</f>
+        <f>ROUND(((J99/J115)*100),1)</f>
         <v>0.7</v>
       </c>
       <c r="P99" s="21">
         <f t="shared" si="11"/>
-        <v>76.000000000000014</v>
+        <v>74.2</v>
       </c>
       <c r="Q99" s="21"/>
       <c r="R99" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S99" s="21"/>
     </row>
     <row r="100" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="B100" s="56"/>
+      <c r="A100" s="85"/>
+      <c r="B100" s="35"/>
       <c r="C100" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="D100" s="12">
-        <v>1</v>
-      </c>
-      <c r="E100" s="12">
-        <v>0</v>
-      </c>
-      <c r="F100" s="12">
-        <v>0</v>
-      </c>
-      <c r="G100" s="12">
-        <v>0</v>
-      </c>
-      <c r="H100" s="12">
-        <v>2</v>
-      </c>
-      <c r="I100" s="12">
-        <v>0</v>
-      </c>
-      <c r="J100" s="12">
+        <v>97</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1</v>
+      </c>
+      <c r="E100" s="22">
+        <v>0</v>
+      </c>
+      <c r="F100" s="22">
+        <v>0</v>
+      </c>
+      <c r="G100" s="22">
+        <v>0</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>1</v>
+      </c>
+      <c r="J100" s="22">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K100" s="21">
         <f t="shared" si="10"/>
-        <v>105.5</v>
+        <v>106.5</v>
       </c>
       <c r="L100" s="21" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="M100" s="21">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N100" s="21">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O100" s="21">
-        <f>ROUND(((J100/J113)*100),1)</f>
-        <v>1.5</v>
+        <f>ROUND(((J100/J115)*100),1)</f>
+        <v>0.7</v>
       </c>
       <c r="P100" s="21">
         <f t="shared" si="11"/>
-        <v>77.500000000000014</v>
-      </c>
-      <c r="Q100" s="21">
-        <v>0</v>
-      </c>
+        <v>74.900000000000006</v>
+      </c>
+      <c r="Q100" s="21"/>
       <c r="R100" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S100" s="21"/>
     </row>
     <row r="101" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="65"/>
-      <c r="B101" s="56"/>
+      <c r="A101" s="87" t="s">
+        <v>106</v>
+      </c>
+      <c r="B101" s="34"/>
       <c r="C101" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D101" s="12">
         <v>1</v>
       </c>
       <c r="E101" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F101" s="12">
         <v>0</v>
@@ -7086,54 +7101,56 @@
         <v>0</v>
       </c>
       <c r="H101" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I101" s="12">
         <v>0</v>
       </c>
       <c r="J101" s="12">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K101" s="21">
         <f t="shared" si="10"/>
-        <v>106.5</v>
+        <v>108.5</v>
       </c>
       <c r="L101" s="21" t="s">
-        <v>95</v>
+        <v>33</v>
       </c>
       <c r="M101" s="21">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N101" s="21">
         <v>9</v>
       </c>
       <c r="O101" s="21">
-        <f>ROUND(((J101/J113)*100),1)</f>
-        <v>0.7</v>
+        <f>ROUND(((J101/J115)*100),1)</f>
+        <v>1.4</v>
       </c>
       <c r="P101" s="21">
         <f t="shared" si="11"/>
-        <v>78.200000000000017</v>
-      </c>
-      <c r="Q101" s="21"/>
+        <v>76.300000000000011</v>
+      </c>
+      <c r="Q101" s="21">
+        <v>0</v>
+      </c>
       <c r="R101" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S101" s="21"/>
     </row>
     <row r="102" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="66"/>
-      <c r="B102" s="56"/>
+      <c r="A102" s="88"/>
+      <c r="B102" s="34"/>
       <c r="C102" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D102" s="12">
         <v>1</v>
       </c>
       <c r="E102" s="12">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="F102" s="12">
         <v>0</v>
@@ -7149,67 +7166,67 @@
       </c>
       <c r="J102" s="12">
         <f t="shared" si="9"/>
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="K102" s="21">
         <f t="shared" si="10"/>
-        <v>108</v>
+        <v>109.5</v>
       </c>
       <c r="L102" s="21" t="s">
         <v>95</v>
       </c>
       <c r="M102" s="21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N102" s="21">
         <v>9</v>
       </c>
       <c r="O102" s="21">
-        <f>ROUND(((J102/J113)*100),1)</f>
-        <v>1.1000000000000001</v>
+        <f>ROUND(((J102/J115)*100),1)</f>
+        <v>0.7</v>
       </c>
       <c r="P102" s="21">
         <f t="shared" si="11"/>
-        <v>79.300000000000011</v>
+        <v>77.000000000000014</v>
       </c>
       <c r="Q102" s="21"/>
       <c r="R102" s="21">
         <f t="shared" si="8"/>
+        <v>1.9</v>
+      </c>
+      <c r="S102" s="21"/>
+    </row>
+    <row r="103" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="89"/>
+      <c r="B103" s="34"/>
+      <c r="C103" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D103" s="12">
+        <v>1</v>
+      </c>
+      <c r="E103" s="12">
         <v>1.5</v>
       </c>
-      <c r="S102" s="21"/>
-    </row>
-    <row r="103" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="66"/>
-      <c r="B103" s="56"/>
-      <c r="C103" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="D103" s="12">
-        <v>5</v>
-      </c>
-      <c r="E103" s="12">
-        <v>0.5</v>
-      </c>
       <c r="F103" s="12">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G103" s="12">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H103" s="12">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I103" s="12">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J103" s="12">
         <f t="shared" si="9"/>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="K103" s="21">
         <f t="shared" si="10"/>
-        <v>110.5</v>
+        <v>111</v>
       </c>
       <c r="L103" s="21" t="s">
         <v>95</v>
@@ -7221,25 +7238,25 @@
         <v>9</v>
       </c>
       <c r="O103" s="21">
-        <f>ROUND(((J103/J113)*100),1)</f>
-        <v>1.9</v>
+        <f>ROUND(((J103/J115)*100),1)</f>
+        <v>1</v>
       </c>
       <c r="P103" s="21">
         <f t="shared" si="11"/>
-        <v>81.200000000000017</v>
+        <v>78.000000000000014</v>
       </c>
       <c r="Q103" s="21"/>
       <c r="R103" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S103" s="21"/>
     </row>
     <row r="104" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="66"/>
-      <c r="B104" s="73"/>
-      <c r="C104" s="70" t="s">
-        <v>111</v>
+      <c r="A104" s="89"/>
+      <c r="B104" s="34"/>
+      <c r="C104" s="19" t="s">
+        <v>110</v>
       </c>
       <c r="D104" s="12">
         <v>5</v>
@@ -7265,102 +7282,102 @@
       </c>
       <c r="K104" s="21">
         <f t="shared" si="10"/>
-        <v>113</v>
+        <v>113.5</v>
       </c>
       <c r="L104" s="21" t="s">
         <v>95</v>
       </c>
       <c r="M104" s="21">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N104" s="21">
         <v>9</v>
       </c>
       <c r="O104" s="21">
-        <f>ROUND(((J104/J113)*100),1)</f>
-        <v>1.9</v>
+        <f>ROUND(((J104/J115)*100),1)</f>
+        <v>1.7</v>
       </c>
       <c r="P104" s="21">
         <f t="shared" si="11"/>
-        <v>83.100000000000023</v>
+        <v>79.700000000000017</v>
       </c>
       <c r="Q104" s="21"/>
       <c r="R104" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S104" s="21"/>
     </row>
     <row r="105" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="67"/>
-      <c r="B105" s="74"/>
-      <c r="C105" s="71" t="s">
-        <v>112</v>
-      </c>
-      <c r="D105" s="2">
-        <v>1</v>
+      <c r="A105" s="89"/>
+      <c r="B105" s="41"/>
+      <c r="C105" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="D105" s="12">
+        <v>5</v>
       </c>
       <c r="E105" s="12">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F105" s="12">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="G105" s="12">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H105" s="12">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I105" s="12">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J105" s="12">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="K105" s="21">
         <f t="shared" si="10"/>
-        <v>115</v>
-      </c>
-      <c r="L105" s="81" t="s">
+        <v>116</v>
+      </c>
+      <c r="L105" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="M105" s="81">
-        <v>4</v>
-      </c>
-      <c r="N105" s="81">
+      <c r="M105" s="21">
+        <v>5</v>
+      </c>
+      <c r="N105" s="21">
         <v>9</v>
       </c>
-      <c r="O105" s="77">
-        <f>ROUND(((J105/J113)*100),1)</f>
-        <v>1.5</v>
+      <c r="O105" s="21">
+        <f>ROUND(((J105/J115)*100),1)</f>
+        <v>1.7</v>
       </c>
       <c r="P105" s="21">
         <f t="shared" si="11"/>
-        <v>84.600000000000023</v>
+        <v>81.40000000000002</v>
       </c>
       <c r="Q105" s="21"/>
       <c r="R105" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S105" s="21"/>
     </row>
     <row r="106" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="67"/>
-      <c r="B106" s="74"/>
-      <c r="C106" s="71" t="s">
-        <v>113</v>
-      </c>
-      <c r="D106" s="23">
+      <c r="A106" s="90"/>
+      <c r="B106" s="42"/>
+      <c r="C106" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="D106" s="2">
         <v>1</v>
       </c>
       <c r="E106" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F106" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G106" s="12">
         <v>0</v>
@@ -7373,266 +7390,266 @@
       </c>
       <c r="J106" s="12">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K106" s="21">
         <f t="shared" si="10"/>
-        <v>116</v>
-      </c>
-      <c r="L106" s="82"/>
-      <c r="M106" s="82"/>
-      <c r="N106" s="82"/>
-      <c r="O106" s="77">
-        <f>ROUND(((J106/J113)*100),1)</f>
-        <v>0.7</v>
+        <v>118</v>
+      </c>
+      <c r="L106" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="M106" s="49">
+        <v>4</v>
+      </c>
+      <c r="N106" s="49">
+        <v>9</v>
+      </c>
+      <c r="O106" s="45">
+        <f>ROUND(((J106/J115)*100),1)</f>
+        <v>1.4</v>
       </c>
       <c r="P106" s="21">
         <f t="shared" si="11"/>
-        <v>85.300000000000026</v>
+        <v>82.800000000000026</v>
       </c>
       <c r="Q106" s="21"/>
       <c r="R106" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S106" s="21"/>
     </row>
     <row r="107" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="66"/>
-      <c r="B107" s="75"/>
-      <c r="C107" s="70" t="s">
-        <v>75</v>
-      </c>
-      <c r="D107" s="88">
-        <v>5</v>
-      </c>
-      <c r="E107" s="89">
+      <c r="A107" s="90"/>
+      <c r="B107" s="42"/>
+      <c r="C107" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="D107" s="23">
+        <v>1</v>
+      </c>
+      <c r="E107" s="12">
         <v>1</v>
       </c>
       <c r="F107" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G107" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H107" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I107" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J107" s="12">
         <f t="shared" si="9"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K107" s="21">
         <f t="shared" si="10"/>
-        <v>121</v>
-      </c>
-      <c r="L107" s="59" t="s">
-        <v>33</v>
-      </c>
-      <c r="M107" s="59">
-        <v>5</v>
-      </c>
-      <c r="N107" s="59">
-        <v>9</v>
-      </c>
-      <c r="O107" s="77">
-        <f>ROUND(((J107/J113)*100),1)</f>
-        <v>3.7</v>
+        <v>119</v>
+      </c>
+      <c r="L107" s="50"/>
+      <c r="M107" s="50"/>
+      <c r="N107" s="50"/>
+      <c r="O107" s="45">
+        <f>ROUND(((J107/J115)*100),1)</f>
+        <v>0.7</v>
       </c>
       <c r="P107" s="21">
         <f t="shared" si="11"/>
-        <v>89.000000000000028</v>
-      </c>
-      <c r="Q107" s="21">
-        <v>0</v>
-      </c>
+        <v>83.500000000000028</v>
+      </c>
+      <c r="Q107" s="21"/>
       <c r="R107" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S107" s="21"/>
     </row>
     <row r="108" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="66"/>
-      <c r="B108" s="76"/>
-      <c r="C108" s="87" t="s">
-        <v>114</v>
-      </c>
-      <c r="D108" s="91">
-        <v>1</v>
-      </c>
-      <c r="E108" s="92">
-        <v>0</v>
+      <c r="A108" s="89"/>
+      <c r="B108" s="43"/>
+      <c r="C108" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="D108" s="56">
+        <v>5</v>
+      </c>
+      <c r="E108" s="57">
+        <v>1</v>
       </c>
       <c r="F108" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G108" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H108" s="12">
         <v>1</v>
       </c>
       <c r="I108" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J108" s="12">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K108" s="21">
         <f t="shared" si="10"/>
-        <v>122</v>
-      </c>
-      <c r="L108" s="83" t="s">
-        <v>95</v>
-      </c>
-      <c r="M108" s="84">
-        <v>2</v>
-      </c>
-      <c r="N108" s="84">
+        <v>124</v>
+      </c>
+      <c r="L108" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="M108" s="36">
+        <v>5</v>
+      </c>
+      <c r="N108" s="36">
         <v>9</v>
       </c>
-      <c r="O108" s="78">
-        <f>ROUND(((J108/J113)*100),1)</f>
-        <v>0.7</v>
+      <c r="O108" s="45">
+        <f>ROUND(((J108/J115)*100),1)</f>
+        <v>3.4</v>
       </c>
       <c r="P108" s="21">
         <f t="shared" si="11"/>
-        <v>89.700000000000031</v>
-      </c>
-      <c r="Q108" s="21"/>
+        <v>86.900000000000034</v>
+      </c>
+      <c r="Q108" s="21">
+        <v>0</v>
+      </c>
       <c r="R108" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S108" s="21"/>
     </row>
-    <row r="109" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="68"/>
-      <c r="B109" s="76"/>
-      <c r="C109" s="87" t="s">
-        <v>93</v>
-      </c>
-      <c r="D109" s="91">
-        <v>5</v>
-      </c>
-      <c r="E109" s="92">
-        <v>2</v>
+    <row r="109" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="89"/>
+      <c r="B109" s="44"/>
+      <c r="C109" s="55" t="s">
+        <v>114</v>
+      </c>
+      <c r="D109" s="59">
+        <v>1</v>
+      </c>
+      <c r="E109" s="60">
+        <v>0</v>
       </c>
       <c r="F109" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G109" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H109" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I109" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J109" s="12">
         <f t="shared" si="9"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K109" s="21">
         <f t="shared" si="10"/>
-        <v>132</v>
-      </c>
-      <c r="L109" s="85" t="s">
+        <v>125</v>
+      </c>
+      <c r="L109" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="M109" s="86">
-        <v>20</v>
-      </c>
-      <c r="N109" s="84">
+      <c r="M109" s="52">
+        <v>2</v>
+      </c>
+      <c r="N109" s="52">
         <v>9</v>
       </c>
-      <c r="O109" s="78">
-        <f>ROUND(((J109/J113)*100),1)</f>
-        <v>7.4</v>
+      <c r="O109" s="46">
+        <f>ROUND(((J109/J115)*100),1)</f>
+        <v>0.7</v>
       </c>
       <c r="P109" s="21">
         <f t="shared" si="11"/>
-        <v>97.100000000000037</v>
+        <v>87.600000000000037</v>
       </c>
       <c r="Q109" s="21"/>
       <c r="R109" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S109" s="21"/>
     </row>
-    <row r="110" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="68"/>
-      <c r="B110" s="76"/>
-      <c r="C110" s="87" t="s">
-        <v>94</v>
-      </c>
-      <c r="D110" s="93">
-        <v>1</v>
-      </c>
-      <c r="E110" s="94">
-        <v>0</v>
+    <row r="110" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="91"/>
+      <c r="B110" s="44"/>
+      <c r="C110" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D110" s="59">
+        <v>5</v>
+      </c>
+      <c r="E110" s="60">
+        <v>2</v>
       </c>
       <c r="F110" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G110" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H110" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I110" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J110" s="12">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K110" s="21">
         <f t="shared" si="10"/>
-        <v>133</v>
-      </c>
-      <c r="L110" s="85" t="s">
+        <v>135</v>
+      </c>
+      <c r="L110" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="M110" s="86">
-        <v>1</v>
-      </c>
-      <c r="N110" s="84">
+      <c r="M110" s="54">
+        <v>20</v>
+      </c>
+      <c r="N110" s="52">
         <v>9</v>
       </c>
-      <c r="O110" s="78">
-        <f>ROUND(((J110/J113)*100),1)</f>
-        <v>0.7</v>
+      <c r="O110" s="46">
+        <f>ROUND(((J110/J115)*100),1)</f>
+        <v>6.9</v>
       </c>
       <c r="P110" s="21">
         <f t="shared" si="11"/>
-        <v>97.80000000000004</v>
+        <v>94.500000000000043</v>
       </c>
       <c r="Q110" s="21"/>
       <c r="R110" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S110" s="21"/>
     </row>
     <row r="111" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="68"/>
-      <c r="B111" s="76"/>
-      <c r="C111" s="87" t="s">
-        <v>96</v>
-      </c>
-      <c r="D111" s="93">
-        <v>1</v>
-      </c>
-      <c r="E111" s="94">
+      <c r="A111" s="91"/>
+      <c r="B111" s="44"/>
+      <c r="C111" s="55" t="s">
+        <v>94</v>
+      </c>
+      <c r="D111" s="61">
+        <v>1</v>
+      </c>
+      <c r="E111" s="62">
         <v>0</v>
       </c>
       <c r="F111" s="12">
@@ -7653,55 +7670,55 @@
       </c>
       <c r="K111" s="21">
         <f t="shared" si="10"/>
-        <v>134</v>
-      </c>
-      <c r="L111" s="85" t="s">
+        <v>136</v>
+      </c>
+      <c r="L111" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="M111" s="86">
-        <v>1</v>
-      </c>
-      <c r="N111" s="84">
+      <c r="M111" s="54">
+        <v>1</v>
+      </c>
+      <c r="N111" s="52">
         <v>9</v>
       </c>
-      <c r="O111" s="78">
-        <f>ROUND(((J111/J113)*100),1)</f>
+      <c r="O111" s="46">
+        <f>ROUND(((J111/J115)*100),1)</f>
         <v>0.7</v>
       </c>
       <c r="P111" s="21">
         <f t="shared" si="11"/>
-        <v>98.500000000000043</v>
+        <v>95.200000000000045</v>
       </c>
       <c r="Q111" s="21"/>
       <c r="R111" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S111" s="21"/>
     </row>
     <row r="112" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="69"/>
-      <c r="B112" s="76"/>
-      <c r="C112" s="87" t="s">
-        <v>97</v>
-      </c>
-      <c r="D112" s="93">
-        <v>1</v>
-      </c>
-      <c r="E112" s="94">
+      <c r="A112" s="91"/>
+      <c r="B112" s="44"/>
+      <c r="C112" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="D112" s="61">
+        <v>1</v>
+      </c>
+      <c r="E112" s="62">
         <v>0</v>
       </c>
       <c r="F112" s="12">
         <v>0</v>
       </c>
       <c r="G112" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H112" s="12">
         <v>0</v>
       </c>
       <c r="I112" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J112" s="12">
         <f t="shared" si="9"/>
@@ -7709,88 +7726,226 @@
       </c>
       <c r="K112" s="21">
         <f t="shared" si="10"/>
-        <v>135</v>
-      </c>
-      <c r="L112" s="85" t="s">
+        <v>137</v>
+      </c>
+      <c r="L112" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="M112" s="86">
-        <v>1</v>
-      </c>
-      <c r="N112" s="84">
+      <c r="M112" s="54">
+        <v>1</v>
+      </c>
+      <c r="N112" s="52">
         <v>9</v>
       </c>
-      <c r="O112" s="78">
-        <f>ROUND(((J112/J113)*100),1)</f>
+      <c r="O112" s="46">
+        <f>ROUND(((J112/J115)*100),1)</f>
         <v>0.7</v>
       </c>
       <c r="P112" s="21">
         <f t="shared" si="11"/>
-        <v>99.200000000000045</v>
+        <v>95.900000000000048</v>
       </c>
       <c r="Q112" s="21"/>
       <c r="R112" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="S112" s="21"/>
     </row>
     <row r="113" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="1"/>
-      <c r="B113" s="72"/>
-      <c r="C113" s="32"/>
-      <c r="D113" s="80"/>
-      <c r="E113" s="90">
-        <f t="shared" ref="E113:J113" si="12">SUM(E60:E112)</f>
-        <v>27</v>
-      </c>
-      <c r="F113" s="29">
+      <c r="A113" s="91"/>
+      <c r="B113" s="44"/>
+      <c r="C113" s="55" t="s">
+        <v>97</v>
+      </c>
+      <c r="D113" s="61">
+        <v>1</v>
+      </c>
+      <c r="E113" s="62">
+        <v>0</v>
+      </c>
+      <c r="F113" s="62">
+        <v>0</v>
+      </c>
+      <c r="G113" s="62">
+        <v>0</v>
+      </c>
+      <c r="H113" s="62">
+        <v>0</v>
+      </c>
+      <c r="I113" s="62">
+        <v>1</v>
+      </c>
+      <c r="J113" s="62">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="K113" s="21">
+        <f t="shared" si="10"/>
+        <v>138</v>
+      </c>
+      <c r="L113" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="M113" s="54">
+        <v>1</v>
+      </c>
+      <c r="N113" s="52">
+        <v>9</v>
+      </c>
+      <c r="O113" s="46">
+        <f>ROUND(((J113/J115)*100),1)</f>
+        <v>0.7</v>
+      </c>
+      <c r="P113" s="21">
+        <f t="shared" si="11"/>
+        <v>96.600000000000051</v>
+      </c>
+      <c r="Q113" s="96"/>
+      <c r="R113" s="96"/>
+      <c r="S113" s="96"/>
+    </row>
+    <row r="114" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="92"/>
+      <c r="B114" s="44"/>
+      <c r="C114" s="97" t="s">
+        <v>116</v>
+      </c>
+      <c r="D114" s="61">
+        <v>5</v>
+      </c>
+      <c r="E114" s="62">
+        <v>1</v>
+      </c>
+      <c r="F114" s="12">
+        <v>1</v>
+      </c>
+      <c r="G114" s="12">
+        <v>1</v>
+      </c>
+      <c r="H114" s="12">
+        <v>1</v>
+      </c>
+      <c r="I114" s="12">
+        <v>1</v>
+      </c>
+      <c r="J114" s="12">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="K114" s="21">
+        <f t="shared" si="10"/>
+        <v>143</v>
+      </c>
+      <c r="L114" s="53"/>
+      <c r="M114" s="54"/>
+      <c r="N114" s="52">
+        <v>9</v>
+      </c>
+      <c r="O114" s="46">
+        <f>ROUND(((J114/J115)*100),1)</f>
+        <v>3.4</v>
+      </c>
+      <c r="P114" s="21">
+        <f t="shared" si="11"/>
+        <v>100.00000000000006</v>
+      </c>
+      <c r="Q114" s="21"/>
+      <c r="R114" s="21">
+        <f>Q114+R112</f>
+        <v>1.9</v>
+      </c>
+      <c r="S114" s="21"/>
+    </row>
+    <row r="115" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="1"/>
+      <c r="B115" s="40"/>
+      <c r="C115" s="32"/>
+      <c r="D115" s="48"/>
+      <c r="E115" s="58">
+        <f t="shared" ref="E115:J115" si="12">SUM(E60:E114)</f>
+        <v>29</v>
+      </c>
+      <c r="F115" s="29">
         <f t="shared" si="12"/>
-        <v>26</v>
-      </c>
-      <c r="G113" s="29">
+        <v>28</v>
+      </c>
+      <c r="G115" s="29">
         <f t="shared" si="12"/>
-        <v>26.5</v>
-      </c>
-      <c r="H113" s="29">
+        <v>28.5</v>
+      </c>
+      <c r="H115" s="29">
         <f t="shared" si="12"/>
-        <v>27</v>
-      </c>
-      <c r="I113" s="29">
+        <v>29</v>
+      </c>
+      <c r="I115" s="29">
         <f t="shared" si="12"/>
-        <v>27</v>
-      </c>
-      <c r="J113" s="21">
+        <v>29</v>
+      </c>
+      <c r="J115" s="21">
         <f t="shared" si="12"/>
-        <v>135</v>
-      </c>
-      <c r="K113" s="8"/>
-      <c r="L113" s="72"/>
-      <c r="M113" s="79"/>
-      <c r="N113" s="80"/>
-      <c r="O113" s="21">
-        <f>SUM(O60:O112)</f>
-        <v>99.200000000000045</v>
-      </c>
-      <c r="P113" s="3"/>
-      <c r="Q113" s="21">
-        <v>0</v>
-      </c>
-      <c r="R113" s="8"/>
-      <c r="S113" s="10"/>
+        <v>145</v>
+      </c>
+      <c r="K115" s="8"/>
+      <c r="L115" s="40"/>
+      <c r="M115" s="47"/>
+      <c r="N115" s="48"/>
+      <c r="O115" s="21">
+        <f>SUM(O60:O114)</f>
+        <v>100.00000000000006</v>
+      </c>
+      <c r="P115" s="3"/>
+      <c r="Q115" s="21">
+        <v>0</v>
+      </c>
+      <c r="R115" s="8"/>
+      <c r="S115" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="E7:K7"/>
-    <mergeCell ref="L7:P7"/>
+    <mergeCell ref="A101:A114"/>
+    <mergeCell ref="A63:A68"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="A72:A82"/>
+    <mergeCell ref="A83:A91"/>
+    <mergeCell ref="A92:A100"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="K54:K59"/>
+    <mergeCell ref="L54:L59"/>
+    <mergeCell ref="M54:M59"/>
+    <mergeCell ref="N54:N59"/>
+    <mergeCell ref="F54:F59"/>
+    <mergeCell ref="G54:G59"/>
+    <mergeCell ref="H54:H59"/>
+    <mergeCell ref="I54:I59"/>
+    <mergeCell ref="J54:J59"/>
+    <mergeCell ref="A54:A59"/>
+    <mergeCell ref="B54:B59"/>
+    <mergeCell ref="C54:C59"/>
+    <mergeCell ref="D54:D59"/>
+    <mergeCell ref="E54:E59"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A51:S51"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="E53:K53"/>
+    <mergeCell ref="L53:P53"/>
+    <mergeCell ref="Q53:S53"/>
+    <mergeCell ref="P54:P59"/>
+    <mergeCell ref="Q54:Q59"/>
+    <mergeCell ref="R54:R59"/>
+    <mergeCell ref="S54:S59"/>
+    <mergeCell ref="O54:O59"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="P8:P13"/>
+    <mergeCell ref="Q8:Q13"/>
+    <mergeCell ref="R8:R13"/>
+    <mergeCell ref="S8:S13"/>
+    <mergeCell ref="A14:A16"/>
     <mergeCell ref="Q7:S7"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="B8:B13"/>
@@ -7807,49 +7962,16 @@
     <mergeCell ref="M8:M13"/>
     <mergeCell ref="N8:N13"/>
     <mergeCell ref="O8:O13"/>
-    <mergeCell ref="P8:P13"/>
-    <mergeCell ref="Q8:Q13"/>
-    <mergeCell ref="R8:R13"/>
-    <mergeCell ref="S8:S13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="A36:A43"/>
-    <mergeCell ref="B54:B59"/>
-    <mergeCell ref="C54:C59"/>
-    <mergeCell ref="D54:D59"/>
-    <mergeCell ref="E54:E59"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A51:S51"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="E53:K53"/>
-    <mergeCell ref="L53:P53"/>
-    <mergeCell ref="Q53:S53"/>
-    <mergeCell ref="P54:P59"/>
-    <mergeCell ref="Q54:Q59"/>
-    <mergeCell ref="R54:R59"/>
-    <mergeCell ref="S54:S59"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="K54:K59"/>
-    <mergeCell ref="L54:L59"/>
-    <mergeCell ref="M54:M59"/>
-    <mergeCell ref="N54:N59"/>
-    <mergeCell ref="O54:O59"/>
-    <mergeCell ref="F54:F59"/>
-    <mergeCell ref="G54:G59"/>
-    <mergeCell ref="H54:H59"/>
-    <mergeCell ref="I54:I59"/>
-    <mergeCell ref="J54:J59"/>
-    <mergeCell ref="A54:A59"/>
-    <mergeCell ref="A100:A112"/>
-    <mergeCell ref="A63:A68"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="A72:A82"/>
-    <mergeCell ref="A83:A90"/>
-    <mergeCell ref="A91:A99"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="E7:K7"/>
+    <mergeCell ref="L7:P7"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="F4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización tiempos de tareas realizadas
</commit_message>
<xml_diff>
--- a/NoteBook/summary/TASK_TEAM.xlsx
+++ b/NoteBook/summary/TASK_TEAM.xlsx
@@ -1598,6 +1598,96 @@
     <xf numFmtId="0" fontId="33" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="10" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1613,98 +1703,8 @@
     <xf numFmtId="0" fontId="61" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="73" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="71" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="10" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1978,7 +1978,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1988,8 +1988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C95" workbookViewId="0">
-      <selection activeCell="Q68" sqref="Q68"/>
+    <sheetView tabSelected="1" topLeftCell="C55" workbookViewId="0">
+      <selection activeCell="Q113" sqref="Q113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2011,16 +2011,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
+      <c r="A1" s="93" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="30"/>
@@ -2030,51 +2030,51 @@
       <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="64"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="94"/>
       <c r="E3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="66">
+      <c r="F3" s="96">
         <v>41719</v>
       </c>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
     </row>
     <row r="4" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="68"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="92"/>
       <c r="E4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="68" t="s">
+      <c r="F4" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="92"/>
     </row>
     <row r="5" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="70"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="91"/>
       <c r="E5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="68">
-        <v>1</v>
-      </c>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
+      <c r="F5" s="92">
+        <v>1</v>
+      </c>
+      <c r="G5" s="92"/>
+      <c r="H5" s="92"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
@@ -2098,200 +2098,200 @@
       <c r="S6" s="25"/>
     </row>
     <row r="7" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="72" t="s">
+      <c r="B7" s="89"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="90"/>
+      <c r="E7" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="73"/>
-      <c r="L7" s="72" t="s">
+      <c r="F7" s="89"/>
+      <c r="G7" s="89"/>
+      <c r="H7" s="89"/>
+      <c r="I7" s="89"/>
+      <c r="J7" s="89"/>
+      <c r="K7" s="90"/>
+      <c r="L7" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="71"/>
-      <c r="N7" s="71"/>
-      <c r="O7" s="71"/>
-      <c r="P7" s="73"/>
-      <c r="Q7" s="72" t="s">
+      <c r="M7" s="89"/>
+      <c r="N7" s="89"/>
+      <c r="O7" s="89"/>
+      <c r="P7" s="90"/>
+      <c r="Q7" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="R7" s="71"/>
-      <c r="S7" s="73"/>
+      <c r="R7" s="89"/>
+      <c r="S7" s="90"/>
     </row>
     <row r="8" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="74" t="s">
+      <c r="A8" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="74" t="s">
+      <c r="B8" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="77" t="s">
+      <c r="C8" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="74" t="s">
+      <c r="D8" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="74" t="s">
+      <c r="E8" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="74" t="s">
+      <c r="F8" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="74" t="s">
+      <c r="G8" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="74" t="s">
+      <c r="H8" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="74" t="s">
+      <c r="I8" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="74" t="s">
+      <c r="J8" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="74" t="s">
+      <c r="K8" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="77" t="s">
+      <c r="L8" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="M8" s="74" t="s">
+      <c r="M8" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="N8" s="74" t="s">
+      <c r="N8" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="O8" s="74" t="s">
+      <c r="O8" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="P8" s="74" t="s">
+      <c r="P8" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="Q8" s="74" t="s">
+      <c r="Q8" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="R8" s="74" t="s">
+      <c r="R8" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="S8" s="74" t="s">
+      <c r="S8" s="76" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="75"/>
-      <c r="B9" s="75"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="78"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="75"/>
-      <c r="P9" s="75"/>
-      <c r="Q9" s="75"/>
-      <c r="R9" s="75"/>
-      <c r="S9" s="75"/>
+      <c r="A9" s="77"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="77"/>
+      <c r="E9" s="77"/>
+      <c r="F9" s="77"/>
+      <c r="G9" s="77"/>
+      <c r="H9" s="77"/>
+      <c r="I9" s="77"/>
+      <c r="J9" s="77"/>
+      <c r="K9" s="77"/>
+      <c r="L9" s="79"/>
+      <c r="M9" s="77"/>
+      <c r="N9" s="77"/>
+      <c r="O9" s="77"/>
+      <c r="P9" s="77"/>
+      <c r="Q9" s="77"/>
+      <c r="R9" s="77"/>
+      <c r="S9" s="77"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="75"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="75"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="78"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="75"/>
-      <c r="O10" s="75"/>
-      <c r="P10" s="75"/>
-      <c r="Q10" s="75"/>
-      <c r="R10" s="75"/>
-      <c r="S10" s="75"/>
+      <c r="A10" s="77"/>
+      <c r="B10" s="77"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="77"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="77"/>
+      <c r="I10" s="77"/>
+      <c r="J10" s="77"/>
+      <c r="K10" s="77"/>
+      <c r="L10" s="79"/>
+      <c r="M10" s="77"/>
+      <c r="N10" s="77"/>
+      <c r="O10" s="77"/>
+      <c r="P10" s="77"/>
+      <c r="Q10" s="77"/>
+      <c r="R10" s="77"/>
+      <c r="S10" s="77"/>
     </row>
     <row r="11" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="75"/>
-      <c r="B11" s="75"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="78"/>
-      <c r="M11" s="75"/>
-      <c r="N11" s="75"/>
-      <c r="O11" s="75"/>
-      <c r="P11" s="75"/>
-      <c r="Q11" s="75"/>
-      <c r="R11" s="75"/>
-      <c r="S11" s="75"/>
+      <c r="A11" s="77"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="79"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="77"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="77"/>
+      <c r="K11" s="77"/>
+      <c r="L11" s="79"/>
+      <c r="M11" s="77"/>
+      <c r="N11" s="77"/>
+      <c r="O11" s="77"/>
+      <c r="P11" s="77"/>
+      <c r="Q11" s="77"/>
+      <c r="R11" s="77"/>
+      <c r="S11" s="77"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="75"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="75"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="75"/>
-      <c r="K12" s="75"/>
-      <c r="L12" s="78"/>
-      <c r="M12" s="75"/>
-      <c r="N12" s="75"/>
-      <c r="O12" s="75"/>
-      <c r="P12" s="75"/>
-      <c r="Q12" s="75"/>
-      <c r="R12" s="75"/>
-      <c r="S12" s="75"/>
+      <c r="A12" s="77"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="79"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="77"/>
+      <c r="H12" s="77"/>
+      <c r="I12" s="77"/>
+      <c r="J12" s="77"/>
+      <c r="K12" s="77"/>
+      <c r="L12" s="79"/>
+      <c r="M12" s="77"/>
+      <c r="N12" s="77"/>
+      <c r="O12" s="77"/>
+      <c r="P12" s="77"/>
+      <c r="Q12" s="77"/>
+      <c r="R12" s="77"/>
+      <c r="S12" s="77"/>
     </row>
     <row r="13" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="76"/>
-      <c r="B13" s="76"/>
-      <c r="C13" s="79"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="76"/>
-      <c r="F13" s="76"/>
-      <c r="G13" s="76"/>
-      <c r="H13" s="76"/>
-      <c r="I13" s="76"/>
-      <c r="J13" s="76"/>
-      <c r="K13" s="75"/>
-      <c r="L13" s="79"/>
-      <c r="M13" s="76"/>
-      <c r="N13" s="76"/>
-      <c r="O13" s="76"/>
-      <c r="P13" s="75"/>
-      <c r="Q13" s="76"/>
-      <c r="R13" s="76"/>
-      <c r="S13" s="76"/>
+      <c r="A13" s="81"/>
+      <c r="B13" s="81"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="81"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="81"/>
+      <c r="K13" s="77"/>
+      <c r="L13" s="80"/>
+      <c r="M13" s="81"/>
+      <c r="N13" s="81"/>
+      <c r="O13" s="81"/>
+      <c r="P13" s="77"/>
+      <c r="Q13" s="81"/>
+      <c r="R13" s="81"/>
+      <c r="S13" s="81"/>
     </row>
     <row r="14" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="80" t="s">
+      <c r="A14" s="83" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="26"/>
@@ -2353,7 +2353,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="81"/>
+      <c r="A15" s="84"/>
       <c r="B15" s="26"/>
       <c r="C15" s="19" t="s">
         <v>34</v>
@@ -2413,7 +2413,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="82"/>
+      <c r="A16" s="85"/>
       <c r="B16" s="26"/>
       <c r="C16" s="19" t="s">
         <v>35</v>
@@ -2473,7 +2473,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="80" t="s">
+      <c r="A17" s="83" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="26"/>
@@ -2535,7 +2535,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="81"/>
+      <c r="A18" s="84"/>
       <c r="B18" s="26"/>
       <c r="C18" s="19" t="s">
         <v>38</v>
@@ -2595,7 +2595,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="82"/>
+      <c r="A19" s="85"/>
       <c r="B19" s="26"/>
       <c r="C19" s="19" t="s">
         <v>39</v>
@@ -2655,7 +2655,7 @@
       </c>
     </row>
     <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="80" t="s">
+      <c r="A20" s="83" t="s">
         <v>40</v>
       </c>
       <c r="B20" s="26"/>
@@ -2717,7 +2717,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="81"/>
+      <c r="A21" s="84"/>
       <c r="B21" s="26"/>
       <c r="C21" s="19" t="s">
         <v>42</v>
@@ -2777,7 +2777,7 @@
       </c>
     </row>
     <row r="22" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="81"/>
+      <c r="A22" s="84"/>
       <c r="B22" s="26"/>
       <c r="C22" s="19" t="s">
         <v>43</v>
@@ -2837,7 +2837,7 @@
       </c>
     </row>
     <row r="23" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="81"/>
+      <c r="A23" s="84"/>
       <c r="B23" s="26"/>
       <c r="C23" s="19" t="s">
         <v>44</v>
@@ -2897,7 +2897,7 @@
       </c>
     </row>
     <row r="24" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="81"/>
+      <c r="A24" s="84"/>
       <c r="B24" s="26"/>
       <c r="C24" s="19" t="s">
         <v>45</v>
@@ -2957,7 +2957,7 @@
       </c>
     </row>
     <row r="25" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="81"/>
+      <c r="A25" s="84"/>
       <c r="B25" s="26"/>
       <c r="C25" s="19" t="s">
         <v>46</v>
@@ -3017,7 +3017,7 @@
       </c>
     </row>
     <row r="26" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="82"/>
+      <c r="A26" s="85"/>
       <c r="B26" s="26"/>
       <c r="C26" s="19" t="s">
         <v>47</v>
@@ -3077,7 +3077,7 @@
       </c>
     </row>
     <row r="27" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="80" t="s">
+      <c r="A27" s="83" t="s">
         <v>48</v>
       </c>
       <c r="B27" s="26"/>
@@ -3139,7 +3139,7 @@
       </c>
     </row>
     <row r="28" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="81"/>
+      <c r="A28" s="84"/>
       <c r="B28" s="26"/>
       <c r="C28" s="19" t="s">
         <v>50</v>
@@ -3199,7 +3199,7 @@
       </c>
     </row>
     <row r="29" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="81"/>
+      <c r="A29" s="84"/>
       <c r="B29" s="26"/>
       <c r="C29" s="19" t="s">
         <v>51</v>
@@ -3259,7 +3259,7 @@
       </c>
     </row>
     <row r="30" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="81"/>
+      <c r="A30" s="84"/>
       <c r="B30" s="26"/>
       <c r="C30" s="19" t="s">
         <v>52</v>
@@ -3319,7 +3319,7 @@
       </c>
     </row>
     <row r="31" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="80" t="s">
+      <c r="A31" s="83" t="s">
         <v>53</v>
       </c>
       <c r="B31" s="26"/>
@@ -3381,7 +3381,7 @@
       </c>
     </row>
     <row r="32" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="81"/>
+      <c r="A32" s="84"/>
       <c r="B32" s="26"/>
       <c r="C32" s="19" t="s">
         <v>55</v>
@@ -3441,7 +3441,7 @@
       </c>
     </row>
     <row r="33" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="81"/>
+      <c r="A33" s="84"/>
       <c r="B33" s="26"/>
       <c r="C33" s="19" t="s">
         <v>56</v>
@@ -3501,7 +3501,7 @@
       </c>
     </row>
     <row r="34" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="81"/>
+      <c r="A34" s="84"/>
       <c r="B34" s="26"/>
       <c r="C34" s="19" t="s">
         <v>57</v>
@@ -3561,7 +3561,7 @@
       </c>
     </row>
     <row r="35" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="82"/>
+      <c r="A35" s="85"/>
       <c r="B35" s="26"/>
       <c r="C35" s="19" t="s">
         <v>58</v>
@@ -3621,7 +3621,7 @@
       </c>
     </row>
     <row r="36" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="80" t="s">
+      <c r="A36" s="83" t="s">
         <v>59</v>
       </c>
       <c r="B36" s="26"/>
@@ -3683,7 +3683,7 @@
       </c>
     </row>
     <row r="37" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="81"/>
+      <c r="A37" s="84"/>
       <c r="B37" s="26"/>
       <c r="C37" s="19" t="s">
         <v>61</v>
@@ -3743,7 +3743,7 @@
       </c>
     </row>
     <row r="38" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="81"/>
+      <c r="A38" s="84"/>
       <c r="B38" s="26"/>
       <c r="C38" s="19" t="s">
         <v>62</v>
@@ -3799,7 +3799,7 @@
       </c>
     </row>
     <row r="39" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="81"/>
+      <c r="A39" s="84"/>
       <c r="B39" s="26"/>
       <c r="C39" s="19" t="s">
         <v>63</v>
@@ -3857,7 +3857,7 @@
       </c>
     </row>
     <row r="40" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="81"/>
+      <c r="A40" s="84"/>
       <c r="B40" s="26"/>
       <c r="C40" s="19" t="s">
         <v>64</v>
@@ -3917,7 +3917,7 @@
       </c>
     </row>
     <row r="41" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="81"/>
+      <c r="A41" s="84"/>
       <c r="B41" s="26"/>
       <c r="C41" s="19" t="s">
         <v>65</v>
@@ -3977,7 +3977,7 @@
       </c>
     </row>
     <row r="42" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="81"/>
+      <c r="A42" s="84"/>
       <c r="B42" s="26"/>
       <c r="C42" s="19" t="s">
         <v>67</v>
@@ -4033,7 +4033,7 @@
       </c>
     </row>
     <row r="43" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="82"/>
+      <c r="A43" s="85"/>
       <c r="B43" s="26"/>
       <c r="C43" s="19" t="s">
         <v>68</v>
@@ -4093,7 +4093,7 @@
       </c>
     </row>
     <row r="44" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="80" t="s">
+      <c r="A44" s="83" t="s">
         <v>69</v>
       </c>
       <c r="B44" s="26"/>
@@ -4155,7 +4155,7 @@
       </c>
     </row>
     <row r="45" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="81"/>
+      <c r="A45" s="84"/>
       <c r="B45" s="26"/>
       <c r="C45" s="19" t="s">
         <v>71</v>
@@ -4211,7 +4211,7 @@
       </c>
     </row>
     <row r="46" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="82"/>
+      <c r="A46" s="85"/>
       <c r="B46" s="26"/>
       <c r="C46" s="19" t="s">
         <v>72</v>
@@ -4271,7 +4271,7 @@
       </c>
     </row>
     <row r="47" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="80" t="s">
+      <c r="A47" s="83" t="s">
         <v>73</v>
       </c>
       <c r="B47" s="26"/>
@@ -4333,7 +4333,7 @@
       </c>
     </row>
     <row r="48" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="82"/>
+      <c r="A48" s="85"/>
       <c r="B48" s="26"/>
       <c r="C48" s="19" t="s">
         <v>75</v>
@@ -4459,27 +4459,27 @@
       <c r="S50" s="9"/>
     </row>
     <row r="51" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="83" t="s">
+      <c r="A51" s="86" t="s">
         <v>76</v>
       </c>
-      <c r="B51" s="84"/>
-      <c r="C51" s="83"/>
-      <c r="D51" s="84"/>
-      <c r="E51" s="84"/>
-      <c r="F51" s="84"/>
-      <c r="G51" s="84"/>
-      <c r="H51" s="84"/>
-      <c r="I51" s="84"/>
-      <c r="J51" s="84"/>
-      <c r="K51" s="84"/>
-      <c r="L51" s="84"/>
-      <c r="M51" s="84"/>
-      <c r="N51" s="84"/>
-      <c r="O51" s="84"/>
-      <c r="P51" s="84"/>
-      <c r="Q51" s="84"/>
-      <c r="R51" s="84"/>
-      <c r="S51" s="84"/>
+      <c r="B51" s="87"/>
+      <c r="C51" s="86"/>
+      <c r="D51" s="87"/>
+      <c r="E51" s="87"/>
+      <c r="F51" s="87"/>
+      <c r="G51" s="87"/>
+      <c r="H51" s="87"/>
+      <c r="I51" s="87"/>
+      <c r="J51" s="87"/>
+      <c r="K51" s="87"/>
+      <c r="L51" s="87"/>
+      <c r="M51" s="87"/>
+      <c r="N51" s="87"/>
+      <c r="O51" s="87"/>
+      <c r="P51" s="87"/>
+      <c r="Q51" s="87"/>
+      <c r="R51" s="87"/>
+      <c r="S51" s="87"/>
     </row>
     <row r="52" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="27"/>
@@ -4503,197 +4503,197 @@
       <c r="S52" s="25"/>
     </row>
     <row r="53" spans="1:19" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="72" t="s">
+      <c r="A53" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="B53" s="71"/>
-      <c r="C53" s="71"/>
-      <c r="D53" s="73"/>
-      <c r="E53" s="72" t="s">
+      <c r="B53" s="89"/>
+      <c r="C53" s="89"/>
+      <c r="D53" s="90"/>
+      <c r="E53" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="F53" s="71"/>
-      <c r="G53" s="71"/>
-      <c r="H53" s="71"/>
-      <c r="I53" s="71"/>
-      <c r="J53" s="71"/>
-      <c r="K53" s="73"/>
-      <c r="L53" s="72" t="s">
+      <c r="F53" s="89"/>
+      <c r="G53" s="89"/>
+      <c r="H53" s="89"/>
+      <c r="I53" s="89"/>
+      <c r="J53" s="89"/>
+      <c r="K53" s="90"/>
+      <c r="L53" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="M53" s="71"/>
-      <c r="N53" s="71"/>
-      <c r="O53" s="71"/>
-      <c r="P53" s="73"/>
-      <c r="Q53" s="72" t="s">
+      <c r="M53" s="89"/>
+      <c r="N53" s="89"/>
+      <c r="O53" s="89"/>
+      <c r="P53" s="90"/>
+      <c r="Q53" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="R53" s="71"/>
-      <c r="S53" s="73"/>
+      <c r="R53" s="89"/>
+      <c r="S53" s="90"/>
     </row>
     <row r="54" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="74" t="s">
+      <c r="A54" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="B54" s="74" t="s">
+      <c r="B54" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="C54" s="77" t="s">
+      <c r="C54" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="D54" s="74" t="s">
+      <c r="D54" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="E54" s="74" t="s">
+      <c r="E54" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="F54" s="74" t="s">
+      <c r="F54" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="G54" s="74" t="s">
+      <c r="G54" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="H54" s="74" t="s">
+      <c r="H54" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="I54" s="74" t="s">
+      <c r="I54" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="J54" s="74" t="s">
+      <c r="J54" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="K54" s="74" t="s">
+      <c r="K54" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="L54" s="77" t="s">
+      <c r="L54" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="M54" s="74" t="s">
+      <c r="M54" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="N54" s="74" t="s">
+      <c r="N54" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="O54" s="74" t="s">
+      <c r="O54" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="P54" s="74" t="s">
+      <c r="P54" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="Q54" s="74" t="s">
+      <c r="Q54" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="R54" s="74" t="s">
+      <c r="R54" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="S54" s="74" t="s">
+      <c r="S54" s="76" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="55" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="75"/>
-      <c r="B55" s="75"/>
-      <c r="C55" s="78"/>
-      <c r="D55" s="75"/>
-      <c r="E55" s="75"/>
-      <c r="F55" s="75"/>
-      <c r="G55" s="75"/>
-      <c r="H55" s="75"/>
-      <c r="I55" s="75"/>
-      <c r="J55" s="75"/>
-      <c r="K55" s="75"/>
-      <c r="L55" s="78"/>
-      <c r="M55" s="75"/>
-      <c r="N55" s="75"/>
-      <c r="O55" s="75"/>
-      <c r="P55" s="75"/>
-      <c r="Q55" s="75"/>
-      <c r="R55" s="75"/>
-      <c r="S55" s="75"/>
+      <c r="A55" s="77"/>
+      <c r="B55" s="77"/>
+      <c r="C55" s="79"/>
+      <c r="D55" s="77"/>
+      <c r="E55" s="77"/>
+      <c r="F55" s="77"/>
+      <c r="G55" s="77"/>
+      <c r="H55" s="77"/>
+      <c r="I55" s="77"/>
+      <c r="J55" s="77"/>
+      <c r="K55" s="77"/>
+      <c r="L55" s="79"/>
+      <c r="M55" s="77"/>
+      <c r="N55" s="77"/>
+      <c r="O55" s="77"/>
+      <c r="P55" s="77"/>
+      <c r="Q55" s="77"/>
+      <c r="R55" s="77"/>
+      <c r="S55" s="77"/>
     </row>
     <row r="56" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="75"/>
-      <c r="B56" s="75"/>
-      <c r="C56" s="78"/>
-      <c r="D56" s="75"/>
-      <c r="E56" s="75"/>
-      <c r="F56" s="75"/>
-      <c r="G56" s="75"/>
-      <c r="H56" s="75"/>
-      <c r="I56" s="75"/>
-      <c r="J56" s="75"/>
-      <c r="K56" s="75"/>
-      <c r="L56" s="78"/>
-      <c r="M56" s="75"/>
-      <c r="N56" s="75"/>
-      <c r="O56" s="75"/>
-      <c r="P56" s="75"/>
-      <c r="Q56" s="75"/>
-      <c r="R56" s="75"/>
-      <c r="S56" s="75"/>
+      <c r="A56" s="77"/>
+      <c r="B56" s="77"/>
+      <c r="C56" s="79"/>
+      <c r="D56" s="77"/>
+      <c r="E56" s="77"/>
+      <c r="F56" s="77"/>
+      <c r="G56" s="77"/>
+      <c r="H56" s="77"/>
+      <c r="I56" s="77"/>
+      <c r="J56" s="77"/>
+      <c r="K56" s="77"/>
+      <c r="L56" s="79"/>
+      <c r="M56" s="77"/>
+      <c r="N56" s="77"/>
+      <c r="O56" s="77"/>
+      <c r="P56" s="77"/>
+      <c r="Q56" s="77"/>
+      <c r="R56" s="77"/>
+      <c r="S56" s="77"/>
     </row>
     <row r="57" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A57" s="75"/>
-      <c r="B57" s="75"/>
-      <c r="C57" s="78"/>
-      <c r="D57" s="75"/>
-      <c r="E57" s="75"/>
-      <c r="F57" s="75"/>
-      <c r="G57" s="75"/>
-      <c r="H57" s="75"/>
-      <c r="I57" s="75"/>
-      <c r="J57" s="75"/>
-      <c r="K57" s="75"/>
-      <c r="L57" s="78"/>
-      <c r="M57" s="75"/>
-      <c r="N57" s="75"/>
-      <c r="O57" s="75"/>
-      <c r="P57" s="75"/>
-      <c r="Q57" s="75"/>
-      <c r="R57" s="75"/>
-      <c r="S57" s="75"/>
+      <c r="A57" s="77"/>
+      <c r="B57" s="77"/>
+      <c r="C57" s="79"/>
+      <c r="D57" s="77"/>
+      <c r="E57" s="77"/>
+      <c r="F57" s="77"/>
+      <c r="G57" s="77"/>
+      <c r="H57" s="77"/>
+      <c r="I57" s="77"/>
+      <c r="J57" s="77"/>
+      <c r="K57" s="77"/>
+      <c r="L57" s="79"/>
+      <c r="M57" s="77"/>
+      <c r="N57" s="77"/>
+      <c r="O57" s="77"/>
+      <c r="P57" s="77"/>
+      <c r="Q57" s="77"/>
+      <c r="R57" s="77"/>
+      <c r="S57" s="77"/>
     </row>
     <row r="58" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A58" s="75"/>
-      <c r="B58" s="75"/>
-      <c r="C58" s="78"/>
-      <c r="D58" s="75"/>
-      <c r="E58" s="75"/>
-      <c r="F58" s="75"/>
-      <c r="G58" s="75"/>
-      <c r="H58" s="75"/>
-      <c r="I58" s="75"/>
-      <c r="J58" s="75"/>
-      <c r="K58" s="75"/>
-      <c r="L58" s="78"/>
-      <c r="M58" s="75"/>
-      <c r="N58" s="75"/>
-      <c r="O58" s="75"/>
-      <c r="P58" s="75"/>
-      <c r="Q58" s="75"/>
-      <c r="R58" s="75"/>
-      <c r="S58" s="75"/>
+      <c r="A58" s="77"/>
+      <c r="B58" s="77"/>
+      <c r="C58" s="79"/>
+      <c r="D58" s="77"/>
+      <c r="E58" s="77"/>
+      <c r="F58" s="77"/>
+      <c r="G58" s="77"/>
+      <c r="H58" s="77"/>
+      <c r="I58" s="77"/>
+      <c r="J58" s="77"/>
+      <c r="K58" s="77"/>
+      <c r="L58" s="79"/>
+      <c r="M58" s="77"/>
+      <c r="N58" s="77"/>
+      <c r="O58" s="77"/>
+      <c r="P58" s="77"/>
+      <c r="Q58" s="77"/>
+      <c r="R58" s="77"/>
+      <c r="S58" s="77"/>
     </row>
     <row r="59" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="86"/>
-      <c r="B59" s="76"/>
-      <c r="C59" s="79"/>
-      <c r="D59" s="76"/>
-      <c r="E59" s="76"/>
-      <c r="F59" s="76"/>
-      <c r="G59" s="76"/>
-      <c r="H59" s="76"/>
-      <c r="I59" s="76"/>
-      <c r="J59" s="76"/>
-      <c r="K59" s="75"/>
-      <c r="L59" s="79"/>
-      <c r="M59" s="76"/>
-      <c r="N59" s="76"/>
-      <c r="O59" s="76"/>
-      <c r="P59" s="75"/>
-      <c r="Q59" s="76"/>
-      <c r="R59" s="76"/>
-      <c r="S59" s="76"/>
+      <c r="A59" s="82"/>
+      <c r="B59" s="81"/>
+      <c r="C59" s="80"/>
+      <c r="D59" s="81"/>
+      <c r="E59" s="81"/>
+      <c r="F59" s="81"/>
+      <c r="G59" s="81"/>
+      <c r="H59" s="81"/>
+      <c r="I59" s="81"/>
+      <c r="J59" s="81"/>
+      <c r="K59" s="77"/>
+      <c r="L59" s="80"/>
+      <c r="M59" s="81"/>
+      <c r="N59" s="81"/>
+      <c r="O59" s="81"/>
+      <c r="P59" s="77"/>
+      <c r="Q59" s="81"/>
+      <c r="R59" s="81"/>
+      <c r="S59" s="81"/>
     </row>
     <row r="60" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="36" t="s">
@@ -4745,9 +4745,7 @@
         <f>O60</f>
         <v>1</v>
       </c>
-      <c r="Q60" s="21">
-        <v>0</v>
-      </c>
+      <c r="Q60" s="21"/>
       <c r="R60" s="21">
         <v>0</v>
       </c>
@@ -4756,7 +4754,7 @@
       </c>
     </row>
     <row r="61" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="85" t="s">
+      <c r="A61" s="72" t="s">
         <v>80</v>
       </c>
       <c r="B61" s="35"/>
@@ -4807,18 +4805,18 @@
         <v>2</v>
       </c>
       <c r="Q61" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R61" s="21">
         <f>Q61+R60</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S61" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="85"/>
+      <c r="A62" s="72"/>
       <c r="B62" s="35"/>
       <c r="C62" s="19" t="s">
         <v>38</v>
@@ -4867,18 +4865,18 @@
         <v>2.7</v>
       </c>
       <c r="Q62" s="21">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R62" s="21">
         <f t="shared" ref="R62:R112" si="8">Q62+R61</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="S62" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="85" t="s">
+      <c r="A63" s="72" t="s">
         <v>82</v>
       </c>
       <c r="B63" s="35"/>
@@ -4929,18 +4927,18 @@
         <v>3.4000000000000004</v>
       </c>
       <c r="Q63" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R63" s="21">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="S63" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="85"/>
+      <c r="A64" s="72"/>
       <c r="B64" s="35"/>
       <c r="C64" s="19" t="s">
         <v>44</v>
@@ -4955,7 +4953,7 @@
         <v>0.5</v>
       </c>
       <c r="G64" s="31">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H64" s="31">
         <v>0.5</v>
@@ -4965,11 +4963,11 @@
       </c>
       <c r="J64" s="31">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="K64" s="21">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v>7.5</v>
       </c>
       <c r="L64" s="21" t="s">
         <v>33</v>
@@ -4982,25 +4980,25 @@
       </c>
       <c r="O64" s="21">
         <f>ROUND(((J64/J115)*100),1)</f>
-        <v>2.1</v>
+        <v>1.7</v>
       </c>
       <c r="P64" s="21">
         <f t="shared" si="7"/>
-        <v>5.5</v>
+        <v>5.1000000000000005</v>
       </c>
       <c r="Q64" s="21">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R64" s="21">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="S64" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="85"/>
+      <c r="A65" s="72"/>
       <c r="B65" s="35"/>
       <c r="C65" s="33" t="s">
         <v>115</v>
@@ -5029,7 +5027,7 @@
       </c>
       <c r="K65" s="21">
         <f t="shared" si="6"/>
-        <v>9.5</v>
+        <v>9</v>
       </c>
       <c r="L65" s="21" t="s">
         <v>33</v>
@@ -5046,21 +5044,19 @@
       </c>
       <c r="P65" s="21">
         <f t="shared" si="7"/>
-        <v>6.5</v>
-      </c>
-      <c r="Q65" s="21">
-        <v>0</v>
-      </c>
+        <v>6.1000000000000005</v>
+      </c>
+      <c r="Q65" s="21"/>
       <c r="R65" s="21">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="S65" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="66" spans="1:19" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="85"/>
+      <c r="A66" s="72"/>
       <c r="B66" s="35"/>
       <c r="C66" s="19" t="s">
         <v>85</v>
@@ -5089,7 +5085,7 @@
       </c>
       <c r="K66" s="21">
         <f t="shared" si="6"/>
-        <v>10.5</v>
+        <v>10</v>
       </c>
       <c r="L66" s="21" t="s">
         <v>33</v>
@@ -5106,21 +5102,21 @@
       </c>
       <c r="P66" s="21">
         <f t="shared" si="7"/>
-        <v>7.2</v>
+        <v>6.8000000000000007</v>
       </c>
       <c r="Q66" s="21">
         <v>1.5</v>
       </c>
       <c r="R66" s="21">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>9</v>
       </c>
       <c r="S66" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:19" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="85"/>
+      <c r="A67" s="72"/>
       <c r="B67" s="35"/>
       <c r="C67" s="19" t="s">
         <v>86</v>
@@ -5149,7 +5145,7 @@
       </c>
       <c r="K67" s="21">
         <f t="shared" si="6"/>
-        <v>11.5</v>
+        <v>11</v>
       </c>
       <c r="L67" s="21" t="s">
         <v>33</v>
@@ -5166,21 +5162,21 @@
       </c>
       <c r="P67" s="21">
         <f t="shared" si="7"/>
-        <v>7.9</v>
+        <v>7.5000000000000009</v>
       </c>
       <c r="Q67" s="21">
-        <v>0.4</v>
+        <v>1.3</v>
       </c>
       <c r="R67" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S67" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:19" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="85"/>
+      <c r="A68" s="72"/>
       <c r="B68" s="35"/>
       <c r="C68" s="19" t="s">
         <v>87</v>
@@ -5209,7 +5205,7 @@
       </c>
       <c r="K68" s="21">
         <f t="shared" si="6"/>
-        <v>12.5</v>
+        <v>12</v>
       </c>
       <c r="L68" s="21" t="s">
         <v>33</v>
@@ -5226,21 +5222,19 @@
       </c>
       <c r="P68" s="21">
         <f t="shared" si="7"/>
-        <v>8.6</v>
-      </c>
-      <c r="Q68" s="21">
-        <v>0</v>
-      </c>
+        <v>8.2000000000000011</v>
+      </c>
+      <c r="Q68" s="21"/>
       <c r="R68" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S68" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="85" t="s">
+      <c r="A69" s="72" t="s">
         <v>88</v>
       </c>
       <c r="B69" s="35"/>
@@ -5271,7 +5265,7 @@
       </c>
       <c r="K69" s="21">
         <f t="shared" si="6"/>
-        <v>14.5</v>
+        <v>14</v>
       </c>
       <c r="L69" s="21" t="s">
         <v>33</v>
@@ -5288,21 +5282,19 @@
       </c>
       <c r="P69" s="21">
         <f t="shared" si="7"/>
-        <v>10</v>
-      </c>
-      <c r="Q69" s="21">
-        <v>0</v>
-      </c>
+        <v>9.6000000000000014</v>
+      </c>
+      <c r="Q69" s="21"/>
       <c r="R69" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S69" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="85"/>
+      <c r="A70" s="72"/>
       <c r="B70" s="35"/>
       <c r="C70" s="19" t="s">
         <v>50</v>
@@ -5331,7 +5323,7 @@
       </c>
       <c r="K70" s="21">
         <f t="shared" si="6"/>
-        <v>15.5</v>
+        <v>15</v>
       </c>
       <c r="L70" s="21" t="s">
         <v>33</v>
@@ -5348,21 +5340,19 @@
       </c>
       <c r="P70" s="21">
         <f t="shared" si="7"/>
-        <v>10.7</v>
-      </c>
-      <c r="Q70" s="21">
-        <v>0</v>
-      </c>
+        <v>10.3</v>
+      </c>
+      <c r="Q70" s="21"/>
       <c r="R70" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S70" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="71" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="85"/>
+      <c r="A71" s="72"/>
       <c r="B71" s="35"/>
       <c r="C71" s="19" t="s">
         <v>51</v>
@@ -5391,7 +5381,7 @@
       </c>
       <c r="K71" s="21">
         <f t="shared" si="6"/>
-        <v>16.5</v>
+        <v>16</v>
       </c>
       <c r="L71" s="21" t="s">
         <v>33</v>
@@ -5408,21 +5398,19 @@
       </c>
       <c r="P71" s="21">
         <f t="shared" si="7"/>
-        <v>11.399999999999999</v>
-      </c>
-      <c r="Q71" s="21">
-        <v>0</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="Q71" s="21"/>
       <c r="R71" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S71" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="72" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="93" t="s">
+      <c r="A72" s="73" t="s">
         <v>89</v>
       </c>
       <c r="B72" s="34"/>
@@ -5453,7 +5441,7 @@
       </c>
       <c r="K72" s="21">
         <f t="shared" si="6"/>
-        <v>18.5</v>
+        <v>18</v>
       </c>
       <c r="L72" s="21" t="s">
         <v>33</v>
@@ -5470,21 +5458,19 @@
       </c>
       <c r="P72" s="21">
         <f t="shared" si="7"/>
-        <v>12.799999999999999</v>
-      </c>
-      <c r="Q72" s="21">
-        <v>0</v>
-      </c>
+        <v>12.4</v>
+      </c>
+      <c r="Q72" s="21"/>
       <c r="R72" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S72" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="73" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="94"/>
+      <c r="A73" s="74"/>
       <c r="B73" s="34"/>
       <c r="C73" s="19" t="s">
         <v>55</v>
@@ -5513,7 +5499,7 @@
       </c>
       <c r="K73" s="21">
         <f t="shared" si="6"/>
-        <v>20.5</v>
+        <v>20</v>
       </c>
       <c r="L73" s="21" t="s">
         <v>33</v>
@@ -5530,21 +5516,19 @@
       </c>
       <c r="P73" s="21">
         <f t="shared" si="7"/>
-        <v>14.2</v>
-      </c>
-      <c r="Q73" s="21">
-        <v>0</v>
-      </c>
+        <v>13.8</v>
+      </c>
+      <c r="Q73" s="21"/>
       <c r="R73" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S73" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="74" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="94"/>
+      <c r="A74" s="74"/>
       <c r="B74" s="34"/>
       <c r="C74" s="19" t="s">
         <v>56</v>
@@ -5573,7 +5557,7 @@
       </c>
       <c r="K74" s="21">
         <f t="shared" si="6"/>
-        <v>21.5</v>
+        <v>21</v>
       </c>
       <c r="L74" s="21" t="s">
         <v>33</v>
@@ -5590,21 +5574,19 @@
       </c>
       <c r="P74" s="21">
         <f t="shared" si="7"/>
-        <v>14.899999999999999</v>
-      </c>
-      <c r="Q74" s="21">
-        <v>0</v>
-      </c>
+        <v>14.5</v>
+      </c>
+      <c r="Q74" s="21"/>
       <c r="R74" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S74" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="94"/>
+      <c r="A75" s="74"/>
       <c r="B75" s="34"/>
       <c r="C75" s="19" t="s">
         <v>57</v>
@@ -5633,7 +5615,7 @@
       </c>
       <c r="K75" s="21">
         <f t="shared" si="6"/>
-        <v>22.5</v>
+        <v>22</v>
       </c>
       <c r="L75" s="21" t="s">
         <v>33</v>
@@ -5650,21 +5632,19 @@
       </c>
       <c r="P75" s="21">
         <f t="shared" si="7"/>
-        <v>15.599999999999998</v>
-      </c>
-      <c r="Q75" s="21">
-        <v>0</v>
-      </c>
+        <v>15.2</v>
+      </c>
+      <c r="Q75" s="21"/>
       <c r="R75" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S75" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="76" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="94"/>
+      <c r="A76" s="74"/>
       <c r="B76" s="34"/>
       <c r="C76" s="19" t="s">
         <v>58</v>
@@ -5693,7 +5673,7 @@
       </c>
       <c r="K76" s="21">
         <f t="shared" si="6"/>
-        <v>23.5</v>
+        <v>23</v>
       </c>
       <c r="L76" s="21" t="s">
         <v>33</v>
@@ -5710,21 +5690,19 @@
       </c>
       <c r="P76" s="21">
         <f t="shared" si="7"/>
-        <v>16.299999999999997</v>
-      </c>
-      <c r="Q76" s="21">
-        <v>0</v>
-      </c>
+        <v>15.899999999999999</v>
+      </c>
+      <c r="Q76" s="21"/>
       <c r="R76" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S76" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="94"/>
+      <c r="A77" s="74"/>
       <c r="B77" s="34"/>
       <c r="C77" s="19" t="s">
         <v>91</v>
@@ -5753,7 +5731,7 @@
       </c>
       <c r="K77" s="21">
         <f t="shared" si="6"/>
-        <v>28.5</v>
+        <v>28</v>
       </c>
       <c r="L77" s="21"/>
       <c r="M77" s="21"/>
@@ -5766,19 +5744,19 @@
       </c>
       <c r="P77" s="21">
         <f t="shared" si="7"/>
-        <v>19.699999999999996</v>
+        <v>19.299999999999997</v>
       </c>
       <c r="Q77" s="21"/>
       <c r="R77" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S77" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="94"/>
+      <c r="A78" s="74"/>
       <c r="B78" s="34"/>
       <c r="C78" s="19" t="s">
         <v>92</v>
@@ -5807,7 +5785,7 @@
       </c>
       <c r="K78" s="21">
         <f t="shared" si="6"/>
-        <v>29.5</v>
+        <v>29</v>
       </c>
       <c r="L78" s="21" t="s">
         <v>33</v>
@@ -5824,19 +5802,19 @@
       </c>
       <c r="P78" s="21">
         <f t="shared" si="7"/>
-        <v>20.399999999999995</v>
+        <v>19.999999999999996</v>
       </c>
       <c r="Q78" s="21"/>
       <c r="R78" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S78" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="79" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="94"/>
+      <c r="A79" s="74"/>
       <c r="B79" s="34"/>
       <c r="C79" s="19" t="s">
         <v>93</v>
@@ -5865,7 +5843,7 @@
       </c>
       <c r="K79" s="21">
         <f t="shared" si="6"/>
-        <v>39.5</v>
+        <v>39</v>
       </c>
       <c r="L79" s="21" t="s">
         <v>33</v>
@@ -5882,17 +5860,17 @@
       </c>
       <c r="P79" s="21">
         <f t="shared" si="7"/>
-        <v>27.299999999999997</v>
+        <v>26.9</v>
       </c>
       <c r="Q79" s="21"/>
       <c r="R79" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S79" s="21"/>
     </row>
     <row r="80" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="94"/>
+      <c r="A80" s="74"/>
       <c r="B80" s="34"/>
       <c r="C80" s="19" t="s">
         <v>94</v>
@@ -5921,7 +5899,7 @@
       </c>
       <c r="K80" s="21">
         <f t="shared" si="6"/>
-        <v>40.5</v>
+        <v>40</v>
       </c>
       <c r="L80" s="21" t="s">
         <v>95</v>
@@ -5938,17 +5916,17 @@
       </c>
       <c r="P80" s="21">
         <f t="shared" si="7"/>
-        <v>27.999999999999996</v>
+        <v>27.599999999999998</v>
       </c>
       <c r="Q80" s="21"/>
       <c r="R80" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S80" s="21"/>
     </row>
     <row r="81" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="94"/>
+      <c r="A81" s="74"/>
       <c r="B81" s="34"/>
       <c r="C81" s="19" t="s">
         <v>96</v>
@@ -5977,7 +5955,7 @@
       </c>
       <c r="K81" s="21">
         <f t="shared" si="6"/>
-        <v>41.5</v>
+        <v>41</v>
       </c>
       <c r="L81" s="21" t="s">
         <v>95</v>
@@ -5994,17 +5972,17 @@
       </c>
       <c r="P81" s="21">
         <f t="shared" si="7"/>
-        <v>28.699999999999996</v>
+        <v>28.299999999999997</v>
       </c>
       <c r="Q81" s="21"/>
       <c r="R81" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S81" s="21"/>
     </row>
     <row r="82" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="95"/>
+      <c r="A82" s="75"/>
       <c r="B82" s="34"/>
       <c r="C82" s="19" t="s">
         <v>97</v>
@@ -6033,7 +6011,7 @@
       </c>
       <c r="K82" s="21">
         <f t="shared" si="6"/>
-        <v>42.5</v>
+        <v>42</v>
       </c>
       <c r="L82" s="21" t="s">
         <v>95</v>
@@ -6050,17 +6028,17 @@
       </c>
       <c r="P82" s="21">
         <f t="shared" si="7"/>
-        <v>29.399999999999995</v>
+        <v>28.999999999999996</v>
       </c>
       <c r="Q82" s="21"/>
       <c r="R82" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S82" s="21"/>
     </row>
     <row r="83" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="85" t="s">
+      <c r="A83" s="72" t="s">
         <v>98</v>
       </c>
       <c r="B83" s="35"/>
@@ -6091,7 +6069,7 @@
       </c>
       <c r="K83" s="21">
         <f>J83+K82</f>
-        <v>47.5</v>
+        <v>47</v>
       </c>
       <c r="L83" s="21" t="s">
         <v>33</v>
@@ -6108,56 +6086,54 @@
       </c>
       <c r="P83" s="21">
         <f>O83+P82</f>
-        <v>32.799999999999997</v>
-      </c>
-      <c r="Q83" s="21">
-        <v>0</v>
-      </c>
+        <v>32.4</v>
+      </c>
+      <c r="Q83" s="21"/>
       <c r="R83" s="21">
         <f>Q83+R82</f>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S83" s="21"/>
     </row>
     <row r="84" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="85"/>
+      <c r="A84" s="72"/>
       <c r="B84" s="35"/>
       <c r="C84" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="D84" s="98">
-        <v>1</v>
-      </c>
-      <c r="E84" s="98">
-        <v>0</v>
-      </c>
-      <c r="F84" s="98">
-        <v>0</v>
-      </c>
-      <c r="G84" s="98">
-        <v>0</v>
-      </c>
-      <c r="H84" s="98">
-        <v>0</v>
-      </c>
-      <c r="I84" s="98">
-        <v>2</v>
-      </c>
-      <c r="J84" s="98">
+      <c r="D84" s="65">
+        <v>1</v>
+      </c>
+      <c r="E84" s="65">
+        <v>0</v>
+      </c>
+      <c r="F84" s="65">
+        <v>0</v>
+      </c>
+      <c r="G84" s="65">
+        <v>0</v>
+      </c>
+      <c r="H84" s="65">
+        <v>0</v>
+      </c>
+      <c r="I84" s="65">
+        <v>2</v>
+      </c>
+      <c r="J84" s="65">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="K84" s="21">
         <f>J84+K83</f>
-        <v>49.5</v>
+        <v>49</v>
       </c>
       <c r="L84" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="M84" s="96">
+      <c r="M84" s="63">
         <v>3</v>
       </c>
-      <c r="N84" s="96">
+      <c r="N84" s="63">
         <v>8</v>
       </c>
       <c r="O84" s="21">
@@ -6166,14 +6142,14 @@
       </c>
       <c r="P84" s="21">
         <f>O84+P83</f>
-        <v>34.199999999999996</v>
-      </c>
-      <c r="Q84" s="96"/>
-      <c r="R84" s="96"/>
-      <c r="S84" s="96"/>
+        <v>33.799999999999997</v>
+      </c>
+      <c r="Q84" s="63"/>
+      <c r="R84" s="63"/>
+      <c r="S84" s="63"/>
     </row>
     <row r="85" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="85"/>
+      <c r="A85" s="72"/>
       <c r="B85" s="35"/>
       <c r="C85" s="14" t="s">
         <v>62</v>
@@ -6202,7 +6178,7 @@
       </c>
       <c r="K85" s="21">
         <f>J85+K83</f>
-        <v>48</v>
+        <v>47.5</v>
       </c>
       <c r="L85" s="21"/>
       <c r="M85" s="21"/>
@@ -6215,19 +6191,17 @@
       </c>
       <c r="P85" s="21">
         <f>O85+P84</f>
-        <v>34.499999999999993</v>
-      </c>
-      <c r="Q85" s="21">
-        <v>0</v>
-      </c>
+        <v>34.099999999999994</v>
+      </c>
+      <c r="Q85" s="21"/>
       <c r="R85" s="21">
         <f>Q85+R83</f>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S85" s="21"/>
     </row>
     <row r="86" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="85"/>
+      <c r="A86" s="72"/>
       <c r="B86" s="35"/>
       <c r="C86" s="19" t="s">
         <v>99</v>
@@ -6256,7 +6230,7 @@
       </c>
       <c r="K86" s="21">
         <f t="shared" si="6"/>
-        <v>48.5</v>
+        <v>48</v>
       </c>
       <c r="L86" s="21" t="s">
         <v>95</v>
@@ -6273,17 +6247,17 @@
       </c>
       <c r="P86" s="21">
         <f t="shared" si="7"/>
-        <v>34.79999999999999</v>
+        <v>34.399999999999991</v>
       </c>
       <c r="Q86" s="21"/>
       <c r="R86" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S86" s="21"/>
     </row>
     <row r="87" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="85"/>
+      <c r="A87" s="72"/>
       <c r="B87" s="35"/>
       <c r="C87" s="19" t="s">
         <v>100</v>
@@ -6312,7 +6286,7 @@
       </c>
       <c r="K87" s="21">
         <f t="shared" si="6"/>
-        <v>50.5</v>
+        <v>50</v>
       </c>
       <c r="L87" s="21" t="s">
         <v>33</v>
@@ -6329,19 +6303,17 @@
       </c>
       <c r="P87" s="21">
         <f t="shared" si="7"/>
-        <v>36.199999999999989</v>
-      </c>
-      <c r="Q87" s="21">
-        <v>0</v>
-      </c>
+        <v>35.79999999999999</v>
+      </c>
+      <c r="Q87" s="21"/>
       <c r="R87" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S87" s="21"/>
     </row>
     <row r="88" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="85"/>
+      <c r="A88" s="72"/>
       <c r="B88" s="35"/>
       <c r="C88" s="19" t="s">
         <v>65</v>
@@ -6370,7 +6342,7 @@
       </c>
       <c r="K88" s="21">
         <f t="shared" si="6"/>
-        <v>71.5</v>
+        <v>71</v>
       </c>
       <c r="L88" s="21" t="s">
         <v>66</v>
@@ -6387,19 +6359,17 @@
       </c>
       <c r="P88" s="21">
         <f t="shared" si="7"/>
-        <v>50.699999999999989</v>
-      </c>
-      <c r="Q88" s="21">
-        <v>0</v>
-      </c>
+        <v>50.29999999999999</v>
+      </c>
+      <c r="Q88" s="21"/>
       <c r="R88" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S88" s="21"/>
     </row>
     <row r="89" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="85"/>
+      <c r="A89" s="72"/>
       <c r="B89" s="35"/>
       <c r="C89" s="19" t="s">
         <v>67</v>
@@ -6428,7 +6398,7 @@
       </c>
       <c r="K89" s="21">
         <f t="shared" si="6"/>
-        <v>74.5</v>
+        <v>74</v>
       </c>
       <c r="L89" s="21"/>
       <c r="M89" s="21"/>
@@ -6441,19 +6411,17 @@
       </c>
       <c r="P89" s="21">
         <f t="shared" si="7"/>
-        <v>52.79999999999999</v>
-      </c>
-      <c r="Q89" s="21">
-        <v>0</v>
-      </c>
+        <v>52.399999999999991</v>
+      </c>
+      <c r="Q89" s="21"/>
       <c r="R89" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S89" s="21"/>
     </row>
     <row r="90" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="85"/>
+      <c r="A90" s="72"/>
       <c r="B90" s="35"/>
       <c r="C90" s="19" t="s">
         <v>68</v>
@@ -6482,7 +6450,7 @@
       </c>
       <c r="K90" s="21">
         <f t="shared" si="6"/>
-        <v>77.5</v>
+        <v>77</v>
       </c>
       <c r="L90" s="21" t="s">
         <v>33</v>
@@ -6499,19 +6467,17 @@
       </c>
       <c r="P90" s="21">
         <f t="shared" si="7"/>
-        <v>54.899999999999991</v>
-      </c>
-      <c r="Q90" s="21">
-        <v>0</v>
-      </c>
+        <v>54.499999999999993</v>
+      </c>
+      <c r="Q90" s="21"/>
       <c r="R90" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S90" s="21"/>
     </row>
     <row r="91" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="85" t="s">
+      <c r="A91" s="72" t="s">
         <v>101</v>
       </c>
       <c r="B91" s="35"/>
@@ -6542,7 +6508,7 @@
       </c>
       <c r="K91" s="21">
         <f t="shared" si="6"/>
-        <v>79.5</v>
+        <v>79</v>
       </c>
       <c r="L91" s="21" t="s">
         <v>66</v>
@@ -6559,19 +6525,17 @@
       </c>
       <c r="P91" s="21">
         <f t="shared" si="7"/>
-        <v>56.29999999999999</v>
-      </c>
-      <c r="Q91" s="21">
-        <v>0</v>
-      </c>
+        <v>55.899999999999991</v>
+      </c>
+      <c r="Q91" s="21"/>
       <c r="R91" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S91" s="21"/>
     </row>
     <row r="92" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="85" t="s">
+      <c r="A92" s="72" t="s">
         <v>101</v>
       </c>
       <c r="B92" s="35"/>
@@ -6602,7 +6566,7 @@
       </c>
       <c r="K92" s="21">
         <f t="shared" si="6"/>
-        <v>84.5</v>
+        <v>84</v>
       </c>
       <c r="L92" s="21" t="s">
         <v>95</v>
@@ -6619,19 +6583,17 @@
       </c>
       <c r="P92" s="21">
         <f t="shared" si="7"/>
-        <v>59.699999999999989</v>
-      </c>
-      <c r="Q92" s="21">
-        <v>0</v>
-      </c>
+        <v>59.29999999999999</v>
+      </c>
+      <c r="Q92" s="21"/>
       <c r="R92" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S92" s="21"/>
     </row>
     <row r="93" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="85"/>
+      <c r="A93" s="72"/>
       <c r="B93" s="35"/>
       <c r="C93" s="19" t="s">
         <v>72</v>
@@ -6660,7 +6622,7 @@
       </c>
       <c r="K93" s="21">
         <f t="shared" si="6"/>
-        <v>86.5</v>
+        <v>86</v>
       </c>
       <c r="L93" s="21" t="s">
         <v>33</v>
@@ -6677,19 +6639,17 @@
       </c>
       <c r="P93" s="21">
         <f t="shared" si="7"/>
-        <v>61.099999999999987</v>
-      </c>
-      <c r="Q93" s="21">
-        <v>0</v>
-      </c>
+        <v>60.699999999999989</v>
+      </c>
+      <c r="Q93" s="21"/>
       <c r="R93" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S93" s="21"/>
     </row>
     <row r="94" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="85"/>
+      <c r="A94" s="72"/>
       <c r="B94" s="35"/>
       <c r="C94" s="19" t="s">
         <v>103</v>
@@ -6704,7 +6664,7 @@
         <v>0</v>
       </c>
       <c r="G94" s="22">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="H94" s="22">
         <v>0</v>
@@ -6714,7 +6674,7 @@
       </c>
       <c r="J94" s="22">
         <f t="shared" ref="J94:J114" si="9">SUM(E94:I94)</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="K94" s="21">
         <f t="shared" ref="K94:K114" si="10">J94+K93</f>
@@ -6731,21 +6691,21 @@
       </c>
       <c r="O94" s="21">
         <f>ROUND(((J94/J115)*100),1)</f>
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="P94" s="21">
         <f t="shared" ref="P94:P114" si="11">O94+P93</f>
-        <v>61.79999999999999</v>
+        <v>61.699999999999989</v>
       </c>
       <c r="Q94" s="21"/>
       <c r="R94" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S94" s="21"/>
     </row>
     <row r="95" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="85"/>
+      <c r="A95" s="72"/>
       <c r="B95" s="35"/>
       <c r="C95" s="19" t="s">
         <v>104</v>
@@ -6791,17 +6751,17 @@
       </c>
       <c r="P95" s="21">
         <f t="shared" si="11"/>
-        <v>65.199999999999989</v>
+        <v>65.099999999999994</v>
       </c>
       <c r="Q95" s="21"/>
       <c r="R95" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S95" s="21"/>
     </row>
     <row r="96" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="85"/>
+      <c r="A96" s="72"/>
       <c r="B96" s="35"/>
       <c r="C96" s="19" t="s">
         <v>105</v>
@@ -6847,17 +6807,17 @@
       </c>
       <c r="P96" s="21">
         <f t="shared" si="11"/>
-        <v>65.899999999999991</v>
+        <v>65.8</v>
       </c>
       <c r="Q96" s="21"/>
       <c r="R96" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S96" s="21"/>
     </row>
     <row r="97" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="85"/>
+      <c r="A97" s="72"/>
       <c r="B97" s="35"/>
       <c r="C97" s="19" t="s">
         <v>93</v>
@@ -6903,17 +6863,17 @@
       </c>
       <c r="P97" s="21">
         <f t="shared" si="11"/>
-        <v>72.8</v>
+        <v>72.7</v>
       </c>
       <c r="Q97" s="21"/>
       <c r="R97" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S97" s="21"/>
     </row>
     <row r="98" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="85"/>
+      <c r="A98" s="72"/>
       <c r="B98" s="35"/>
       <c r="C98" s="19" t="s">
         <v>94</v>
@@ -6959,17 +6919,17 @@
       </c>
       <c r="P98" s="21">
         <f t="shared" si="11"/>
-        <v>73.5</v>
+        <v>73.400000000000006</v>
       </c>
       <c r="Q98" s="21"/>
       <c r="R98" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S98" s="21"/>
     </row>
     <row r="99" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="85"/>
+      <c r="A99" s="72"/>
       <c r="B99" s="35"/>
       <c r="C99" s="19" t="s">
         <v>96</v>
@@ -7015,17 +6975,17 @@
       </c>
       <c r="P99" s="21">
         <f t="shared" si="11"/>
-        <v>74.2</v>
+        <v>74.100000000000009</v>
       </c>
       <c r="Q99" s="21"/>
       <c r="R99" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S99" s="21"/>
     </row>
     <row r="100" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="85"/>
+      <c r="A100" s="72"/>
       <c r="B100" s="35"/>
       <c r="C100" s="19" t="s">
         <v>97</v>
@@ -7071,17 +7031,17 @@
       </c>
       <c r="P100" s="21">
         <f t="shared" si="11"/>
-        <v>74.900000000000006</v>
+        <v>74.800000000000011</v>
       </c>
       <c r="Q100" s="21"/>
       <c r="R100" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S100" s="21"/>
     </row>
     <row r="101" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="87" t="s">
+      <c r="A101" s="66" t="s">
         <v>106</v>
       </c>
       <c r="B101" s="34"/>
@@ -7129,19 +7089,17 @@
       </c>
       <c r="P101" s="21">
         <f t="shared" si="11"/>
-        <v>76.300000000000011</v>
-      </c>
-      <c r="Q101" s="21">
-        <v>0</v>
-      </c>
+        <v>76.200000000000017</v>
+      </c>
+      <c r="Q101" s="21"/>
       <c r="R101" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S101" s="21"/>
     </row>
     <row r="102" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="88"/>
+      <c r="A102" s="67"/>
       <c r="B102" s="34"/>
       <c r="C102" s="19" t="s">
         <v>108</v>
@@ -7187,17 +7145,17 @@
       </c>
       <c r="P102" s="21">
         <f t="shared" si="11"/>
-        <v>77.000000000000014</v>
+        <v>76.90000000000002</v>
       </c>
       <c r="Q102" s="21"/>
       <c r="R102" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S102" s="21"/>
     </row>
     <row r="103" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="89"/>
+      <c r="A103" s="68"/>
       <c r="B103" s="34"/>
       <c r="C103" s="19" t="s">
         <v>109</v>
@@ -7243,17 +7201,17 @@
       </c>
       <c r="P103" s="21">
         <f t="shared" si="11"/>
-        <v>78.000000000000014</v>
+        <v>77.90000000000002</v>
       </c>
       <c r="Q103" s="21"/>
       <c r="R103" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S103" s="21"/>
     </row>
     <row r="104" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="89"/>
+      <c r="A104" s="68"/>
       <c r="B104" s="34"/>
       <c r="C104" s="19" t="s">
         <v>110</v>
@@ -7299,17 +7257,17 @@
       </c>
       <c r="P104" s="21">
         <f t="shared" si="11"/>
-        <v>79.700000000000017</v>
+        <v>79.600000000000023</v>
       </c>
       <c r="Q104" s="21"/>
       <c r="R104" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S104" s="21"/>
     </row>
     <row r="105" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="89"/>
+      <c r="A105" s="68"/>
       <c r="B105" s="41"/>
       <c r="C105" s="38" t="s">
         <v>111</v>
@@ -7355,17 +7313,17 @@
       </c>
       <c r="P105" s="21">
         <f t="shared" si="11"/>
-        <v>81.40000000000002</v>
+        <v>81.300000000000026</v>
       </c>
       <c r="Q105" s="21"/>
       <c r="R105" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S105" s="21"/>
     </row>
     <row r="106" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="90"/>
+      <c r="A106" s="69"/>
       <c r="B106" s="42"/>
       <c r="C106" s="39" t="s">
         <v>112</v>
@@ -7411,17 +7369,17 @@
       </c>
       <c r="P106" s="21">
         <f t="shared" si="11"/>
-        <v>82.800000000000026</v>
+        <v>82.700000000000031</v>
       </c>
       <c r="Q106" s="21"/>
       <c r="R106" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S106" s="21"/>
     </row>
     <row r="107" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="90"/>
+      <c r="A107" s="69"/>
       <c r="B107" s="42"/>
       <c r="C107" s="39" t="s">
         <v>113</v>
@@ -7461,17 +7419,17 @@
       </c>
       <c r="P107" s="21">
         <f t="shared" si="11"/>
-        <v>83.500000000000028</v>
+        <v>83.400000000000034</v>
       </c>
       <c r="Q107" s="21"/>
       <c r="R107" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S107" s="21"/>
     </row>
     <row r="108" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="89"/>
+      <c r="A108" s="68"/>
       <c r="B108" s="43"/>
       <c r="C108" s="38" t="s">
         <v>75</v>
@@ -7517,19 +7475,17 @@
       </c>
       <c r="P108" s="21">
         <f t="shared" si="11"/>
-        <v>86.900000000000034</v>
-      </c>
-      <c r="Q108" s="21">
-        <v>0</v>
-      </c>
+        <v>86.80000000000004</v>
+      </c>
+      <c r="Q108" s="21"/>
       <c r="R108" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S108" s="21"/>
     </row>
     <row r="109" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="89"/>
+      <c r="A109" s="68"/>
       <c r="B109" s="44"/>
       <c r="C109" s="55" t="s">
         <v>114</v>
@@ -7575,17 +7531,17 @@
       </c>
       <c r="P109" s="21">
         <f t="shared" si="11"/>
-        <v>87.600000000000037</v>
+        <v>87.500000000000043</v>
       </c>
       <c r="Q109" s="21"/>
       <c r="R109" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S109" s="21"/>
     </row>
     <row r="110" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="91"/>
+      <c r="A110" s="70"/>
       <c r="B110" s="44"/>
       <c r="C110" s="55" t="s">
         <v>93</v>
@@ -7631,17 +7587,17 @@
       </c>
       <c r="P110" s="21">
         <f t="shared" si="11"/>
-        <v>94.500000000000043</v>
+        <v>94.400000000000048</v>
       </c>
       <c r="Q110" s="21"/>
       <c r="R110" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S110" s="21"/>
     </row>
     <row r="111" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="91"/>
+      <c r="A111" s="70"/>
       <c r="B111" s="44"/>
       <c r="C111" s="55" t="s">
         <v>94</v>
@@ -7687,17 +7643,17 @@
       </c>
       <c r="P111" s="21">
         <f t="shared" si="11"/>
-        <v>95.200000000000045</v>
+        <v>95.100000000000051</v>
       </c>
       <c r="Q111" s="21"/>
       <c r="R111" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S111" s="21"/>
     </row>
     <row r="112" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="91"/>
+      <c r="A112" s="70"/>
       <c r="B112" s="44"/>
       <c r="C112" s="55" t="s">
         <v>96</v>
@@ -7743,17 +7699,17 @@
       </c>
       <c r="P112" s="21">
         <f t="shared" si="11"/>
-        <v>95.900000000000048</v>
+        <v>95.800000000000054</v>
       </c>
       <c r="Q112" s="21"/>
       <c r="R112" s="21">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S112" s="21"/>
     </row>
     <row r="113" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="91"/>
+      <c r="A113" s="70"/>
       <c r="B113" s="44"/>
       <c r="C113" s="55" t="s">
         <v>97</v>
@@ -7799,16 +7755,16 @@
       </c>
       <c r="P113" s="21">
         <f t="shared" si="11"/>
-        <v>96.600000000000051</v>
-      </c>
-      <c r="Q113" s="96"/>
-      <c r="R113" s="96"/>
-      <c r="S113" s="96"/>
+        <v>96.500000000000057</v>
+      </c>
+      <c r="Q113" s="63"/>
+      <c r="R113" s="63"/>
+      <c r="S113" s="63"/>
     </row>
     <row r="114" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="92"/>
+      <c r="A114" s="71"/>
       <c r="B114" s="44"/>
-      <c r="C114" s="97" t="s">
+      <c r="C114" s="64" t="s">
         <v>116</v>
       </c>
       <c r="D114" s="61">
@@ -7848,12 +7804,12 @@
       </c>
       <c r="P114" s="21">
         <f t="shared" si="11"/>
-        <v>100.00000000000006</v>
+        <v>99.900000000000063</v>
       </c>
       <c r="Q114" s="21"/>
       <c r="R114" s="21">
         <f>Q114+R112</f>
-        <v>1.9</v>
+        <v>10.3</v>
       </c>
       <c r="S114" s="21"/>
     </row>
@@ -7892,60 +7848,25 @@
       <c r="N115" s="48"/>
       <c r="O115" s="21">
         <f>SUM(O60:O114)</f>
-        <v>100.00000000000006</v>
+        <v>99.900000000000063</v>
       </c>
       <c r="P115" s="3"/>
-      <c r="Q115" s="21">
-        <v>0</v>
-      </c>
+      <c r="Q115" s="21"/>
       <c r="R115" s="8"/>
       <c r="S115" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="A101:A114"/>
-    <mergeCell ref="A63:A68"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="A72:A82"/>
-    <mergeCell ref="A83:A91"/>
-    <mergeCell ref="A92:A100"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="K54:K59"/>
-    <mergeCell ref="L54:L59"/>
-    <mergeCell ref="M54:M59"/>
-    <mergeCell ref="N54:N59"/>
-    <mergeCell ref="F54:F59"/>
-    <mergeCell ref="G54:G59"/>
-    <mergeCell ref="H54:H59"/>
-    <mergeCell ref="I54:I59"/>
-    <mergeCell ref="J54:J59"/>
-    <mergeCell ref="A54:A59"/>
-    <mergeCell ref="B54:B59"/>
-    <mergeCell ref="C54:C59"/>
-    <mergeCell ref="D54:D59"/>
-    <mergeCell ref="E54:E59"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A51:S51"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="E53:K53"/>
-    <mergeCell ref="L53:P53"/>
-    <mergeCell ref="Q53:S53"/>
-    <mergeCell ref="P54:P59"/>
-    <mergeCell ref="Q54:Q59"/>
-    <mergeCell ref="R54:R59"/>
-    <mergeCell ref="S54:S59"/>
-    <mergeCell ref="O54:O59"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="A36:A43"/>
-    <mergeCell ref="P8:P13"/>
-    <mergeCell ref="Q8:Q13"/>
-    <mergeCell ref="R8:R13"/>
-    <mergeCell ref="S8:S13"/>
-    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="E7:K7"/>
+    <mergeCell ref="L7:P7"/>
     <mergeCell ref="Q7:S7"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="B8:B13"/>
@@ -7962,16 +7883,49 @@
     <mergeCell ref="M8:M13"/>
     <mergeCell ref="N8:N13"/>
     <mergeCell ref="O8:O13"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="E7:K7"/>
-    <mergeCell ref="L7:P7"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="P8:P13"/>
+    <mergeCell ref="Q8:Q13"/>
+    <mergeCell ref="R8:R13"/>
+    <mergeCell ref="S8:S13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="P54:P59"/>
+    <mergeCell ref="Q54:Q59"/>
+    <mergeCell ref="R54:R59"/>
+    <mergeCell ref="S54:S59"/>
+    <mergeCell ref="O54:O59"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A51:S51"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="E53:K53"/>
+    <mergeCell ref="L53:P53"/>
+    <mergeCell ref="Q53:S53"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="K54:K59"/>
+    <mergeCell ref="L54:L59"/>
+    <mergeCell ref="M54:M59"/>
+    <mergeCell ref="N54:N59"/>
+    <mergeCell ref="F54:F59"/>
+    <mergeCell ref="G54:G59"/>
+    <mergeCell ref="H54:H59"/>
+    <mergeCell ref="I54:I59"/>
+    <mergeCell ref="J54:J59"/>
+    <mergeCell ref="A54:A59"/>
+    <mergeCell ref="B54:B59"/>
+    <mergeCell ref="C54:C59"/>
+    <mergeCell ref="D54:D59"/>
+    <mergeCell ref="E54:E59"/>
+    <mergeCell ref="A101:A114"/>
+    <mergeCell ref="A63:A68"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="A72:A82"/>
+    <mergeCell ref="A83:A91"/>
+    <mergeCell ref="A92:A100"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizacion TASK de equipo hasta semana 8
</commit_message>
<xml_diff>
--- a/NoteBook/summary/TASK_TEAM.xlsx
+++ b/NoteBook/summary/TASK_TEAM.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FabiánEduardo\Documents\GitHub\tsp\NoteBook\summary\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="8760" windowHeight="6105"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1621,6 +1626,90 @@
     <xf numFmtId="0" fontId="58" fillId="10" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="80" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="82" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="81" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="81" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="42" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1639,9 +1728,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1649,87 +1735,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="73" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="42" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="80" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="82" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="81" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="81" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2004,7 +2009,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2014,8 +2019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D51" workbookViewId="0">
-      <selection activeCell="R61" sqref="R61"/>
+    <sheetView tabSelected="1" topLeftCell="B82" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R116" sqref="R116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2037,16 +2042,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="92" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
+      <c r="A1" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="29"/>
@@ -2056,51 +2061,51 @@
       <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="93"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="93"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="70"/>
       <c r="E3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="95">
+      <c r="F3" s="72">
         <v>41719</v>
       </c>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
     </row>
     <row r="4" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="97"/>
-      <c r="D4" s="91"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="74"/>
       <c r="E4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="91" t="s">
+      <c r="F4" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
     </row>
     <row r="5" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="90"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="90"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="76"/>
       <c r="E5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="91">
-        <v>1</v>
-      </c>
-      <c r="G5" s="91"/>
-      <c r="H5" s="91"/>
+      <c r="F5" s="74">
+        <v>1</v>
+      </c>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
@@ -2124,200 +2129,200 @@
       <c r="S6" s="24"/>
     </row>
     <row r="7" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="88"/>
-      <c r="C7" s="88"/>
-      <c r="D7" s="89"/>
-      <c r="E7" s="87" t="s">
+      <c r="B7" s="77"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="88"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="88"/>
-      <c r="I7" s="88"/>
-      <c r="J7" s="88"/>
-      <c r="K7" s="89"/>
-      <c r="L7" s="87" t="s">
+      <c r="F7" s="77"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="79"/>
+      <c r="L7" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="88"/>
-      <c r="N7" s="88"/>
-      <c r="O7" s="88"/>
-      <c r="P7" s="89"/>
-      <c r="Q7" s="87" t="s">
+      <c r="M7" s="77"/>
+      <c r="N7" s="77"/>
+      <c r="O7" s="77"/>
+      <c r="P7" s="79"/>
+      <c r="Q7" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="R7" s="88"/>
-      <c r="S7" s="89"/>
+      <c r="R7" s="77"/>
+      <c r="S7" s="79"/>
     </row>
     <row r="8" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="77" t="s">
+      <c r="C8" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="75" t="s">
+      <c r="D8" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="75" t="s">
+      <c r="E8" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="75" t="s">
+      <c r="F8" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="75" t="s">
+      <c r="G8" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="75" t="s">
+      <c r="I8" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="75" t="s">
+      <c r="J8" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="75" t="s">
+      <c r="K8" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="77" t="s">
+      <c r="L8" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="M8" s="75" t="s">
+      <c r="M8" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="N8" s="75" t="s">
+      <c r="N8" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="O8" s="75" t="s">
+      <c r="O8" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="P8" s="75" t="s">
+      <c r="P8" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="Q8" s="75" t="s">
+      <c r="Q8" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="R8" s="75" t="s">
+      <c r="R8" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="S8" s="75" t="s">
+      <c r="S8" s="80" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="76"/>
-      <c r="B9" s="76"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="76"/>
-      <c r="F9" s="76"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="76"/>
-      <c r="I9" s="76"/>
-      <c r="J9" s="76"/>
-      <c r="K9" s="76"/>
-      <c r="L9" s="78"/>
-      <c r="M9" s="76"/>
-      <c r="N9" s="76"/>
-      <c r="O9" s="76"/>
-      <c r="P9" s="76"/>
-      <c r="Q9" s="76"/>
-      <c r="R9" s="76"/>
-      <c r="S9" s="76"/>
+      <c r="A9" s="81"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="84"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="81"/>
+      <c r="G9" s="81"/>
+      <c r="H9" s="81"/>
+      <c r="I9" s="81"/>
+      <c r="J9" s="81"/>
+      <c r="K9" s="81"/>
+      <c r="L9" s="84"/>
+      <c r="M9" s="81"/>
+      <c r="N9" s="81"/>
+      <c r="O9" s="81"/>
+      <c r="P9" s="81"/>
+      <c r="Q9" s="81"/>
+      <c r="R9" s="81"/>
+      <c r="S9" s="81"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="76"/>
-      <c r="B10" s="76"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="76"/>
-      <c r="G10" s="76"/>
-      <c r="H10" s="76"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="76"/>
-      <c r="K10" s="76"/>
-      <c r="L10" s="78"/>
-      <c r="M10" s="76"/>
-      <c r="N10" s="76"/>
-      <c r="O10" s="76"/>
-      <c r="P10" s="76"/>
-      <c r="Q10" s="76"/>
-      <c r="R10" s="76"/>
-      <c r="S10" s="76"/>
+      <c r="A10" s="81"/>
+      <c r="B10" s="81"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="81"/>
+      <c r="H10" s="81"/>
+      <c r="I10" s="81"/>
+      <c r="J10" s="81"/>
+      <c r="K10" s="81"/>
+      <c r="L10" s="84"/>
+      <c r="M10" s="81"/>
+      <c r="N10" s="81"/>
+      <c r="O10" s="81"/>
+      <c r="P10" s="81"/>
+      <c r="Q10" s="81"/>
+      <c r="R10" s="81"/>
+      <c r="S10" s="81"/>
     </row>
     <row r="11" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="76"/>
-      <c r="B11" s="76"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="76"/>
-      <c r="H11" s="76"/>
-      <c r="I11" s="76"/>
-      <c r="J11" s="76"/>
-      <c r="K11" s="76"/>
-      <c r="L11" s="78"/>
-      <c r="M11" s="76"/>
-      <c r="N11" s="76"/>
-      <c r="O11" s="76"/>
-      <c r="P11" s="76"/>
-      <c r="Q11" s="76"/>
-      <c r="R11" s="76"/>
-      <c r="S11" s="76"/>
+      <c r="A11" s="81"/>
+      <c r="B11" s="81"/>
+      <c r="C11" s="84"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="81"/>
+      <c r="L11" s="84"/>
+      <c r="M11" s="81"/>
+      <c r="N11" s="81"/>
+      <c r="O11" s="81"/>
+      <c r="P11" s="81"/>
+      <c r="Q11" s="81"/>
+      <c r="R11" s="81"/>
+      <c r="S11" s="81"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="76"/>
-      <c r="B12" s="76"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="76"/>
-      <c r="G12" s="76"/>
-      <c r="H12" s="76"/>
-      <c r="I12" s="76"/>
-      <c r="J12" s="76"/>
-      <c r="K12" s="76"/>
-      <c r="L12" s="78"/>
-      <c r="M12" s="76"/>
-      <c r="N12" s="76"/>
-      <c r="O12" s="76"/>
-      <c r="P12" s="76"/>
-      <c r="Q12" s="76"/>
-      <c r="R12" s="76"/>
-      <c r="S12" s="76"/>
+      <c r="A12" s="81"/>
+      <c r="B12" s="81"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="81"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="81"/>
+      <c r="L12" s="84"/>
+      <c r="M12" s="81"/>
+      <c r="N12" s="81"/>
+      <c r="O12" s="81"/>
+      <c r="P12" s="81"/>
+      <c r="Q12" s="81"/>
+      <c r="R12" s="81"/>
+      <c r="S12" s="81"/>
     </row>
     <row r="13" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="80"/>
-      <c r="B13" s="80"/>
-      <c r="C13" s="79"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="80"/>
-      <c r="H13" s="80"/>
-      <c r="I13" s="80"/>
-      <c r="J13" s="80"/>
-      <c r="K13" s="76"/>
-      <c r="L13" s="79"/>
-      <c r="M13" s="80"/>
-      <c r="N13" s="80"/>
-      <c r="O13" s="80"/>
-      <c r="P13" s="76"/>
-      <c r="Q13" s="80"/>
-      <c r="R13" s="80"/>
-      <c r="S13" s="80"/>
+      <c r="A13" s="82"/>
+      <c r="B13" s="82"/>
+      <c r="C13" s="85"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="82"/>
+      <c r="I13" s="82"/>
+      <c r="J13" s="82"/>
+      <c r="K13" s="81"/>
+      <c r="L13" s="85"/>
+      <c r="M13" s="82"/>
+      <c r="N13" s="82"/>
+      <c r="O13" s="82"/>
+      <c r="P13" s="81"/>
+      <c r="Q13" s="82"/>
+      <c r="R13" s="82"/>
+      <c r="S13" s="82"/>
     </row>
     <row r="14" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="82" t="s">
+      <c r="A14" s="86" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="25"/>
@@ -2379,7 +2384,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="83"/>
+      <c r="A15" s="87"/>
       <c r="B15" s="25"/>
       <c r="C15" s="18" t="s">
         <v>34</v>
@@ -2439,7 +2444,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="84"/>
+      <c r="A16" s="88"/>
       <c r="B16" s="25"/>
       <c r="C16" s="18" t="s">
         <v>35</v>
@@ -2499,7 +2504,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="82" t="s">
+      <c r="A17" s="86" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="25"/>
@@ -2561,7 +2566,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="83"/>
+      <c r="A18" s="87"/>
       <c r="B18" s="25"/>
       <c r="C18" s="18" t="s">
         <v>38</v>
@@ -2621,7 +2626,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="84"/>
+      <c r="A19" s="88"/>
       <c r="B19" s="25"/>
       <c r="C19" s="18" t="s">
         <v>39</v>
@@ -2681,7 +2686,7 @@
       </c>
     </row>
     <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="82" t="s">
+      <c r="A20" s="86" t="s">
         <v>40</v>
       </c>
       <c r="B20" s="25"/>
@@ -2743,7 +2748,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="83"/>
+      <c r="A21" s="87"/>
       <c r="B21" s="25"/>
       <c r="C21" s="18" t="s">
         <v>42</v>
@@ -2803,7 +2808,7 @@
       </c>
     </row>
     <row r="22" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="83"/>
+      <c r="A22" s="87"/>
       <c r="B22" s="25"/>
       <c r="C22" s="18" t="s">
         <v>43</v>
@@ -2863,7 +2868,7 @@
       </c>
     </row>
     <row r="23" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="83"/>
+      <c r="A23" s="87"/>
       <c r="B23" s="25"/>
       <c r="C23" s="18" t="s">
         <v>44</v>
@@ -2923,7 +2928,7 @@
       </c>
     </row>
     <row r="24" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="83"/>
+      <c r="A24" s="87"/>
       <c r="B24" s="25"/>
       <c r="C24" s="18" t="s">
         <v>45</v>
@@ -2983,7 +2988,7 @@
       </c>
     </row>
     <row r="25" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="83"/>
+      <c r="A25" s="87"/>
       <c r="B25" s="25"/>
       <c r="C25" s="18" t="s">
         <v>46</v>
@@ -3043,7 +3048,7 @@
       </c>
     </row>
     <row r="26" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="84"/>
+      <c r="A26" s="88"/>
       <c r="B26" s="25"/>
       <c r="C26" s="18" t="s">
         <v>47</v>
@@ -3103,7 +3108,7 @@
       </c>
     </row>
     <row r="27" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="82" t="s">
+      <c r="A27" s="86" t="s">
         <v>48</v>
       </c>
       <c r="B27" s="25"/>
@@ -3165,7 +3170,7 @@
       </c>
     </row>
     <row r="28" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="83"/>
+      <c r="A28" s="87"/>
       <c r="B28" s="25"/>
       <c r="C28" s="18" t="s">
         <v>50</v>
@@ -3225,7 +3230,7 @@
       </c>
     </row>
     <row r="29" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="83"/>
+      <c r="A29" s="87"/>
       <c r="B29" s="25"/>
       <c r="C29" s="18" t="s">
         <v>51</v>
@@ -3285,7 +3290,7 @@
       </c>
     </row>
     <row r="30" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="83"/>
+      <c r="A30" s="87"/>
       <c r="B30" s="25"/>
       <c r="C30" s="18" t="s">
         <v>52</v>
@@ -3345,7 +3350,7 @@
       </c>
     </row>
     <row r="31" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="82" t="s">
+      <c r="A31" s="86" t="s">
         <v>53</v>
       </c>
       <c r="B31" s="25"/>
@@ -3407,7 +3412,7 @@
       </c>
     </row>
     <row r="32" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="83"/>
+      <c r="A32" s="87"/>
       <c r="B32" s="25"/>
       <c r="C32" s="18" t="s">
         <v>55</v>
@@ -3467,7 +3472,7 @@
       </c>
     </row>
     <row r="33" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="83"/>
+      <c r="A33" s="87"/>
       <c r="B33" s="25"/>
       <c r="C33" s="18" t="s">
         <v>56</v>
@@ -3527,7 +3532,7 @@
       </c>
     </row>
     <row r="34" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="83"/>
+      <c r="A34" s="87"/>
       <c r="B34" s="25"/>
       <c r="C34" s="18" t="s">
         <v>57</v>
@@ -3587,7 +3592,7 @@
       </c>
     </row>
     <row r="35" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="84"/>
+      <c r="A35" s="88"/>
       <c r="B35" s="25"/>
       <c r="C35" s="18" t="s">
         <v>58</v>
@@ -3647,7 +3652,7 @@
       </c>
     </row>
     <row r="36" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="82" t="s">
+      <c r="A36" s="86" t="s">
         <v>59</v>
       </c>
       <c r="B36" s="25"/>
@@ -3709,7 +3714,7 @@
       </c>
     </row>
     <row r="37" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="83"/>
+      <c r="A37" s="87"/>
       <c r="B37" s="25"/>
       <c r="C37" s="18" t="s">
         <v>61</v>
@@ -3769,7 +3774,7 @@
       </c>
     </row>
     <row r="38" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="83"/>
+      <c r="A38" s="87"/>
       <c r="B38" s="25"/>
       <c r="C38" s="18" t="s">
         <v>62</v>
@@ -3825,7 +3830,7 @@
       </c>
     </row>
     <row r="39" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="83"/>
+      <c r="A39" s="87"/>
       <c r="B39" s="25"/>
       <c r="C39" s="18" t="s">
         <v>63</v>
@@ -3883,7 +3888,7 @@
       </c>
     </row>
     <row r="40" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="83"/>
+      <c r="A40" s="87"/>
       <c r="B40" s="25"/>
       <c r="C40" s="18" t="s">
         <v>64</v>
@@ -3943,7 +3948,7 @@
       </c>
     </row>
     <row r="41" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="83"/>
+      <c r="A41" s="87"/>
       <c r="B41" s="25"/>
       <c r="C41" s="18" t="s">
         <v>65</v>
@@ -4003,7 +4008,7 @@
       </c>
     </row>
     <row r="42" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="83"/>
+      <c r="A42" s="87"/>
       <c r="B42" s="25"/>
       <c r="C42" s="18" t="s">
         <v>67</v>
@@ -4059,7 +4064,7 @@
       </c>
     </row>
     <row r="43" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="84"/>
+      <c r="A43" s="88"/>
       <c r="B43" s="25"/>
       <c r="C43" s="18" t="s">
         <v>68</v>
@@ -4119,7 +4124,7 @@
       </c>
     </row>
     <row r="44" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="82" t="s">
+      <c r="A44" s="86" t="s">
         <v>69</v>
       </c>
       <c r="B44" s="25"/>
@@ -4181,7 +4186,7 @@
       </c>
     </row>
     <row r="45" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="83"/>
+      <c r="A45" s="87"/>
       <c r="B45" s="25"/>
       <c r="C45" s="18" t="s">
         <v>71</v>
@@ -4237,7 +4242,7 @@
       </c>
     </row>
     <row r="46" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="84"/>
+      <c r="A46" s="88"/>
       <c r="B46" s="25"/>
       <c r="C46" s="18" t="s">
         <v>72</v>
@@ -4297,7 +4302,7 @@
       </c>
     </row>
     <row r="47" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="82" t="s">
+      <c r="A47" s="86" t="s">
         <v>73</v>
       </c>
       <c r="B47" s="25"/>
@@ -4359,7 +4364,7 @@
       </c>
     </row>
     <row r="48" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="84"/>
+      <c r="A48" s="88"/>
       <c r="B48" s="25"/>
       <c r="C48" s="18" t="s">
         <v>75</v>
@@ -4485,27 +4490,27 @@
       <c r="S50" s="9"/>
     </row>
     <row r="51" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="85" t="s">
+      <c r="A51" s="89" t="s">
         <v>76</v>
       </c>
-      <c r="B51" s="86"/>
-      <c r="C51" s="85"/>
-      <c r="D51" s="86"/>
-      <c r="E51" s="86"/>
-      <c r="F51" s="86"/>
-      <c r="G51" s="86"/>
-      <c r="H51" s="86"/>
-      <c r="I51" s="86"/>
-      <c r="J51" s="86"/>
-      <c r="K51" s="86"/>
-      <c r="L51" s="86"/>
-      <c r="M51" s="86"/>
-      <c r="N51" s="86"/>
-      <c r="O51" s="86"/>
-      <c r="P51" s="86"/>
-      <c r="Q51" s="86"/>
-      <c r="R51" s="86"/>
-      <c r="S51" s="86"/>
+      <c r="B51" s="90"/>
+      <c r="C51" s="89"/>
+      <c r="D51" s="90"/>
+      <c r="E51" s="90"/>
+      <c r="F51" s="90"/>
+      <c r="G51" s="90"/>
+      <c r="H51" s="90"/>
+      <c r="I51" s="90"/>
+      <c r="J51" s="90"/>
+      <c r="K51" s="90"/>
+      <c r="L51" s="90"/>
+      <c r="M51" s="90"/>
+      <c r="N51" s="90"/>
+      <c r="O51" s="90"/>
+      <c r="P51" s="90"/>
+      <c r="Q51" s="90"/>
+      <c r="R51" s="90"/>
+      <c r="S51" s="90"/>
     </row>
     <row r="52" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="26"/>
@@ -4529,197 +4534,197 @@
       <c r="S52" s="24"/>
     </row>
     <row r="53" spans="1:19" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="87" t="s">
+      <c r="A53" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="B53" s="88"/>
-      <c r="C53" s="88"/>
-      <c r="D53" s="89"/>
-      <c r="E53" s="87" t="s">
+      <c r="B53" s="77"/>
+      <c r="C53" s="77"/>
+      <c r="D53" s="79"/>
+      <c r="E53" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="F53" s="88"/>
-      <c r="G53" s="88"/>
-      <c r="H53" s="88"/>
-      <c r="I53" s="88"/>
-      <c r="J53" s="88"/>
-      <c r="K53" s="89"/>
-      <c r="L53" s="87" t="s">
+      <c r="F53" s="77"/>
+      <c r="G53" s="77"/>
+      <c r="H53" s="77"/>
+      <c r="I53" s="77"/>
+      <c r="J53" s="77"/>
+      <c r="K53" s="79"/>
+      <c r="L53" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="M53" s="88"/>
-      <c r="N53" s="88"/>
-      <c r="O53" s="88"/>
-      <c r="P53" s="89"/>
-      <c r="Q53" s="87" t="s">
+      <c r="M53" s="77"/>
+      <c r="N53" s="77"/>
+      <c r="O53" s="77"/>
+      <c r="P53" s="79"/>
+      <c r="Q53" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="R53" s="88"/>
-      <c r="S53" s="89"/>
+      <c r="R53" s="77"/>
+      <c r="S53" s="79"/>
     </row>
     <row r="54" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="75" t="s">
+      <c r="A54" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="B54" s="75" t="s">
+      <c r="B54" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="C54" s="77" t="s">
+      <c r="C54" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="D54" s="75" t="s">
+      <c r="D54" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="E54" s="75" t="s">
+      <c r="E54" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="F54" s="75" t="s">
+      <c r="F54" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="G54" s="75" t="s">
+      <c r="G54" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="H54" s="75" t="s">
+      <c r="H54" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="I54" s="75" t="s">
+      <c r="I54" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="J54" s="75" t="s">
+      <c r="J54" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="K54" s="75" t="s">
+      <c r="K54" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="L54" s="77" t="s">
+      <c r="L54" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="M54" s="75" t="s">
+      <c r="M54" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="N54" s="75" t="s">
+      <c r="N54" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="O54" s="75" t="s">
+      <c r="O54" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="P54" s="75" t="s">
+      <c r="P54" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="Q54" s="75" t="s">
+      <c r="Q54" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="R54" s="75" t="s">
+      <c r="R54" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="S54" s="75" t="s">
+      <c r="S54" s="80" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="55" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="76"/>
-      <c r="B55" s="76"/>
-      <c r="C55" s="78"/>
-      <c r="D55" s="76"/>
-      <c r="E55" s="76"/>
-      <c r="F55" s="76"/>
-      <c r="G55" s="76"/>
-      <c r="H55" s="76"/>
-      <c r="I55" s="76"/>
-      <c r="J55" s="76"/>
-      <c r="K55" s="76"/>
-      <c r="L55" s="78"/>
-      <c r="M55" s="76"/>
-      <c r="N55" s="76"/>
-      <c r="O55" s="76"/>
-      <c r="P55" s="76"/>
-      <c r="Q55" s="76"/>
-      <c r="R55" s="76"/>
-      <c r="S55" s="76"/>
+      <c r="A55" s="81"/>
+      <c r="B55" s="81"/>
+      <c r="C55" s="84"/>
+      <c r="D55" s="81"/>
+      <c r="E55" s="81"/>
+      <c r="F55" s="81"/>
+      <c r="G55" s="81"/>
+      <c r="H55" s="81"/>
+      <c r="I55" s="81"/>
+      <c r="J55" s="81"/>
+      <c r="K55" s="81"/>
+      <c r="L55" s="84"/>
+      <c r="M55" s="81"/>
+      <c r="N55" s="81"/>
+      <c r="O55" s="81"/>
+      <c r="P55" s="81"/>
+      <c r="Q55" s="81"/>
+      <c r="R55" s="81"/>
+      <c r="S55" s="81"/>
     </row>
     <row r="56" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="76"/>
-      <c r="B56" s="76"/>
-      <c r="C56" s="78"/>
-      <c r="D56" s="76"/>
-      <c r="E56" s="76"/>
-      <c r="F56" s="76"/>
-      <c r="G56" s="76"/>
-      <c r="H56" s="76"/>
-      <c r="I56" s="76"/>
-      <c r="J56" s="76"/>
-      <c r="K56" s="76"/>
-      <c r="L56" s="78"/>
-      <c r="M56" s="76"/>
-      <c r="N56" s="76"/>
-      <c r="O56" s="76"/>
-      <c r="P56" s="76"/>
-      <c r="Q56" s="76"/>
-      <c r="R56" s="76"/>
-      <c r="S56" s="76"/>
+      <c r="A56" s="81"/>
+      <c r="B56" s="81"/>
+      <c r="C56" s="84"/>
+      <c r="D56" s="81"/>
+      <c r="E56" s="81"/>
+      <c r="F56" s="81"/>
+      <c r="G56" s="81"/>
+      <c r="H56" s="81"/>
+      <c r="I56" s="81"/>
+      <c r="J56" s="81"/>
+      <c r="K56" s="81"/>
+      <c r="L56" s="84"/>
+      <c r="M56" s="81"/>
+      <c r="N56" s="81"/>
+      <c r="O56" s="81"/>
+      <c r="P56" s="81"/>
+      <c r="Q56" s="81"/>
+      <c r="R56" s="81"/>
+      <c r="S56" s="81"/>
     </row>
     <row r="57" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A57" s="76"/>
-      <c r="B57" s="76"/>
-      <c r="C57" s="78"/>
-      <c r="D57" s="76"/>
-      <c r="E57" s="76"/>
-      <c r="F57" s="76"/>
-      <c r="G57" s="76"/>
-      <c r="H57" s="76"/>
-      <c r="I57" s="76"/>
-      <c r="J57" s="76"/>
-      <c r="K57" s="76"/>
-      <c r="L57" s="78"/>
-      <c r="M57" s="76"/>
-      <c r="N57" s="76"/>
-      <c r="O57" s="76"/>
-      <c r="P57" s="76"/>
-      <c r="Q57" s="76"/>
-      <c r="R57" s="76"/>
-      <c r="S57" s="76"/>
+      <c r="A57" s="81"/>
+      <c r="B57" s="81"/>
+      <c r="C57" s="84"/>
+      <c r="D57" s="81"/>
+      <c r="E57" s="81"/>
+      <c r="F57" s="81"/>
+      <c r="G57" s="81"/>
+      <c r="H57" s="81"/>
+      <c r="I57" s="81"/>
+      <c r="J57" s="81"/>
+      <c r="K57" s="81"/>
+      <c r="L57" s="84"/>
+      <c r="M57" s="81"/>
+      <c r="N57" s="81"/>
+      <c r="O57" s="81"/>
+      <c r="P57" s="81"/>
+      <c r="Q57" s="81"/>
+      <c r="R57" s="81"/>
+      <c r="S57" s="81"/>
     </row>
     <row r="58" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A58" s="76"/>
-      <c r="B58" s="76"/>
-      <c r="C58" s="78"/>
-      <c r="D58" s="76"/>
-      <c r="E58" s="76"/>
-      <c r="F58" s="76"/>
-      <c r="G58" s="76"/>
-      <c r="H58" s="76"/>
-      <c r="I58" s="76"/>
-      <c r="J58" s="76"/>
-      <c r="K58" s="76"/>
-      <c r="L58" s="78"/>
-      <c r="M58" s="76"/>
-      <c r="N58" s="76"/>
-      <c r="O58" s="76"/>
-      <c r="P58" s="76"/>
-      <c r="Q58" s="76"/>
-      <c r="R58" s="76"/>
-      <c r="S58" s="76"/>
+      <c r="A58" s="81"/>
+      <c r="B58" s="81"/>
+      <c r="C58" s="84"/>
+      <c r="D58" s="81"/>
+      <c r="E58" s="81"/>
+      <c r="F58" s="81"/>
+      <c r="G58" s="81"/>
+      <c r="H58" s="81"/>
+      <c r="I58" s="81"/>
+      <c r="J58" s="81"/>
+      <c r="K58" s="81"/>
+      <c r="L58" s="84"/>
+      <c r="M58" s="81"/>
+      <c r="N58" s="81"/>
+      <c r="O58" s="81"/>
+      <c r="P58" s="81"/>
+      <c r="Q58" s="81"/>
+      <c r="R58" s="81"/>
+      <c r="S58" s="81"/>
     </row>
     <row r="59" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="81"/>
-      <c r="B59" s="80"/>
-      <c r="C59" s="79"/>
-      <c r="D59" s="80"/>
-      <c r="E59" s="80"/>
-      <c r="F59" s="80"/>
-      <c r="G59" s="80"/>
-      <c r="H59" s="80"/>
-      <c r="I59" s="80"/>
-      <c r="J59" s="80"/>
-      <c r="K59" s="76"/>
-      <c r="L59" s="79"/>
-      <c r="M59" s="80"/>
-      <c r="N59" s="80"/>
-      <c r="O59" s="80"/>
-      <c r="P59" s="76"/>
-      <c r="Q59" s="80"/>
-      <c r="R59" s="80"/>
-      <c r="S59" s="80"/>
+      <c r="A59" s="92"/>
+      <c r="B59" s="82"/>
+      <c r="C59" s="85"/>
+      <c r="D59" s="82"/>
+      <c r="E59" s="82"/>
+      <c r="F59" s="82"/>
+      <c r="G59" s="82"/>
+      <c r="H59" s="82"/>
+      <c r="I59" s="82"/>
+      <c r="J59" s="82"/>
+      <c r="K59" s="81"/>
+      <c r="L59" s="85"/>
+      <c r="M59" s="82"/>
+      <c r="N59" s="82"/>
+      <c r="O59" s="82"/>
+      <c r="P59" s="81"/>
+      <c r="Q59" s="82"/>
+      <c r="R59" s="82"/>
+      <c r="S59" s="82"/>
     </row>
     <row r="60" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="35" t="s">
@@ -4783,7 +4788,7 @@
       </c>
     </row>
     <row r="61" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="71" t="s">
+      <c r="A61" s="91" t="s">
         <v>79</v>
       </c>
       <c r="B61" s="34"/>
@@ -4816,7 +4821,7 @@
         <f t="shared" ref="K61:K93" si="6">J61+K60</f>
         <v>3</v>
       </c>
-      <c r="L61" s="101" t="s">
+      <c r="L61" s="68" t="s">
         <v>33</v>
       </c>
       <c r="M61" s="20">
@@ -4845,7 +4850,7 @@
       </c>
     </row>
     <row r="62" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="71"/>
+      <c r="A62" s="91"/>
       <c r="B62" s="34"/>
       <c r="C62" s="18" t="s">
         <v>38</v>
@@ -4897,7 +4902,7 @@
         <v>0.5</v>
       </c>
       <c r="R62" s="20">
-        <f t="shared" ref="R62:R112" si="8">Q62+R61</f>
+        <f t="shared" ref="R62:R113" si="8">Q62+R61</f>
         <v>4</v>
       </c>
       <c r="S62" s="20">
@@ -4905,7 +4910,7 @@
       </c>
     </row>
     <row r="63" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="71" t="s">
+      <c r="A63" s="91" t="s">
         <v>81</v>
       </c>
       <c r="B63" s="34"/>
@@ -4967,7 +4972,7 @@
       </c>
     </row>
     <row r="64" spans="1:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="71"/>
+      <c r="A64" s="91"/>
       <c r="B64" s="34"/>
       <c r="C64" s="18" t="s">
         <v>44</v>
@@ -5027,7 +5032,7 @@
       </c>
     </row>
     <row r="65" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="71"/>
+      <c r="A65" s="91"/>
       <c r="B65" s="34"/>
       <c r="C65" s="32" t="s">
         <v>114</v>
@@ -5075,17 +5080,19 @@
         <f t="shared" si="7"/>
         <v>6.1000000000000005</v>
       </c>
-      <c r="Q65" s="20"/>
+      <c r="Q65" s="20">
+        <v>2</v>
+      </c>
       <c r="R65" s="20">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="S65" s="20">
         <v>7</v>
       </c>
     </row>
     <row r="66" spans="1:19" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="71"/>
+      <c r="A66" s="91"/>
       <c r="B66" s="34"/>
       <c r="C66" s="18" t="s">
         <v>84</v>
@@ -5138,14 +5145,14 @@
       </c>
       <c r="R66" s="20">
         <f t="shared" si="8"/>
-        <v>11.5</v>
+        <v>13.5</v>
       </c>
       <c r="S66" s="20">
         <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:19" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="71"/>
+      <c r="A67" s="91"/>
       <c r="B67" s="34"/>
       <c r="C67" s="18" t="s">
         <v>85</v>
@@ -5198,14 +5205,14 @@
       </c>
       <c r="R67" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
+        <v>14.8</v>
       </c>
       <c r="S67" s="20">
         <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:19" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="71"/>
+      <c r="A68" s="91"/>
       <c r="B68" s="34"/>
       <c r="C68" s="18" t="s">
         <v>86</v>
@@ -5253,17 +5260,19 @@
         <f t="shared" si="7"/>
         <v>8.2000000000000011</v>
       </c>
-      <c r="Q68" s="20"/>
+      <c r="Q68" s="20">
+        <v>1.2</v>
+      </c>
       <c r="R68" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
+        <v>16</v>
       </c>
       <c r="S68" s="20">
         <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="71" t="s">
+      <c r="A69" s="91" t="s">
         <v>87</v>
       </c>
       <c r="B69" s="34"/>
@@ -5313,17 +5322,19 @@
         <f t="shared" si="7"/>
         <v>9.6000000000000014</v>
       </c>
-      <c r="Q69" s="20"/>
+      <c r="Q69" s="20">
+        <v>1.5</v>
+      </c>
       <c r="R69" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
+        <v>17.5</v>
       </c>
       <c r="S69" s="20">
         <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="71"/>
+      <c r="A70" s="91"/>
       <c r="B70" s="34"/>
       <c r="C70" s="18" t="s">
         <v>50</v>
@@ -5371,17 +5382,19 @@
         <f t="shared" si="7"/>
         <v>10.3</v>
       </c>
-      <c r="Q70" s="20"/>
+      <c r="Q70" s="20">
+        <v>2</v>
+      </c>
       <c r="R70" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
+        <v>19.5</v>
       </c>
       <c r="S70" s="20">
         <v>7</v>
       </c>
     </row>
     <row r="71" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="71"/>
+      <c r="A71" s="91"/>
       <c r="B71" s="34"/>
       <c r="C71" s="18" t="s">
         <v>51</v>
@@ -5429,17 +5442,19 @@
         <f t="shared" si="7"/>
         <v>11</v>
       </c>
-      <c r="Q71" s="20"/>
+      <c r="Q71" s="20">
+        <v>1.5</v>
+      </c>
       <c r="R71" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
+        <v>21</v>
       </c>
       <c r="S71" s="20">
         <v>7</v>
       </c>
     </row>
     <row r="72" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="72" t="s">
+      <c r="A72" s="99" t="s">
         <v>88</v>
       </c>
       <c r="B72" s="33"/>
@@ -5489,17 +5504,19 @@
         <f t="shared" si="7"/>
         <v>12.4</v>
       </c>
-      <c r="Q72" s="20"/>
+      <c r="Q72" s="20">
+        <v>2.5</v>
+      </c>
       <c r="R72" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
+        <v>23.5</v>
       </c>
       <c r="S72" s="20">
         <v>7</v>
       </c>
     </row>
     <row r="73" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="73"/>
+      <c r="A73" s="100"/>
       <c r="B73" s="33"/>
       <c r="C73" s="18" t="s">
         <v>55</v>
@@ -5547,17 +5564,19 @@
         <f t="shared" si="7"/>
         <v>13.8</v>
       </c>
-      <c r="Q73" s="20"/>
+      <c r="Q73" s="20">
+        <v>2.1</v>
+      </c>
       <c r="R73" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
+        <v>25.6</v>
       </c>
       <c r="S73" s="20">
         <v>7</v>
       </c>
     </row>
     <row r="74" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="73"/>
+      <c r="A74" s="100"/>
       <c r="B74" s="33"/>
       <c r="C74" s="18" t="s">
         <v>56</v>
@@ -5605,17 +5624,19 @@
         <f t="shared" si="7"/>
         <v>14.5</v>
       </c>
-      <c r="Q74" s="20"/>
+      <c r="Q74" s="20">
+        <v>1.3</v>
+      </c>
       <c r="R74" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
+        <v>26.900000000000002</v>
       </c>
       <c r="S74" s="20">
         <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="73"/>
+      <c r="A75" s="100"/>
       <c r="B75" s="33"/>
       <c r="C75" s="18" t="s">
         <v>57</v>
@@ -5663,17 +5684,19 @@
         <f t="shared" si="7"/>
         <v>15.2</v>
       </c>
-      <c r="Q75" s="20"/>
+      <c r="Q75" s="20">
+        <v>1</v>
+      </c>
       <c r="R75" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
+        <v>27.900000000000002</v>
       </c>
       <c r="S75" s="20">
         <v>7</v>
       </c>
     </row>
     <row r="76" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="73"/>
+      <c r="A76" s="100"/>
       <c r="B76" s="33"/>
       <c r="C76" s="18" t="s">
         <v>58</v>
@@ -5721,17 +5744,19 @@
         <f t="shared" si="7"/>
         <v>15.899999999999999</v>
       </c>
-      <c r="Q76" s="20"/>
+      <c r="Q76" s="20">
+        <v>1.5</v>
+      </c>
       <c r="R76" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
+        <v>29.400000000000002</v>
       </c>
       <c r="S76" s="20">
         <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="73"/>
+      <c r="A77" s="100"/>
       <c r="B77" s="33"/>
       <c r="C77" s="18" t="s">
         <v>90</v>
@@ -5775,17 +5800,19 @@
         <f t="shared" si="7"/>
         <v>19.299999999999997</v>
       </c>
-      <c r="Q77" s="20"/>
+      <c r="Q77" s="20">
+        <v>5.9</v>
+      </c>
       <c r="R77" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
+        <v>35.300000000000004</v>
       </c>
       <c r="S77" s="20">
         <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="73"/>
+      <c r="A78" s="100"/>
       <c r="B78" s="33"/>
       <c r="C78" s="18" t="s">
         <v>91</v>
@@ -5822,7 +5849,7 @@
       <c r="M78" s="20">
         <v>2</v>
       </c>
-      <c r="N78" s="99">
+      <c r="N78" s="66">
         <v>7</v>
       </c>
       <c r="O78" s="20">
@@ -5833,17 +5860,19 @@
         <f t="shared" si="7"/>
         <v>19.999999999999996</v>
       </c>
-      <c r="Q78" s="20"/>
+      <c r="Q78" s="20">
+        <v>1</v>
+      </c>
       <c r="R78" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
+        <v>36.300000000000004</v>
       </c>
       <c r="S78" s="20">
         <v>7</v>
       </c>
     </row>
     <row r="79" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="73"/>
+      <c r="A79" s="100"/>
       <c r="B79" s="33"/>
       <c r="C79" s="18" t="s">
         <v>92</v>
@@ -5891,15 +5920,19 @@
         <f t="shared" si="7"/>
         <v>26.9</v>
       </c>
-      <c r="Q79" s="20"/>
+      <c r="Q79" s="20">
+        <v>11.4</v>
+      </c>
       <c r="R79" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
-      </c>
-      <c r="S79" s="20"/>
+        <v>47.7</v>
+      </c>
+      <c r="S79" s="20">
+        <v>7</v>
+      </c>
     </row>
     <row r="80" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="73"/>
+      <c r="A80" s="100"/>
       <c r="B80" s="33"/>
       <c r="C80" s="18" t="s">
         <v>93</v>
@@ -5947,15 +5980,19 @@
         <f t="shared" si="7"/>
         <v>27.599999999999998</v>
       </c>
-      <c r="Q80" s="20"/>
+      <c r="Q80" s="20">
+        <v>1.5</v>
+      </c>
       <c r="R80" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
-      </c>
-      <c r="S80" s="20"/>
+        <v>49.2</v>
+      </c>
+      <c r="S80" s="20">
+        <v>7</v>
+      </c>
     </row>
     <row r="81" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="73"/>
+      <c r="A81" s="100"/>
       <c r="B81" s="33"/>
       <c r="C81" s="18" t="s">
         <v>95</v>
@@ -6003,15 +6040,19 @@
         <f t="shared" si="7"/>
         <v>28.299999999999997</v>
       </c>
-      <c r="Q81" s="20"/>
+      <c r="Q81" s="20">
+        <v>1.2</v>
+      </c>
       <c r="R81" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
-      </c>
-      <c r="S81" s="20"/>
+        <v>50.400000000000006</v>
+      </c>
+      <c r="S81" s="20">
+        <v>7</v>
+      </c>
     </row>
     <row r="82" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="74"/>
+      <c r="A82" s="101"/>
       <c r="B82" s="33"/>
       <c r="C82" s="18" t="s">
         <v>96</v>
@@ -6059,15 +6100,19 @@
         <f t="shared" si="7"/>
         <v>28.999999999999996</v>
       </c>
-      <c r="Q82" s="20"/>
+      <c r="Q82" s="20">
+        <v>0.5</v>
+      </c>
       <c r="R82" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
-      </c>
-      <c r="S82" s="20"/>
+        <v>50.900000000000006</v>
+      </c>
+      <c r="S82" s="20">
+        <v>7</v>
+      </c>
     </row>
     <row r="83" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="71" t="s">
+      <c r="A83" s="91" t="s">
         <v>97</v>
       </c>
       <c r="B83" s="34"/>
@@ -6117,15 +6162,19 @@
         <f>O83+P82</f>
         <v>32.4</v>
       </c>
-      <c r="Q83" s="20"/>
+      <c r="Q83" s="20">
+        <v>1.9</v>
+      </c>
       <c r="R83" s="20">
         <f>Q83+R82</f>
-        <v>12.8</v>
-      </c>
-      <c r="S83" s="20"/>
+        <v>52.800000000000004</v>
+      </c>
+      <c r="S83" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="84" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="71"/>
+      <c r="A84" s="91"/>
       <c r="B84" s="34"/>
       <c r="C84" s="18" t="s">
         <v>61</v>
@@ -6173,12 +6222,19 @@
         <f>O84+P83</f>
         <v>33.799999999999997</v>
       </c>
-      <c r="Q84" s="62"/>
-      <c r="R84" s="62"/>
-      <c r="S84" s="62"/>
+      <c r="Q84" s="62">
+        <v>1</v>
+      </c>
+      <c r="R84" s="20">
+        <f>Q84+R83</f>
+        <v>53.800000000000004</v>
+      </c>
+      <c r="S84" s="62">
+        <v>8</v>
+      </c>
     </row>
     <row r="85" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="71"/>
+      <c r="A85" s="91"/>
       <c r="B85" s="34"/>
       <c r="C85" s="14" t="s">
         <v>62</v>
@@ -6222,15 +6278,19 @@
         <f>O85+P84</f>
         <v>34.099999999999994</v>
       </c>
-      <c r="Q85" s="20"/>
+      <c r="Q85" s="20">
+        <v>0.6</v>
+      </c>
       <c r="R85" s="20">
-        <f>Q85+R83</f>
-        <v>12.8</v>
-      </c>
-      <c r="S85" s="20"/>
+        <f>Q85+R84</f>
+        <v>54.400000000000006</v>
+      </c>
+      <c r="S85" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="86" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="71"/>
+      <c r="A86" s="91"/>
       <c r="B86" s="34"/>
       <c r="C86" s="18" t="s">
         <v>98</v>
@@ -6278,15 +6338,19 @@
         <f t="shared" si="7"/>
         <v>34.399999999999991</v>
       </c>
-      <c r="Q86" s="20"/>
+      <c r="Q86" s="20">
+        <v>0.7</v>
+      </c>
       <c r="R86" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
-      </c>
-      <c r="S86" s="20"/>
+        <v>55.100000000000009</v>
+      </c>
+      <c r="S86" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="87" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="71"/>
+      <c r="A87" s="91"/>
       <c r="B87" s="34"/>
       <c r="C87" s="18" t="s">
         <v>99</v>
@@ -6334,15 +6398,19 @@
         <f t="shared" si="7"/>
         <v>35.79999999999999</v>
       </c>
-      <c r="Q87" s="20"/>
+      <c r="Q87" s="20">
+        <v>2.5</v>
+      </c>
       <c r="R87" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
-      </c>
-      <c r="S87" s="20"/>
+        <v>57.600000000000009</v>
+      </c>
+      <c r="S87" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="88" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="71"/>
+      <c r="A88" s="91"/>
       <c r="B88" s="34"/>
       <c r="C88" s="18" t="s">
         <v>65</v>
@@ -6390,15 +6458,19 @@
         <f t="shared" si="7"/>
         <v>50.29999999999999</v>
       </c>
-      <c r="Q88" s="20"/>
+      <c r="Q88" s="20">
+        <v>21.2</v>
+      </c>
       <c r="R88" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
-      </c>
-      <c r="S88" s="20"/>
+        <v>78.800000000000011</v>
+      </c>
+      <c r="S88" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="89" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="71"/>
+      <c r="A89" s="91"/>
       <c r="B89" s="34"/>
       <c r="C89" s="18" t="s">
         <v>67</v>
@@ -6442,15 +6514,19 @@
         <f t="shared" si="7"/>
         <v>52.399999999999991</v>
       </c>
-      <c r="Q89" s="20"/>
+      <c r="Q89" s="20">
+        <v>2</v>
+      </c>
       <c r="R89" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
-      </c>
-      <c r="S89" s="20"/>
+        <v>80.800000000000011</v>
+      </c>
+      <c r="S89" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="90" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="71"/>
+      <c r="A90" s="91"/>
       <c r="B90" s="34"/>
       <c r="C90" s="18" t="s">
         <v>68</v>
@@ -6498,15 +6574,19 @@
         <f t="shared" si="7"/>
         <v>54.499999999999993</v>
       </c>
-      <c r="Q90" s="20"/>
+      <c r="Q90" s="20">
+        <v>4.2</v>
+      </c>
       <c r="R90" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
-      </c>
-      <c r="S90" s="20"/>
+        <v>85.000000000000014</v>
+      </c>
+      <c r="S90" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="91" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="71" t="s">
+      <c r="A91" s="91" t="s">
         <v>100</v>
       </c>
       <c r="B91" s="34"/>
@@ -6556,15 +6636,19 @@
         <f t="shared" si="7"/>
         <v>55.899999999999991</v>
       </c>
-      <c r="Q91" s="20"/>
+      <c r="Q91" s="20">
+        <v>3</v>
+      </c>
       <c r="R91" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
-      </c>
-      <c r="S91" s="20"/>
+        <v>88.000000000000014</v>
+      </c>
+      <c r="S91" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="92" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="71" t="s">
+      <c r="A92" s="91" t="s">
         <v>100</v>
       </c>
       <c r="B92" s="34"/>
@@ -6614,15 +6698,19 @@
         <f t="shared" si="7"/>
         <v>59.29999999999999</v>
       </c>
-      <c r="Q92" s="20"/>
+      <c r="Q92" s="20">
+        <v>6.2</v>
+      </c>
       <c r="R92" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
-      </c>
-      <c r="S92" s="20"/>
+        <v>94.200000000000017</v>
+      </c>
+      <c r="S92" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="93" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="71"/>
+      <c r="A93" s="91"/>
       <c r="B93" s="34"/>
       <c r="C93" s="18" t="s">
         <v>72</v>
@@ -6670,15 +6758,19 @@
         <f t="shared" si="7"/>
         <v>60.699999999999989</v>
       </c>
-      <c r="Q93" s="20"/>
+      <c r="Q93" s="20">
+        <v>3</v>
+      </c>
       <c r="R93" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
-      </c>
-      <c r="S93" s="20"/>
+        <v>97.200000000000017</v>
+      </c>
+      <c r="S93" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="94" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="71"/>
+      <c r="A94" s="91"/>
       <c r="B94" s="34"/>
       <c r="C94" s="18" t="s">
         <v>102</v>
@@ -6726,15 +6818,19 @@
         <f t="shared" ref="P94:P114" si="11">O94+P93</f>
         <v>61.699999999999989</v>
       </c>
-      <c r="Q94" s="20"/>
+      <c r="Q94" s="20">
+        <v>1</v>
+      </c>
       <c r="R94" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
-      </c>
-      <c r="S94" s="20"/>
+        <v>98.200000000000017</v>
+      </c>
+      <c r="S94" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="95" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="71"/>
+      <c r="A95" s="91"/>
       <c r="B95" s="34"/>
       <c r="C95" s="18" t="s">
         <v>103</v>
@@ -6782,15 +6878,19 @@
         <f t="shared" si="11"/>
         <v>65.099999999999994</v>
       </c>
-      <c r="Q95" s="20"/>
+      <c r="Q95" s="20">
+        <v>4.5</v>
+      </c>
       <c r="R95" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
-      </c>
-      <c r="S95" s="20"/>
+        <v>102.70000000000002</v>
+      </c>
+      <c r="S95" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="96" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="71"/>
+      <c r="A96" s="91"/>
       <c r="B96" s="34"/>
       <c r="C96" s="18" t="s">
         <v>104</v>
@@ -6838,15 +6938,19 @@
         <f t="shared" si="11"/>
         <v>65.8</v>
       </c>
-      <c r="Q96" s="20"/>
+      <c r="Q96" s="20">
+        <v>1</v>
+      </c>
       <c r="R96" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
-      </c>
-      <c r="S96" s="20"/>
+        <v>103.70000000000002</v>
+      </c>
+      <c r="S96" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="97" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="71"/>
+      <c r="A97" s="91"/>
       <c r="B97" s="34"/>
       <c r="C97" s="18" t="s">
         <v>92</v>
@@ -6894,17 +6998,21 @@
         <f t="shared" si="11"/>
         <v>72.7</v>
       </c>
-      <c r="Q97" s="20"/>
+      <c r="Q97" s="20">
+        <v>9.6</v>
+      </c>
       <c r="R97" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
-      </c>
-      <c r="S97" s="20"/>
+        <v>113.30000000000001</v>
+      </c>
+      <c r="S97" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="98" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="71"/>
+      <c r="A98" s="91"/>
       <c r="B98" s="34"/>
-      <c r="C98" s="98" t="s">
+      <c r="C98" s="65" t="s">
         <v>93</v>
       </c>
       <c r="D98" s="21">
@@ -6950,15 +7058,19 @@
         <f t="shared" si="11"/>
         <v>73.400000000000006</v>
       </c>
-      <c r="Q98" s="20"/>
+      <c r="Q98" s="20">
+        <v>1.5</v>
+      </c>
       <c r="R98" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
-      </c>
-      <c r="S98" s="20"/>
+        <v>114.80000000000001</v>
+      </c>
+      <c r="S98" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="99" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="71"/>
+      <c r="A99" s="91"/>
       <c r="B99" s="34"/>
       <c r="C99" s="18" t="s">
         <v>95</v>
@@ -7006,15 +7118,19 @@
         <f t="shared" si="11"/>
         <v>74.100000000000009</v>
       </c>
-      <c r="Q99" s="20"/>
+      <c r="Q99" s="20">
+        <v>1.7</v>
+      </c>
       <c r="R99" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
-      </c>
-      <c r="S99" s="20"/>
+        <v>116.50000000000001</v>
+      </c>
+      <c r="S99" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="100" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="71"/>
+      <c r="A100" s="91"/>
       <c r="B100" s="34"/>
       <c r="C100" s="18" t="s">
         <v>96</v>
@@ -7062,15 +7178,19 @@
         <f t="shared" si="11"/>
         <v>74.800000000000011</v>
       </c>
-      <c r="Q100" s="20"/>
+      <c r="Q100" s="20">
+        <v>0.5</v>
+      </c>
       <c r="R100" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
-      </c>
-      <c r="S100" s="20"/>
+        <v>117.00000000000001</v>
+      </c>
+      <c r="S100" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="101" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="65" t="s">
+      <c r="A101" s="93" t="s">
         <v>105</v>
       </c>
       <c r="B101" s="33"/>
@@ -7123,12 +7243,12 @@
       <c r="Q101" s="20"/>
       <c r="R101" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
+        <v>117.00000000000001</v>
       </c>
       <c r="S101" s="20"/>
     </row>
     <row r="102" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="66"/>
+      <c r="A102" s="94"/>
       <c r="B102" s="33"/>
       <c r="C102" s="18" t="s">
         <v>107</v>
@@ -7179,12 +7299,12 @@
       <c r="Q102" s="20"/>
       <c r="R102" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
+        <v>117.00000000000001</v>
       </c>
       <c r="S102" s="20"/>
     </row>
     <row r="103" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="67"/>
+      <c r="A103" s="95"/>
       <c r="B103" s="33"/>
       <c r="C103" s="18" t="s">
         <v>108</v>
@@ -7235,12 +7355,12 @@
       <c r="Q103" s="20"/>
       <c r="R103" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
+        <v>117.00000000000001</v>
       </c>
       <c r="S103" s="20"/>
     </row>
     <row r="104" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="67"/>
+      <c r="A104" s="95"/>
       <c r="B104" s="33"/>
       <c r="C104" s="18" t="s">
         <v>109</v>
@@ -7291,12 +7411,12 @@
       <c r="Q104" s="20"/>
       <c r="R104" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
+        <v>117.00000000000001</v>
       </c>
       <c r="S104" s="20"/>
     </row>
     <row r="105" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="67"/>
+      <c r="A105" s="95"/>
       <c r="B105" s="40"/>
       <c r="C105" s="37" t="s">
         <v>110</v>
@@ -7347,12 +7467,12 @@
       <c r="Q105" s="20"/>
       <c r="R105" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
+        <v>117.00000000000001</v>
       </c>
       <c r="S105" s="20"/>
     </row>
     <row r="106" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="68"/>
+      <c r="A106" s="96"/>
       <c r="B106" s="41"/>
       <c r="C106" s="38" t="s">
         <v>111</v>
@@ -7403,12 +7523,12 @@
       <c r="Q106" s="20"/>
       <c r="R106" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
+        <v>117.00000000000001</v>
       </c>
       <c r="S106" s="20"/>
     </row>
     <row r="107" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="68"/>
+      <c r="A107" s="96"/>
       <c r="B107" s="41"/>
       <c r="C107" s="38" t="s">
         <v>112</v>
@@ -7439,7 +7559,7 @@
         <f t="shared" si="10"/>
         <v>119</v>
       </c>
-      <c r="L107" s="100" t="s">
+      <c r="L107" s="67" t="s">
         <v>94</v>
       </c>
       <c r="M107" s="49">
@@ -7459,12 +7579,12 @@
       <c r="Q107" s="20"/>
       <c r="R107" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
+        <v>117.00000000000001</v>
       </c>
       <c r="S107" s="20"/>
     </row>
     <row r="108" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="67"/>
+      <c r="A108" s="95"/>
       <c r="B108" s="42"/>
       <c r="C108" s="37" t="s">
         <v>75</v>
@@ -7515,12 +7635,12 @@
       <c r="Q108" s="20"/>
       <c r="R108" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
+        <v>117.00000000000001</v>
       </c>
       <c r="S108" s="20"/>
     </row>
     <row r="109" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="67"/>
+      <c r="A109" s="95"/>
       <c r="B109" s="43"/>
       <c r="C109" s="54" t="s">
         <v>113</v>
@@ -7571,12 +7691,12 @@
       <c r="Q109" s="20"/>
       <c r="R109" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
+        <v>117.00000000000001</v>
       </c>
       <c r="S109" s="20"/>
     </row>
     <row r="110" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="69"/>
+      <c r="A110" s="97"/>
       <c r="B110" s="43"/>
       <c r="C110" s="54" t="s">
         <v>92</v>
@@ -7627,12 +7747,12 @@
       <c r="Q110" s="20"/>
       <c r="R110" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
+        <v>117.00000000000001</v>
       </c>
       <c r="S110" s="20"/>
     </row>
     <row r="111" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="69"/>
+      <c r="A111" s="97"/>
       <c r="B111" s="43"/>
       <c r="C111" s="54" t="s">
         <v>93</v>
@@ -7683,12 +7803,12 @@
       <c r="Q111" s="20"/>
       <c r="R111" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
+        <v>117.00000000000001</v>
       </c>
       <c r="S111" s="20"/>
     </row>
     <row r="112" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="69"/>
+      <c r="A112" s="97"/>
       <c r="B112" s="43"/>
       <c r="C112" s="54" t="s">
         <v>95</v>
@@ -7739,12 +7859,12 @@
       <c r="Q112" s="20"/>
       <c r="R112" s="20">
         <f t="shared" si="8"/>
-        <v>12.8</v>
+        <v>117.00000000000001</v>
       </c>
       <c r="S112" s="20"/>
     </row>
     <row r="113" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="69"/>
+      <c r="A113" s="97"/>
       <c r="B113" s="43"/>
       <c r="C113" s="54" t="s">
         <v>96</v>
@@ -7793,11 +7913,14 @@
         <v>96.500000000000057</v>
       </c>
       <c r="Q113" s="62"/>
-      <c r="R113" s="62"/>
+      <c r="R113" s="20">
+        <f t="shared" si="8"/>
+        <v>117.00000000000001</v>
+      </c>
       <c r="S113" s="62"/>
     </row>
     <row r="114" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="70"/>
+      <c r="A114" s="98"/>
       <c r="B114" s="43"/>
       <c r="C114" s="63" t="s">
         <v>115</v>
@@ -7844,7 +7967,7 @@
       <c r="Q114" s="20"/>
       <c r="R114" s="20">
         <f>Q114+R112</f>
-        <v>12.8</v>
+        <v>117.00000000000001</v>
       </c>
       <c r="S114" s="20"/>
     </row>
@@ -7886,22 +8009,58 @@
         <v>99.900000000000063</v>
       </c>
       <c r="P115" s="3"/>
-      <c r="Q115" s="20"/>
+      <c r="Q115" s="20">
+        <f>SUM(Q60:Q114)</f>
+        <v>117.00000000000001</v>
+      </c>
       <c r="R115" s="8"/>
       <c r="S115" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="E7:K7"/>
-    <mergeCell ref="L7:P7"/>
+    <mergeCell ref="A101:A114"/>
+    <mergeCell ref="A63:A68"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="A72:A82"/>
+    <mergeCell ref="A83:A91"/>
+    <mergeCell ref="A92:A100"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="K54:K59"/>
+    <mergeCell ref="L54:L59"/>
+    <mergeCell ref="M54:M59"/>
+    <mergeCell ref="N54:N59"/>
+    <mergeCell ref="F54:F59"/>
+    <mergeCell ref="G54:G59"/>
+    <mergeCell ref="H54:H59"/>
+    <mergeCell ref="I54:I59"/>
+    <mergeCell ref="J54:J59"/>
+    <mergeCell ref="A54:A59"/>
+    <mergeCell ref="B54:B59"/>
+    <mergeCell ref="C54:C59"/>
+    <mergeCell ref="D54:D59"/>
+    <mergeCell ref="E54:E59"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A51:S51"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="E53:K53"/>
+    <mergeCell ref="L53:P53"/>
+    <mergeCell ref="Q53:S53"/>
+    <mergeCell ref="P54:P59"/>
+    <mergeCell ref="Q54:Q59"/>
+    <mergeCell ref="R54:R59"/>
+    <mergeCell ref="S54:S59"/>
+    <mergeCell ref="O54:O59"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="P8:P13"/>
+    <mergeCell ref="Q8:Q13"/>
+    <mergeCell ref="R8:R13"/>
+    <mergeCell ref="S8:S13"/>
+    <mergeCell ref="A14:A16"/>
     <mergeCell ref="Q7:S7"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="B8:B13"/>
@@ -7918,49 +8077,16 @@
     <mergeCell ref="M8:M13"/>
     <mergeCell ref="N8:N13"/>
     <mergeCell ref="O8:O13"/>
-    <mergeCell ref="P8:P13"/>
-    <mergeCell ref="Q8:Q13"/>
-    <mergeCell ref="R8:R13"/>
-    <mergeCell ref="S8:S13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="A36:A43"/>
-    <mergeCell ref="P54:P59"/>
-    <mergeCell ref="Q54:Q59"/>
-    <mergeCell ref="R54:R59"/>
-    <mergeCell ref="S54:S59"/>
-    <mergeCell ref="O54:O59"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A51:S51"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="E53:K53"/>
-    <mergeCell ref="L53:P53"/>
-    <mergeCell ref="Q53:S53"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="K54:K59"/>
-    <mergeCell ref="L54:L59"/>
-    <mergeCell ref="M54:M59"/>
-    <mergeCell ref="N54:N59"/>
-    <mergeCell ref="F54:F59"/>
-    <mergeCell ref="G54:G59"/>
-    <mergeCell ref="H54:H59"/>
-    <mergeCell ref="I54:I59"/>
-    <mergeCell ref="J54:J59"/>
-    <mergeCell ref="A54:A59"/>
-    <mergeCell ref="B54:B59"/>
-    <mergeCell ref="C54:C59"/>
-    <mergeCell ref="D54:D59"/>
-    <mergeCell ref="E54:E59"/>
-    <mergeCell ref="A101:A114"/>
-    <mergeCell ref="A63:A68"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="A72:A82"/>
-    <mergeCell ref="A83:A91"/>
-    <mergeCell ref="A92:A100"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="E7:K7"/>
+    <mergeCell ref="L7:P7"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="F4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Correccion error TASK Equipo
</commit_message>
<xml_diff>
--- a/NoteBook/summary/TASK_TEAM.xlsx
+++ b/NoteBook/summary/TASK_TEAM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\GitHub\tsp\NoteBook\summary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FabiánEduardo\Documents\GitHub\tsp\NoteBook\summary\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1638,6 +1638,87 @@
     <xf numFmtId="0" fontId="81" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1653,89 +1734,8 @@
     <xf numFmtId="0" fontId="61" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="73" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="71" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2019,8 +2019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D97" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U113" sqref="U113"/>
+    <sheetView tabSelected="1" topLeftCell="D98" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K84" sqref="K84:K85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2042,16 +2042,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
+      <c r="A1" s="96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="29"/>
@@ -2061,51 +2061,51 @@
       <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="70"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="97"/>
       <c r="E3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="72">
+      <c r="F3" s="99">
         <v>41719</v>
       </c>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
     </row>
     <row r="4" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="75"/>
-      <c r="D4" s="74"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="95"/>
       <c r="E4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="74" t="s">
+      <c r="F4" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
+      <c r="G4" s="95"/>
+      <c r="H4" s="95"/>
     </row>
     <row r="5" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="76"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="76"/>
+      <c r="B5" s="94"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="94"/>
       <c r="E5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="74">
-        <v>1</v>
-      </c>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
+      <c r="F5" s="95">
+        <v>1</v>
+      </c>
+      <c r="G5" s="95"/>
+      <c r="H5" s="95"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
@@ -2129,197 +2129,197 @@
       <c r="S6" s="24"/>
     </row>
     <row r="7" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="77"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="78" t="s">
+      <c r="B7" s="92"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="93"/>
+      <c r="E7" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="77"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="77"/>
-      <c r="I7" s="77"/>
-      <c r="J7" s="77"/>
-      <c r="K7" s="79"/>
-      <c r="L7" s="78" t="s">
+      <c r="F7" s="92"/>
+      <c r="G7" s="92"/>
+      <c r="H7" s="92"/>
+      <c r="I7" s="92"/>
+      <c r="J7" s="92"/>
+      <c r="K7" s="93"/>
+      <c r="L7" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="77"/>
-      <c r="N7" s="77"/>
-      <c r="O7" s="77"/>
-      <c r="P7" s="79"/>
-      <c r="Q7" s="78" t="s">
+      <c r="M7" s="92"/>
+      <c r="N7" s="92"/>
+      <c r="O7" s="92"/>
+      <c r="P7" s="93"/>
+      <c r="Q7" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="R7" s="77"/>
-      <c r="S7" s="79"/>
+      <c r="R7" s="92"/>
+      <c r="S7" s="93"/>
     </row>
     <row r="8" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="80" t="s">
+      <c r="A8" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="83" t="s">
+      <c r="C8" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="80" t="s">
+      <c r="D8" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="80" t="s">
+      <c r="E8" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="80" t="s">
+      <c r="F8" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="80" t="s">
+      <c r="G8" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="80" t="s">
+      <c r="H8" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="80" t="s">
+      <c r="I8" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="80" t="s">
+      <c r="J8" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="80" t="s">
+      <c r="K8" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="83" t="s">
+      <c r="L8" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="M8" s="80" t="s">
+      <c r="M8" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="N8" s="80" t="s">
+      <c r="N8" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="O8" s="80" t="s">
+      <c r="O8" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="P8" s="80" t="s">
+      <c r="P8" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="Q8" s="80" t="s">
+      <c r="Q8" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="R8" s="80" t="s">
+      <c r="R8" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="S8" s="80" t="s">
+      <c r="S8" s="79" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="81"/>
-      <c r="B9" s="81"/>
-      <c r="C9" s="84"/>
-      <c r="D9" s="81"/>
-      <c r="E9" s="81"/>
-      <c r="F9" s="81"/>
-      <c r="G9" s="81"/>
-      <c r="H9" s="81"/>
-      <c r="I9" s="81"/>
-      <c r="J9" s="81"/>
-      <c r="K9" s="81"/>
-      <c r="L9" s="84"/>
-      <c r="M9" s="81"/>
-      <c r="N9" s="81"/>
-      <c r="O9" s="81"/>
-      <c r="P9" s="81"/>
-      <c r="Q9" s="81"/>
-      <c r="R9" s="81"/>
-      <c r="S9" s="81"/>
+      <c r="A9" s="80"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="80"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="80"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="80"/>
+      <c r="L9" s="82"/>
+      <c r="M9" s="80"/>
+      <c r="N9" s="80"/>
+      <c r="O9" s="80"/>
+      <c r="P9" s="80"/>
+      <c r="Q9" s="80"/>
+      <c r="R9" s="80"/>
+      <c r="S9" s="80"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="81"/>
-      <c r="B10" s="81"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="81"/>
-      <c r="F10" s="81"/>
-      <c r="G10" s="81"/>
-      <c r="H10" s="81"/>
-      <c r="I10" s="81"/>
-      <c r="J10" s="81"/>
-      <c r="K10" s="81"/>
-      <c r="L10" s="84"/>
-      <c r="M10" s="81"/>
-      <c r="N10" s="81"/>
-      <c r="O10" s="81"/>
-      <c r="P10" s="81"/>
-      <c r="Q10" s="81"/>
-      <c r="R10" s="81"/>
-      <c r="S10" s="81"/>
+      <c r="A10" s="80"/>
+      <c r="B10" s="80"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="80"/>
+      <c r="G10" s="80"/>
+      <c r="H10" s="80"/>
+      <c r="I10" s="80"/>
+      <c r="J10" s="80"/>
+      <c r="K10" s="80"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="80"/>
+      <c r="N10" s="80"/>
+      <c r="O10" s="80"/>
+      <c r="P10" s="80"/>
+      <c r="Q10" s="80"/>
+      <c r="R10" s="80"/>
+      <c r="S10" s="80"/>
     </row>
     <row r="11" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="81"/>
-      <c r="B11" s="81"/>
-      <c r="C11" s="84"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="81"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="81"/>
-      <c r="I11" s="81"/>
-      <c r="J11" s="81"/>
-      <c r="K11" s="81"/>
-      <c r="L11" s="84"/>
-      <c r="M11" s="81"/>
-      <c r="N11" s="81"/>
-      <c r="O11" s="81"/>
-      <c r="P11" s="81"/>
-      <c r="Q11" s="81"/>
-      <c r="R11" s="81"/>
-      <c r="S11" s="81"/>
+      <c r="A11" s="80"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="80"/>
+      <c r="G11" s="80"/>
+      <c r="H11" s="80"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="80"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="82"/>
+      <c r="M11" s="80"/>
+      <c r="N11" s="80"/>
+      <c r="O11" s="80"/>
+      <c r="P11" s="80"/>
+      <c r="Q11" s="80"/>
+      <c r="R11" s="80"/>
+      <c r="S11" s="80"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="81"/>
-      <c r="B12" s="81"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="81"/>
-      <c r="E12" s="81"/>
-      <c r="F12" s="81"/>
-      <c r="G12" s="81"/>
-      <c r="H12" s="81"/>
-      <c r="I12" s="81"/>
-      <c r="J12" s="81"/>
-      <c r="K12" s="81"/>
-      <c r="L12" s="84"/>
-      <c r="M12" s="81"/>
-      <c r="N12" s="81"/>
-      <c r="O12" s="81"/>
-      <c r="P12" s="81"/>
-      <c r="Q12" s="81"/>
-      <c r="R12" s="81"/>
-      <c r="S12" s="81"/>
+      <c r="A12" s="80"/>
+      <c r="B12" s="80"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="80"/>
+      <c r="F12" s="80"/>
+      <c r="G12" s="80"/>
+      <c r="H12" s="80"/>
+      <c r="I12" s="80"/>
+      <c r="J12" s="80"/>
+      <c r="K12" s="80"/>
+      <c r="L12" s="82"/>
+      <c r="M12" s="80"/>
+      <c r="N12" s="80"/>
+      <c r="O12" s="80"/>
+      <c r="P12" s="80"/>
+      <c r="Q12" s="80"/>
+      <c r="R12" s="80"/>
+      <c r="S12" s="80"/>
     </row>
     <row r="13" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="82"/>
-      <c r="B13" s="82"/>
-      <c r="C13" s="85"/>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
-      <c r="F13" s="82"/>
-      <c r="G13" s="82"/>
-      <c r="H13" s="82"/>
-      <c r="I13" s="82"/>
-      <c r="J13" s="82"/>
-      <c r="K13" s="81"/>
-      <c r="L13" s="85"/>
-      <c r="M13" s="82"/>
-      <c r="N13" s="82"/>
-      <c r="O13" s="82"/>
-      <c r="P13" s="81"/>
-      <c r="Q13" s="82"/>
-      <c r="R13" s="82"/>
-      <c r="S13" s="82"/>
+      <c r="A13" s="84"/>
+      <c r="B13" s="84"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="84"/>
+      <c r="E13" s="84"/>
+      <c r="F13" s="84"/>
+      <c r="G13" s="84"/>
+      <c r="H13" s="84"/>
+      <c r="I13" s="84"/>
+      <c r="J13" s="84"/>
+      <c r="K13" s="80"/>
+      <c r="L13" s="83"/>
+      <c r="M13" s="84"/>
+      <c r="N13" s="84"/>
+      <c r="O13" s="84"/>
+      <c r="P13" s="80"/>
+      <c r="Q13" s="84"/>
+      <c r="R13" s="84"/>
+      <c r="S13" s="84"/>
     </row>
     <row r="14" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="86" t="s">
@@ -4534,197 +4534,197 @@
       <c r="S52" s="24"/>
     </row>
     <row r="53" spans="1:19" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="78" t="s">
+      <c r="A53" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="B53" s="77"/>
-      <c r="C53" s="77"/>
-      <c r="D53" s="79"/>
-      <c r="E53" s="78" t="s">
+      <c r="B53" s="92"/>
+      <c r="C53" s="92"/>
+      <c r="D53" s="93"/>
+      <c r="E53" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="F53" s="77"/>
-      <c r="G53" s="77"/>
-      <c r="H53" s="77"/>
-      <c r="I53" s="77"/>
-      <c r="J53" s="77"/>
-      <c r="K53" s="79"/>
-      <c r="L53" s="78" t="s">
+      <c r="F53" s="92"/>
+      <c r="G53" s="92"/>
+      <c r="H53" s="92"/>
+      <c r="I53" s="92"/>
+      <c r="J53" s="92"/>
+      <c r="K53" s="93"/>
+      <c r="L53" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="M53" s="77"/>
-      <c r="N53" s="77"/>
-      <c r="O53" s="77"/>
-      <c r="P53" s="79"/>
-      <c r="Q53" s="78" t="s">
+      <c r="M53" s="92"/>
+      <c r="N53" s="92"/>
+      <c r="O53" s="92"/>
+      <c r="P53" s="93"/>
+      <c r="Q53" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="R53" s="77"/>
-      <c r="S53" s="79"/>
+      <c r="R53" s="92"/>
+      <c r="S53" s="93"/>
     </row>
     <row r="54" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="80" t="s">
+      <c r="A54" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="B54" s="80" t="s">
+      <c r="B54" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="C54" s="83" t="s">
+      <c r="C54" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="D54" s="80" t="s">
+      <c r="D54" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="E54" s="80" t="s">
+      <c r="E54" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="F54" s="80" t="s">
+      <c r="F54" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="G54" s="80" t="s">
+      <c r="G54" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="H54" s="80" t="s">
+      <c r="H54" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="I54" s="80" t="s">
+      <c r="I54" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="J54" s="80" t="s">
+      <c r="J54" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="K54" s="80" t="s">
+      <c r="K54" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="L54" s="83" t="s">
+      <c r="L54" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="M54" s="80" t="s">
+      <c r="M54" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="N54" s="80" t="s">
+      <c r="N54" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="O54" s="80" t="s">
+      <c r="O54" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="P54" s="80" t="s">
+      <c r="P54" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="Q54" s="80" t="s">
+      <c r="Q54" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="R54" s="80" t="s">
+      <c r="R54" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="S54" s="80" t="s">
+      <c r="S54" s="79" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="55" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="81"/>
-      <c r="B55" s="81"/>
-      <c r="C55" s="84"/>
-      <c r="D55" s="81"/>
-      <c r="E55" s="81"/>
-      <c r="F55" s="81"/>
-      <c r="G55" s="81"/>
-      <c r="H55" s="81"/>
-      <c r="I55" s="81"/>
-      <c r="J55" s="81"/>
-      <c r="K55" s="81"/>
-      <c r="L55" s="84"/>
-      <c r="M55" s="81"/>
-      <c r="N55" s="81"/>
-      <c r="O55" s="81"/>
-      <c r="P55" s="81"/>
-      <c r="Q55" s="81"/>
-      <c r="R55" s="81"/>
-      <c r="S55" s="81"/>
+      <c r="A55" s="80"/>
+      <c r="B55" s="80"/>
+      <c r="C55" s="82"/>
+      <c r="D55" s="80"/>
+      <c r="E55" s="80"/>
+      <c r="F55" s="80"/>
+      <c r="G55" s="80"/>
+      <c r="H55" s="80"/>
+      <c r="I55" s="80"/>
+      <c r="J55" s="80"/>
+      <c r="K55" s="80"/>
+      <c r="L55" s="82"/>
+      <c r="M55" s="80"/>
+      <c r="N55" s="80"/>
+      <c r="O55" s="80"/>
+      <c r="P55" s="80"/>
+      <c r="Q55" s="80"/>
+      <c r="R55" s="80"/>
+      <c r="S55" s="80"/>
     </row>
     <row r="56" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="81"/>
-      <c r="B56" s="81"/>
-      <c r="C56" s="84"/>
-      <c r="D56" s="81"/>
-      <c r="E56" s="81"/>
-      <c r="F56" s="81"/>
-      <c r="G56" s="81"/>
-      <c r="H56" s="81"/>
-      <c r="I56" s="81"/>
-      <c r="J56" s="81"/>
-      <c r="K56" s="81"/>
-      <c r="L56" s="84"/>
-      <c r="M56" s="81"/>
-      <c r="N56" s="81"/>
-      <c r="O56" s="81"/>
-      <c r="P56" s="81"/>
-      <c r="Q56" s="81"/>
-      <c r="R56" s="81"/>
-      <c r="S56" s="81"/>
+      <c r="A56" s="80"/>
+      <c r="B56" s="80"/>
+      <c r="C56" s="82"/>
+      <c r="D56" s="80"/>
+      <c r="E56" s="80"/>
+      <c r="F56" s="80"/>
+      <c r="G56" s="80"/>
+      <c r="H56" s="80"/>
+      <c r="I56" s="80"/>
+      <c r="J56" s="80"/>
+      <c r="K56" s="80"/>
+      <c r="L56" s="82"/>
+      <c r="M56" s="80"/>
+      <c r="N56" s="80"/>
+      <c r="O56" s="80"/>
+      <c r="P56" s="80"/>
+      <c r="Q56" s="80"/>
+      <c r="R56" s="80"/>
+      <c r="S56" s="80"/>
     </row>
     <row r="57" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A57" s="81"/>
-      <c r="B57" s="81"/>
-      <c r="C57" s="84"/>
-      <c r="D57" s="81"/>
-      <c r="E57" s="81"/>
-      <c r="F57" s="81"/>
-      <c r="G57" s="81"/>
-      <c r="H57" s="81"/>
-      <c r="I57" s="81"/>
-      <c r="J57" s="81"/>
-      <c r="K57" s="81"/>
-      <c r="L57" s="84"/>
-      <c r="M57" s="81"/>
-      <c r="N57" s="81"/>
-      <c r="O57" s="81"/>
-      <c r="P57" s="81"/>
-      <c r="Q57" s="81"/>
-      <c r="R57" s="81"/>
-      <c r="S57" s="81"/>
+      <c r="A57" s="80"/>
+      <c r="B57" s="80"/>
+      <c r="C57" s="82"/>
+      <c r="D57" s="80"/>
+      <c r="E57" s="80"/>
+      <c r="F57" s="80"/>
+      <c r="G57" s="80"/>
+      <c r="H57" s="80"/>
+      <c r="I57" s="80"/>
+      <c r="J57" s="80"/>
+      <c r="K57" s="80"/>
+      <c r="L57" s="82"/>
+      <c r="M57" s="80"/>
+      <c r="N57" s="80"/>
+      <c r="O57" s="80"/>
+      <c r="P57" s="80"/>
+      <c r="Q57" s="80"/>
+      <c r="R57" s="80"/>
+      <c r="S57" s="80"/>
     </row>
     <row r="58" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A58" s="81"/>
-      <c r="B58" s="81"/>
-      <c r="C58" s="84"/>
-      <c r="D58" s="81"/>
-      <c r="E58" s="81"/>
-      <c r="F58" s="81"/>
-      <c r="G58" s="81"/>
-      <c r="H58" s="81"/>
-      <c r="I58" s="81"/>
-      <c r="J58" s="81"/>
-      <c r="K58" s="81"/>
-      <c r="L58" s="84"/>
-      <c r="M58" s="81"/>
-      <c r="N58" s="81"/>
-      <c r="O58" s="81"/>
-      <c r="P58" s="81"/>
-      <c r="Q58" s="81"/>
-      <c r="R58" s="81"/>
-      <c r="S58" s="81"/>
+      <c r="A58" s="80"/>
+      <c r="B58" s="80"/>
+      <c r="C58" s="82"/>
+      <c r="D58" s="80"/>
+      <c r="E58" s="80"/>
+      <c r="F58" s="80"/>
+      <c r="G58" s="80"/>
+      <c r="H58" s="80"/>
+      <c r="I58" s="80"/>
+      <c r="J58" s="80"/>
+      <c r="K58" s="80"/>
+      <c r="L58" s="82"/>
+      <c r="M58" s="80"/>
+      <c r="N58" s="80"/>
+      <c r="O58" s="80"/>
+      <c r="P58" s="80"/>
+      <c r="Q58" s="80"/>
+      <c r="R58" s="80"/>
+      <c r="S58" s="80"/>
     </row>
     <row r="59" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="92"/>
-      <c r="B59" s="82"/>
-      <c r="C59" s="85"/>
-      <c r="D59" s="82"/>
-      <c r="E59" s="82"/>
-      <c r="F59" s="82"/>
-      <c r="G59" s="82"/>
-      <c r="H59" s="82"/>
-      <c r="I59" s="82"/>
-      <c r="J59" s="82"/>
-      <c r="K59" s="81"/>
-      <c r="L59" s="85"/>
-      <c r="M59" s="82"/>
-      <c r="N59" s="82"/>
-      <c r="O59" s="82"/>
-      <c r="P59" s="81"/>
-      <c r="Q59" s="82"/>
-      <c r="R59" s="82"/>
-      <c r="S59" s="82"/>
+      <c r="A59" s="85"/>
+      <c r="B59" s="84"/>
+      <c r="C59" s="83"/>
+      <c r="D59" s="84"/>
+      <c r="E59" s="84"/>
+      <c r="F59" s="84"/>
+      <c r="G59" s="84"/>
+      <c r="H59" s="84"/>
+      <c r="I59" s="84"/>
+      <c r="J59" s="84"/>
+      <c r="K59" s="80"/>
+      <c r="L59" s="83"/>
+      <c r="M59" s="84"/>
+      <c r="N59" s="84"/>
+      <c r="O59" s="84"/>
+      <c r="P59" s="80"/>
+      <c r="Q59" s="84"/>
+      <c r="R59" s="84"/>
+      <c r="S59" s="84"/>
     </row>
     <row r="60" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="35" t="s">
@@ -4788,7 +4788,7 @@
       </c>
     </row>
     <row r="61" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="91" t="s">
+      <c r="A61" s="75" t="s">
         <v>79</v>
       </c>
       <c r="B61" s="34"/>
@@ -4850,7 +4850,7 @@
       </c>
     </row>
     <row r="62" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="91"/>
+      <c r="A62" s="75"/>
       <c r="B62" s="34"/>
       <c r="C62" s="18" t="s">
         <v>38</v>
@@ -4910,7 +4910,7 @@
       </c>
     </row>
     <row r="63" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="91" t="s">
+      <c r="A63" s="75" t="s">
         <v>81</v>
       </c>
       <c r="B63" s="34"/>
@@ -4972,7 +4972,7 @@
       </c>
     </row>
     <row r="64" spans="1:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="91"/>
+      <c r="A64" s="75"/>
       <c r="B64" s="34"/>
       <c r="C64" s="18" t="s">
         <v>44</v>
@@ -5032,7 +5032,7 @@
       </c>
     </row>
     <row r="65" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="91"/>
+      <c r="A65" s="75"/>
       <c r="B65" s="34"/>
       <c r="C65" s="32" t="s">
         <v>114</v>
@@ -5092,7 +5092,7 @@
       </c>
     </row>
     <row r="66" spans="1:19" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="91"/>
+      <c r="A66" s="75"/>
       <c r="B66" s="34"/>
       <c r="C66" s="18" t="s">
         <v>84</v>
@@ -5152,7 +5152,7 @@
       </c>
     </row>
     <row r="67" spans="1:19" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="91"/>
+      <c r="A67" s="75"/>
       <c r="B67" s="34"/>
       <c r="C67" s="18" t="s">
         <v>85</v>
@@ -5212,7 +5212,7 @@
       </c>
     </row>
     <row r="68" spans="1:19" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="91"/>
+      <c r="A68" s="75"/>
       <c r="B68" s="34"/>
       <c r="C68" s="18" t="s">
         <v>86</v>
@@ -5272,7 +5272,7 @@
       </c>
     </row>
     <row r="69" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="91" t="s">
+      <c r="A69" s="75" t="s">
         <v>87</v>
       </c>
       <c r="B69" s="34"/>
@@ -5334,7 +5334,7 @@
       </c>
     </row>
     <row r="70" spans="1:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="91"/>
+      <c r="A70" s="75"/>
       <c r="B70" s="34"/>
       <c r="C70" s="18" t="s">
         <v>50</v>
@@ -5394,7 +5394,7 @@
       </c>
     </row>
     <row r="71" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="91"/>
+      <c r="A71" s="75"/>
       <c r="B71" s="34"/>
       <c r="C71" s="18" t="s">
         <v>51</v>
@@ -5454,7 +5454,7 @@
       </c>
     </row>
     <row r="72" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="99" t="s">
+      <c r="A72" s="76" t="s">
         <v>88</v>
       </c>
       <c r="B72" s="33"/>
@@ -5516,7 +5516,7 @@
       </c>
     </row>
     <row r="73" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="100"/>
+      <c r="A73" s="77"/>
       <c r="B73" s="33"/>
       <c r="C73" s="18" t="s">
         <v>55</v>
@@ -5576,7 +5576,7 @@
       </c>
     </row>
     <row r="74" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="100"/>
+      <c r="A74" s="77"/>
       <c r="B74" s="33"/>
       <c r="C74" s="18" t="s">
         <v>56</v>
@@ -5636,7 +5636,7 @@
       </c>
     </row>
     <row r="75" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="100"/>
+      <c r="A75" s="77"/>
       <c r="B75" s="33"/>
       <c r="C75" s="18" t="s">
         <v>57</v>
@@ -5696,7 +5696,7 @@
       </c>
     </row>
     <row r="76" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="100"/>
+      <c r="A76" s="77"/>
       <c r="B76" s="33"/>
       <c r="C76" s="18" t="s">
         <v>58</v>
@@ -5756,7 +5756,7 @@
       </c>
     </row>
     <row r="77" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="100"/>
+      <c r="A77" s="77"/>
       <c r="B77" s="33"/>
       <c r="C77" s="18" t="s">
         <v>90</v>
@@ -5812,7 +5812,7 @@
       </c>
     </row>
     <row r="78" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="100"/>
+      <c r="A78" s="77"/>
       <c r="B78" s="33"/>
       <c r="C78" s="18" t="s">
         <v>91</v>
@@ -5872,7 +5872,7 @@
       </c>
     </row>
     <row r="79" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="100"/>
+      <c r="A79" s="77"/>
       <c r="B79" s="33"/>
       <c r="C79" s="18" t="s">
         <v>92</v>
@@ -5932,7 +5932,7 @@
       </c>
     </row>
     <row r="80" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="100"/>
+      <c r="A80" s="77"/>
       <c r="B80" s="33"/>
       <c r="C80" s="18" t="s">
         <v>93</v>
@@ -5992,7 +5992,7 @@
       </c>
     </row>
     <row r="81" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="100"/>
+      <c r="A81" s="77"/>
       <c r="B81" s="33"/>
       <c r="C81" s="18" t="s">
         <v>95</v>
@@ -6052,7 +6052,7 @@
       </c>
     </row>
     <row r="82" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="101"/>
+      <c r="A82" s="78"/>
       <c r="B82" s="33"/>
       <c r="C82" s="18" t="s">
         <v>96</v>
@@ -6112,7 +6112,7 @@
       </c>
     </row>
     <row r="83" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="91" t="s">
+      <c r="A83" s="75" t="s">
         <v>97</v>
       </c>
       <c r="B83" s="34"/>
@@ -6174,7 +6174,7 @@
       </c>
     </row>
     <row r="84" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="91"/>
+      <c r="A84" s="75"/>
       <c r="B84" s="34"/>
       <c r="C84" s="18" t="s">
         <v>61</v>
@@ -6234,7 +6234,7 @@
       </c>
     </row>
     <row r="85" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="91"/>
+      <c r="A85" s="75"/>
       <c r="B85" s="34"/>
       <c r="C85" s="14" t="s">
         <v>62</v>
@@ -6262,8 +6262,8 @@
         <v>0.5</v>
       </c>
       <c r="K85" s="20">
-        <f>J85+K83</f>
-        <v>47.5</v>
+        <f>J85+K84</f>
+        <v>49.5</v>
       </c>
       <c r="L85" s="20"/>
       <c r="M85" s="20"/>
@@ -6290,7 +6290,7 @@
       </c>
     </row>
     <row r="86" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="91"/>
+      <c r="A86" s="75"/>
       <c r="B86" s="34"/>
       <c r="C86" s="18" t="s">
         <v>98</v>
@@ -6319,7 +6319,7 @@
       </c>
       <c r="K86" s="20">
         <f t="shared" si="6"/>
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L86" s="20" t="s">
         <v>94</v>
@@ -6350,7 +6350,7 @@
       </c>
     </row>
     <row r="87" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="91"/>
+      <c r="A87" s="75"/>
       <c r="B87" s="34"/>
       <c r="C87" s="18" t="s">
         <v>99</v>
@@ -6379,7 +6379,7 @@
       </c>
       <c r="K87" s="20">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L87" s="20" t="s">
         <v>33</v>
@@ -6410,7 +6410,7 @@
       </c>
     </row>
     <row r="88" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="91"/>
+      <c r="A88" s="75"/>
       <c r="B88" s="34"/>
       <c r="C88" s="18" t="s">
         <v>65</v>
@@ -6439,7 +6439,7 @@
       </c>
       <c r="K88" s="20">
         <f t="shared" si="6"/>
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L88" s="20" t="s">
         <v>66</v>
@@ -6470,7 +6470,7 @@
       </c>
     </row>
     <row r="89" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="91"/>
+      <c r="A89" s="75"/>
       <c r="B89" s="34"/>
       <c r="C89" s="18" t="s">
         <v>67</v>
@@ -6499,7 +6499,7 @@
       </c>
       <c r="K89" s="20">
         <f t="shared" si="6"/>
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L89" s="20"/>
       <c r="M89" s="20"/>
@@ -6526,7 +6526,7 @@
       </c>
     </row>
     <row r="90" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="91"/>
+      <c r="A90" s="75"/>
       <c r="B90" s="34"/>
       <c r="C90" s="18" t="s">
         <v>68</v>
@@ -6555,7 +6555,7 @@
       </c>
       <c r="K90" s="20">
         <f t="shared" si="6"/>
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L90" s="20" t="s">
         <v>33</v>
@@ -6586,7 +6586,7 @@
       </c>
     </row>
     <row r="91" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="91" t="s">
+      <c r="A91" s="75" t="s">
         <v>100</v>
       </c>
       <c r="B91" s="34"/>
@@ -6617,7 +6617,7 @@
       </c>
       <c r="K91" s="20">
         <f t="shared" si="6"/>
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="L91" s="20" t="s">
         <v>66</v>
@@ -6648,7 +6648,7 @@
       </c>
     </row>
     <row r="92" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="91" t="s">
+      <c r="A92" s="75" t="s">
         <v>100</v>
       </c>
       <c r="B92" s="34"/>
@@ -6679,7 +6679,7 @@
       </c>
       <c r="K92" s="20">
         <f t="shared" si="6"/>
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="L92" s="20" t="s">
         <v>94</v>
@@ -6710,7 +6710,7 @@
       </c>
     </row>
     <row r="93" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="91"/>
+      <c r="A93" s="75"/>
       <c r="B93" s="34"/>
       <c r="C93" s="18" t="s">
         <v>72</v>
@@ -6739,7 +6739,7 @@
       </c>
       <c r="K93" s="20">
         <f t="shared" si="6"/>
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L93" s="20" t="s">
         <v>33</v>
@@ -6770,7 +6770,7 @@
       </c>
     </row>
     <row r="94" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="91"/>
+      <c r="A94" s="75"/>
       <c r="B94" s="34"/>
       <c r="C94" s="18" t="s">
         <v>102</v>
@@ -6799,7 +6799,7 @@
       </c>
       <c r="K94" s="20">
         <f t="shared" ref="K94:K114" si="10">J94+K93</f>
-        <v>87.5</v>
+        <v>89.5</v>
       </c>
       <c r="L94" s="20" t="s">
         <v>94</v>
@@ -6830,7 +6830,7 @@
       </c>
     </row>
     <row r="95" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="91"/>
+      <c r="A95" s="75"/>
       <c r="B95" s="34"/>
       <c r="C95" s="18" t="s">
         <v>103</v>
@@ -6859,7 +6859,7 @@
       </c>
       <c r="K95" s="20">
         <f t="shared" si="10"/>
-        <v>92.5</v>
+        <v>94.5</v>
       </c>
       <c r="L95" s="20" t="s">
         <v>94</v>
@@ -6890,7 +6890,7 @@
       </c>
     </row>
     <row r="96" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="91"/>
+      <c r="A96" s="75"/>
       <c r="B96" s="34"/>
       <c r="C96" s="18" t="s">
         <v>104</v>
@@ -6919,7 +6919,7 @@
       </c>
       <c r="K96" s="20">
         <f t="shared" si="10"/>
-        <v>93.5</v>
+        <v>95.5</v>
       </c>
       <c r="L96" s="20" t="s">
         <v>94</v>
@@ -6950,7 +6950,7 @@
       </c>
     </row>
     <row r="97" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="91"/>
+      <c r="A97" s="75"/>
       <c r="B97" s="34"/>
       <c r="C97" s="18" t="s">
         <v>92</v>
@@ -6979,7 +6979,7 @@
       </c>
       <c r="K97" s="20">
         <f t="shared" si="10"/>
-        <v>103.5</v>
+        <v>105.5</v>
       </c>
       <c r="L97" s="20" t="s">
         <v>94</v>
@@ -7010,7 +7010,7 @@
       </c>
     </row>
     <row r="98" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="91"/>
+      <c r="A98" s="75"/>
       <c r="B98" s="34"/>
       <c r="C98" s="65" t="s">
         <v>93</v>
@@ -7039,7 +7039,7 @@
       </c>
       <c r="K98" s="20">
         <f t="shared" si="10"/>
-        <v>104.5</v>
+        <v>106.5</v>
       </c>
       <c r="L98" s="20" t="s">
         <v>94</v>
@@ -7070,7 +7070,7 @@
       </c>
     </row>
     <row r="99" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="91"/>
+      <c r="A99" s="75"/>
       <c r="B99" s="34"/>
       <c r="C99" s="18" t="s">
         <v>95</v>
@@ -7099,7 +7099,7 @@
       </c>
       <c r="K99" s="20">
         <f t="shared" si="10"/>
-        <v>105.5</v>
+        <v>107.5</v>
       </c>
       <c r="L99" s="20" t="s">
         <v>94</v>
@@ -7130,7 +7130,7 @@
       </c>
     </row>
     <row r="100" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="91"/>
+      <c r="A100" s="75"/>
       <c r="B100" s="34"/>
       <c r="C100" s="18" t="s">
         <v>96</v>
@@ -7159,7 +7159,7 @@
       </c>
       <c r="K100" s="20">
         <f t="shared" si="10"/>
-        <v>106.5</v>
+        <v>108.5</v>
       </c>
       <c r="L100" s="20" t="s">
         <v>94</v>
@@ -7190,7 +7190,7 @@
       </c>
     </row>
     <row r="101" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="93" t="s">
+      <c r="A101" s="69" t="s">
         <v>105</v>
       </c>
       <c r="B101" s="33"/>
@@ -7221,7 +7221,7 @@
       </c>
       <c r="K101" s="20">
         <f t="shared" si="10"/>
-        <v>108.5</v>
+        <v>110.5</v>
       </c>
       <c r="L101" s="20" t="s">
         <v>33</v>
@@ -7252,7 +7252,7 @@
       </c>
     </row>
     <row r="102" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="94"/>
+      <c r="A102" s="70"/>
       <c r="B102" s="33"/>
       <c r="C102" s="18" t="s">
         <v>107</v>
@@ -7281,7 +7281,7 @@
       </c>
       <c r="K102" s="20">
         <f t="shared" si="10"/>
-        <v>109.5</v>
+        <v>111.5</v>
       </c>
       <c r="L102" s="20" t="s">
         <v>94</v>
@@ -7312,7 +7312,7 @@
       </c>
     </row>
     <row r="103" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="95"/>
+      <c r="A103" s="71"/>
       <c r="B103" s="33"/>
       <c r="C103" s="18" t="s">
         <v>108</v>
@@ -7341,7 +7341,7 @@
       </c>
       <c r="K103" s="20">
         <f t="shared" si="10"/>
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="L103" s="20" t="s">
         <v>94</v>
@@ -7372,7 +7372,7 @@
       </c>
     </row>
     <row r="104" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="95"/>
+      <c r="A104" s="71"/>
       <c r="B104" s="33"/>
       <c r="C104" s="18" t="s">
         <v>109</v>
@@ -7401,7 +7401,7 @@
       </c>
       <c r="K104" s="20">
         <f t="shared" si="10"/>
-        <v>113.5</v>
+        <v>115.5</v>
       </c>
       <c r="L104" s="20" t="s">
         <v>94</v>
@@ -7432,7 +7432,7 @@
       </c>
     </row>
     <row r="105" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="95"/>
+      <c r="A105" s="71"/>
       <c r="B105" s="40"/>
       <c r="C105" s="37" t="s">
         <v>110</v>
@@ -7461,7 +7461,7 @@
       </c>
       <c r="K105" s="20">
         <f t="shared" si="10"/>
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="L105" s="20" t="s">
         <v>94</v>
@@ -7492,7 +7492,7 @@
       </c>
     </row>
     <row r="106" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="96"/>
+      <c r="A106" s="72"/>
       <c r="B106" s="41"/>
       <c r="C106" s="38" t="s">
         <v>111</v>
@@ -7521,7 +7521,7 @@
       </c>
       <c r="K106" s="20">
         <f t="shared" si="10"/>
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="L106" s="48" t="s">
         <v>94</v>
@@ -7552,7 +7552,7 @@
       </c>
     </row>
     <row r="107" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="96"/>
+      <c r="A107" s="72"/>
       <c r="B107" s="41"/>
       <c r="C107" s="38" t="s">
         <v>112</v>
@@ -7581,7 +7581,7 @@
       </c>
       <c r="K107" s="20">
         <f t="shared" si="10"/>
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="L107" s="67" t="s">
         <v>94</v>
@@ -7612,7 +7612,7 @@
       </c>
     </row>
     <row r="108" spans="1:19" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="95"/>
+      <c r="A108" s="71"/>
       <c r="B108" s="42"/>
       <c r="C108" s="37" t="s">
         <v>75</v>
@@ -7641,7 +7641,7 @@
       </c>
       <c r="K108" s="20">
         <f t="shared" si="10"/>
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="L108" s="35" t="s">
         <v>33</v>
@@ -7672,7 +7672,7 @@
       </c>
     </row>
     <row r="109" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="95"/>
+      <c r="A109" s="71"/>
       <c r="B109" s="43"/>
       <c r="C109" s="54" t="s">
         <v>113</v>
@@ -7701,7 +7701,7 @@
       </c>
       <c r="K109" s="20">
         <f t="shared" si="10"/>
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="L109" s="50" t="s">
         <v>94</v>
@@ -7732,7 +7732,7 @@
       </c>
     </row>
     <row r="110" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="97"/>
+      <c r="A110" s="73"/>
       <c r="B110" s="43"/>
       <c r="C110" s="54" t="s">
         <v>92</v>
@@ -7761,7 +7761,7 @@
       </c>
       <c r="K110" s="20">
         <f t="shared" si="10"/>
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L110" s="52" t="s">
         <v>94</v>
@@ -7792,7 +7792,7 @@
       </c>
     </row>
     <row r="111" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="97"/>
+      <c r="A111" s="73"/>
       <c r="B111" s="43"/>
       <c r="C111" s="54" t="s">
         <v>93</v>
@@ -7821,7 +7821,7 @@
       </c>
       <c r="K111" s="20">
         <f t="shared" si="10"/>
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="L111" s="52" t="s">
         <v>94</v>
@@ -7852,7 +7852,7 @@
       </c>
     </row>
     <row r="112" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="97"/>
+      <c r="A112" s="73"/>
       <c r="B112" s="43"/>
       <c r="C112" s="54" t="s">
         <v>95</v>
@@ -7881,7 +7881,7 @@
       </c>
       <c r="K112" s="20">
         <f t="shared" si="10"/>
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="L112" s="52" t="s">
         <v>94</v>
@@ -7912,7 +7912,7 @@
       </c>
     </row>
     <row r="113" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="97"/>
+      <c r="A113" s="73"/>
       <c r="B113" s="43"/>
       <c r="C113" s="54" t="s">
         <v>96</v>
@@ -7941,7 +7941,7 @@
       </c>
       <c r="K113" s="20">
         <f t="shared" si="10"/>
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="L113" s="36" t="s">
         <v>94</v>
@@ -7972,7 +7972,7 @@
       </c>
     </row>
     <row r="114" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="98"/>
+      <c r="A114" s="74"/>
       <c r="B114" s="43"/>
       <c r="C114" s="63" t="s">
         <v>115</v>
@@ -8001,7 +8001,7 @@
       </c>
       <c r="K114" s="20">
         <f t="shared" si="10"/>
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="L114" s="52"/>
       <c r="M114" s="53"/>
@@ -8074,49 +8074,16 @@
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="A101:A114"/>
-    <mergeCell ref="A63:A68"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="A72:A82"/>
-    <mergeCell ref="A83:A91"/>
-    <mergeCell ref="A92:A100"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="K54:K59"/>
-    <mergeCell ref="L54:L59"/>
-    <mergeCell ref="M54:M59"/>
-    <mergeCell ref="N54:N59"/>
-    <mergeCell ref="F54:F59"/>
-    <mergeCell ref="G54:G59"/>
-    <mergeCell ref="H54:H59"/>
-    <mergeCell ref="I54:I59"/>
-    <mergeCell ref="J54:J59"/>
-    <mergeCell ref="A54:A59"/>
-    <mergeCell ref="B54:B59"/>
-    <mergeCell ref="C54:C59"/>
-    <mergeCell ref="D54:D59"/>
-    <mergeCell ref="E54:E59"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A51:S51"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="E53:K53"/>
-    <mergeCell ref="L53:P53"/>
-    <mergeCell ref="Q53:S53"/>
-    <mergeCell ref="P54:P59"/>
-    <mergeCell ref="Q54:Q59"/>
-    <mergeCell ref="R54:R59"/>
-    <mergeCell ref="S54:S59"/>
-    <mergeCell ref="O54:O59"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="A36:A43"/>
-    <mergeCell ref="P8:P13"/>
-    <mergeCell ref="Q8:Q13"/>
-    <mergeCell ref="R8:R13"/>
-    <mergeCell ref="S8:S13"/>
-    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="E7:K7"/>
+    <mergeCell ref="L7:P7"/>
     <mergeCell ref="Q7:S7"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="B8:B13"/>
@@ -8133,16 +8100,49 @@
     <mergeCell ref="M8:M13"/>
     <mergeCell ref="N8:N13"/>
     <mergeCell ref="O8:O13"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="E7:K7"/>
-    <mergeCell ref="L7:P7"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="P8:P13"/>
+    <mergeCell ref="Q8:Q13"/>
+    <mergeCell ref="R8:R13"/>
+    <mergeCell ref="S8:S13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="P54:P59"/>
+    <mergeCell ref="Q54:Q59"/>
+    <mergeCell ref="R54:R59"/>
+    <mergeCell ref="S54:S59"/>
+    <mergeCell ref="O54:O59"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A51:S51"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="E53:K53"/>
+    <mergeCell ref="L53:P53"/>
+    <mergeCell ref="Q53:S53"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="K54:K59"/>
+    <mergeCell ref="L54:L59"/>
+    <mergeCell ref="M54:M59"/>
+    <mergeCell ref="N54:N59"/>
+    <mergeCell ref="F54:F59"/>
+    <mergeCell ref="G54:G59"/>
+    <mergeCell ref="H54:H59"/>
+    <mergeCell ref="I54:I59"/>
+    <mergeCell ref="J54:J59"/>
+    <mergeCell ref="A54:A59"/>
+    <mergeCell ref="B54:B59"/>
+    <mergeCell ref="C54:C59"/>
+    <mergeCell ref="D54:D59"/>
+    <mergeCell ref="E54:E59"/>
+    <mergeCell ref="A101:A114"/>
+    <mergeCell ref="A63:A68"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="A72:A82"/>
+    <mergeCell ref="A83:A91"/>
+    <mergeCell ref="A92:A100"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>